<commit_message>
GolfReader now saves the Courses read in. now handles a golf course that is 9 holes.
</commit_message>
<xml_diff>
--- a/spec/fixtures/Golf.xlsx
+++ b/spec/fixtures/Golf.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulkristoff/dev/golf/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D892D5B9-6B8C-3D4A-B1C6-D700E5993851}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B37E9CB-F085-C448-94B0-71DA35A3A1AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1540" windowWidth="30200" windowHeight="17440" activeTab="1" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
+    <workbookView xWindow="2780" yWindow="1540" windowWidth="30200" windowHeight="17440" activeTab="2" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
   </bookViews>
   <sheets>
-    <sheet name="Knight's play" sheetId="1" r:id="rId1"/>
-    <sheet name="Lochmere" sheetId="2" r:id="rId2"/>
+    <sheet name="Knight's play 1-9" sheetId="1" r:id="rId1"/>
+    <sheet name="Knight's play 10-18" sheetId="3" r:id="rId2"/>
+    <sheet name="Knight's play 19-27" sheetId="4" r:id="rId3"/>
+    <sheet name="Lochmere" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="19">
   <si>
     <t>Hole</t>
   </si>
@@ -79,9 +81,6 @@
   </si>
   <si>
     <t>Slope</t>
-  </si>
-  <si>
-    <t>Avg</t>
   </si>
   <si>
     <t>Address</t>
@@ -476,17 +475,700 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{045CE2A8-F6DB-4143-9691-363739FD69FB}">
-  <dimension ref="A1:V32"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="K30" sqref="A30:K33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1">
+        <v>7</v>
+      </c>
+      <c r="I2" s="1">
+        <v>8</v>
+      </c>
+      <c r="J2" s="1">
+        <v>9</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>126</v>
+      </c>
+      <c r="C4" s="1">
+        <v>100</v>
+      </c>
+      <c r="D4" s="1">
+        <v>139</v>
+      </c>
+      <c r="E4" s="1">
+        <v>194</v>
+      </c>
+      <c r="F4" s="1">
+        <v>106</v>
+      </c>
+      <c r="G4" s="1">
+        <v>166</v>
+      </c>
+      <c r="H4" s="1">
+        <v>123</v>
+      </c>
+      <c r="I4" s="1">
+        <v>171</v>
+      </c>
+      <c r="J4" s="4">
+        <v>151</v>
+      </c>
+      <c r="K4" s="5">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>93</v>
+      </c>
+      <c r="C5" s="1">
+        <v>80</v>
+      </c>
+      <c r="D5" s="1">
+        <v>114</v>
+      </c>
+      <c r="E5" s="1">
+        <v>174</v>
+      </c>
+      <c r="F5" s="1">
+        <v>91</v>
+      </c>
+      <c r="G5" s="1">
+        <v>121</v>
+      </c>
+      <c r="H5" s="1">
+        <v>101</v>
+      </c>
+      <c r="I5" s="1">
+        <v>140</v>
+      </c>
+      <c r="J5" s="1">
+        <v>133</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1">
+        <v>60</v>
+      </c>
+      <c r="C6" s="1">
+        <v>46</v>
+      </c>
+      <c r="D6" s="1">
+        <v>85</v>
+      </c>
+      <c r="E6" s="1">
+        <v>115</v>
+      </c>
+      <c r="F6" s="1">
+        <v>56</v>
+      </c>
+      <c r="G6" s="1">
+        <v>98</v>
+      </c>
+      <c r="H6" s="1">
+        <v>52</v>
+      </c>
+      <c r="I6" s="1">
+        <v>93</v>
+      </c>
+      <c r="J6" s="1">
+        <v>92</v>
+      </c>
+      <c r="K6" s="1">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1">
+        <v>3</v>
+      </c>
+      <c r="F7" s="1">
+        <v>3</v>
+      </c>
+      <c r="G7" s="1">
+        <v>3</v>
+      </c>
+      <c r="H7" s="1">
+        <v>3</v>
+      </c>
+      <c r="I7" s="1">
+        <v>3</v>
+      </c>
+      <c r="J7" s="1">
+        <v>3</v>
+      </c>
+      <c r="K7" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>44067</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+      <c r="I10">
+        <v>6</v>
+      </c>
+      <c r="J10">
+        <v>5</v>
+      </c>
+      <c r="K10" s="1">
+        <f>SUM(B10:J10)</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <v>2</v>
+      </c>
+      <c r="K11" s="1">
+        <f>SUM(B11:J11)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>44074</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <v>4</v>
+      </c>
+      <c r="I14">
+        <v>3</v>
+      </c>
+      <c r="J14">
+        <v>7</v>
+      </c>
+      <c r="K14" s="1">
+        <f>SUM(B14:J14)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>3</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="J15">
+        <v>2</v>
+      </c>
+      <c r="K15" s="1">
+        <f>SUM(B15:J15)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="6">
+        <v>44081</v>
+      </c>
+      <c r="B18" s="7">
+        <v>5</v>
+      </c>
+      <c r="C18" s="7">
+        <v>3</v>
+      </c>
+      <c r="D18" s="7">
+        <v>4</v>
+      </c>
+      <c r="E18" s="7">
+        <v>5</v>
+      </c>
+      <c r="F18" s="7">
+        <v>4</v>
+      </c>
+      <c r="G18" s="7">
+        <v>4</v>
+      </c>
+      <c r="H18" s="7">
+        <v>4</v>
+      </c>
+      <c r="I18" s="7">
+        <v>4</v>
+      </c>
+      <c r="J18" s="7">
+        <v>4</v>
+      </c>
+      <c r="K18" s="8">
+        <f>SUM(B18:J18)</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="7">
+        <v>2</v>
+      </c>
+      <c r="C19" s="7">
+        <v>2</v>
+      </c>
+      <c r="D19" s="7">
+        <v>2</v>
+      </c>
+      <c r="E19" s="7">
+        <v>3</v>
+      </c>
+      <c r="F19" s="7">
+        <v>2</v>
+      </c>
+      <c r="G19" s="7">
+        <v>2</v>
+      </c>
+      <c r="H19" s="7">
+        <v>3</v>
+      </c>
+      <c r="I19" s="7">
+        <v>1</v>
+      </c>
+      <c r="J19" s="7">
+        <v>1</v>
+      </c>
+      <c r="K19" s="8">
+        <f>SUM(B19:J19)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="6">
+        <v>44090</v>
+      </c>
+      <c r="B22" s="7">
+        <v>4</v>
+      </c>
+      <c r="C22" s="7">
+        <v>4</v>
+      </c>
+      <c r="D22" s="7">
+        <v>3</v>
+      </c>
+      <c r="E22" s="7">
+        <v>4</v>
+      </c>
+      <c r="F22" s="7">
+        <v>3</v>
+      </c>
+      <c r="G22" s="7">
+        <v>4</v>
+      </c>
+      <c r="H22" s="7">
+        <v>4</v>
+      </c>
+      <c r="I22" s="7">
+        <v>4</v>
+      </c>
+      <c r="J22" s="7">
+        <v>4</v>
+      </c>
+      <c r="K22" s="8">
+        <f>SUM(B22:J22)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="7">
+        <v>3</v>
+      </c>
+      <c r="C23" s="7">
+        <v>2</v>
+      </c>
+      <c r="D23" s="7">
+        <v>1</v>
+      </c>
+      <c r="E23" s="7">
+        <v>2</v>
+      </c>
+      <c r="F23" s="7">
+        <v>2</v>
+      </c>
+      <c r="G23" s="7">
+        <v>3</v>
+      </c>
+      <c r="H23" s="7">
+        <v>3</v>
+      </c>
+      <c r="I23" s="7">
+        <v>2</v>
+      </c>
+      <c r="J23" s="7">
+        <v>3</v>
+      </c>
+      <c r="K23" s="8">
+        <f>SUM(B23:J23)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K24" s="7"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="8"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="6">
+        <v>44102</v>
+      </c>
+      <c r="B26" s="7">
+        <v>4</v>
+      </c>
+      <c r="C26" s="7">
+        <v>3</v>
+      </c>
+      <c r="D26" s="7">
+        <v>4</v>
+      </c>
+      <c r="E26" s="7">
+        <v>5</v>
+      </c>
+      <c r="F26" s="7">
+        <v>3</v>
+      </c>
+      <c r="G26" s="7">
+        <v>3</v>
+      </c>
+      <c r="H26" s="7">
+        <v>3</v>
+      </c>
+      <c r="I26" s="7">
+        <v>5</v>
+      </c>
+      <c r="J26" s="7">
+        <v>4</v>
+      </c>
+      <c r="K26" s="8">
+        <f>SUM(B26:J26)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="7">
+        <v>2</v>
+      </c>
+      <c r="C27" s="7">
+        <v>1</v>
+      </c>
+      <c r="D27" s="7">
+        <v>2</v>
+      </c>
+      <c r="E27" s="7">
+        <v>2</v>
+      </c>
+      <c r="F27" s="7">
+        <v>2</v>
+      </c>
+      <c r="G27" s="7">
+        <v>1</v>
+      </c>
+      <c r="H27" s="7">
+        <v>2</v>
+      </c>
+      <c r="I27" s="7">
+        <v>2</v>
+      </c>
+      <c r="J27" s="7">
+        <v>2</v>
+      </c>
+      <c r="K27" s="8">
+        <f>SUM(B27:J27)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="K10 K14 K18:K19" formulaRange="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8526A8B9-0C97-E94E-BA2A-E4D31B8BA027}">
+  <dimension ref="A1:V30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
@@ -523,39 +1205,17 @@
       <c r="K2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="1">
-        <v>10</v>
-      </c>
-      <c r="M2" s="1">
-        <v>11</v>
-      </c>
-      <c r="N2" s="1">
-        <v>12</v>
-      </c>
-      <c r="O2" s="1">
-        <v>13</v>
-      </c>
-      <c r="P2" s="1">
-        <v>14</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>15</v>
-      </c>
-      <c r="R2" s="1">
-        <v>16</v>
-      </c>
-      <c r="S2" s="1">
-        <v>17</v>
-      </c>
-      <c r="T2" s="1">
-        <v>18</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
@@ -586,204 +1246,108 @@
         <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="C4" s="1">
-        <v>100</v>
+        <v>160</v>
       </c>
       <c r="D4" s="1">
-        <v>139</v>
+        <v>213</v>
       </c>
       <c r="E4" s="1">
+        <v>102</v>
+      </c>
+      <c r="F4" s="1">
+        <v>112</v>
+      </c>
+      <c r="G4" s="1">
+        <v>105</v>
+      </c>
+      <c r="H4" s="1">
         <v>194</v>
       </c>
-      <c r="F4" s="1">
-        <v>106</v>
-      </c>
-      <c r="G4" s="1">
-        <v>166</v>
-      </c>
-      <c r="H4" s="1">
-        <v>123</v>
-      </c>
       <c r="I4" s="1">
-        <v>171</v>
-      </c>
-      <c r="J4" s="4">
-        <v>151</v>
-      </c>
-      <c r="K4" s="5">
-        <v>1276</v>
-      </c>
-      <c r="L4" s="1">
-        <v>134</v>
-      </c>
-      <c r="M4" s="1">
-        <v>160</v>
-      </c>
-      <c r="N4" s="1">
-        <v>213</v>
-      </c>
-      <c r="O4" s="1">
-        <v>102</v>
-      </c>
-      <c r="P4" s="1">
-        <v>112</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>105</v>
-      </c>
-      <c r="R4" s="1">
-        <v>194</v>
-      </c>
-      <c r="S4" s="1">
         <v>140</v>
       </c>
-      <c r="T4" s="1">
+      <c r="J4" s="1">
         <v>165</v>
       </c>
-      <c r="U4" s="1">
+      <c r="K4" s="1">
         <v>1325</v>
       </c>
-      <c r="V4" s="1">
-        <v>2601</v>
-      </c>
+      <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="C5" s="1">
-        <v>80</v>
+        <v>138</v>
       </c>
       <c r="D5" s="1">
-        <v>114</v>
+        <v>169</v>
       </c>
       <c r="E5" s="1">
-        <v>174</v>
+        <v>84</v>
       </c>
       <c r="F5" s="1">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G5" s="1">
-        <v>121</v>
+        <v>87</v>
       </c>
       <c r="H5" s="1">
-        <v>101</v>
+        <v>164</v>
       </c>
       <c r="I5" s="1">
-        <v>140</v>
+        <v>107</v>
       </c>
       <c r="J5" s="1">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="K5" s="1">
-        <v>1047</v>
-      </c>
-      <c r="L5" s="1">
-        <v>104</v>
-      </c>
-      <c r="M5" s="1">
-        <v>138</v>
-      </c>
-      <c r="N5" s="1">
-        <v>169</v>
-      </c>
-      <c r="O5" s="1">
-        <v>84</v>
-      </c>
-      <c r="P5" s="1">
-        <v>88</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>87</v>
-      </c>
-      <c r="R5" s="1">
-        <v>164</v>
-      </c>
-      <c r="S5" s="1">
-        <v>107</v>
-      </c>
-      <c r="T5" s="1">
-        <v>136</v>
-      </c>
-      <c r="U5" s="1">
         <v>1077</v>
       </c>
-      <c r="V5" s="1">
-        <v>2124</v>
-      </c>
+      <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="1">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="C6" s="1">
-        <v>46</v>
+        <v>85</v>
       </c>
       <c r="D6" s="1">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="E6" s="1">
-        <v>115</v>
+        <v>64</v>
       </c>
       <c r="F6" s="1">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="G6" s="1">
-        <v>98</v>
+        <v>71</v>
       </c>
       <c r="H6" s="1">
-        <v>52</v>
+        <v>99</v>
       </c>
       <c r="I6" s="1">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="J6" s="1">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K6" s="1">
-        <v>697</v>
-      </c>
-      <c r="L6" s="1">
-        <v>77</v>
-      </c>
-      <c r="M6" s="1">
-        <v>85</v>
-      </c>
-      <c r="N6" s="1">
-        <v>110</v>
-      </c>
-      <c r="O6" s="1">
-        <v>64</v>
-      </c>
-      <c r="P6" s="1">
-        <v>72</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>71</v>
-      </c>
-      <c r="R6" s="1">
-        <v>99</v>
-      </c>
-      <c r="S6" s="1">
-        <v>78</v>
-      </c>
-      <c r="T6" s="1">
-        <v>90</v>
-      </c>
-      <c r="U6" s="1">
         <v>746</v>
       </c>
-      <c r="V6" s="1">
-        <v>1443</v>
-      </c>
+      <c r="L6" s="1"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -819,39 +1383,7 @@
       <c r="K7" s="1">
         <v>27</v>
       </c>
-      <c r="L7" s="1">
-        <v>3</v>
-      </c>
-      <c r="M7" s="1">
-        <v>3</v>
-      </c>
-      <c r="N7" s="1">
-        <v>3</v>
-      </c>
-      <c r="O7" s="1">
-        <v>3</v>
-      </c>
-      <c r="P7" s="1">
-        <v>3</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>3</v>
-      </c>
-      <c r="R7" s="1">
-        <v>3</v>
-      </c>
-      <c r="S7" s="1">
-        <v>3</v>
-      </c>
-      <c r="T7" s="1">
-        <v>3</v>
-      </c>
-      <c r="U7" s="1">
-        <v>27</v>
-      </c>
-      <c r="V7" s="1">
-        <v>54</v>
-      </c>
+      <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -869,22 +1401,22 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H10">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I10">
         <v>6</v>
@@ -894,43 +1426,9 @@
       </c>
       <c r="K10" s="1">
         <f>SUM(B10:J10)</f>
-        <v>39</v>
-      </c>
-      <c r="L10">
-        <v>4</v>
-      </c>
-      <c r="M10">
-        <v>6</v>
-      </c>
-      <c r="N10">
-        <v>5</v>
-      </c>
-      <c r="O10">
-        <v>4</v>
-      </c>
-      <c r="P10">
-        <v>4</v>
-      </c>
-      <c r="Q10">
-        <v>4</v>
-      </c>
-      <c r="R10">
-        <v>6</v>
-      </c>
-      <c r="S10">
-        <v>6</v>
-      </c>
-      <c r="T10">
-        <v>5</v>
-      </c>
-      <c r="U10" s="1">
-        <f>SUM(L10:T10)</f>
         <v>44</v>
       </c>
-      <c r="V10" s="1">
-        <f>K10+U10</f>
-        <v>83</v>
-      </c>
+      <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
@@ -940,14 +1438,14 @@
         <v>2</v>
       </c>
       <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
         <v>1</v>
       </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
       <c r="F11">
         <v>2</v>
       </c>
@@ -955,174 +1453,92 @@
         <v>2</v>
       </c>
       <c r="H11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J11">
         <v>2</v>
       </c>
       <c r="K11" s="1">
         <f>SUM(B11:J11)</f>
-        <v>17</v>
-      </c>
-      <c r="L11">
-        <v>2</v>
-      </c>
-      <c r="M11">
-        <v>2</v>
-      </c>
-      <c r="N11">
-        <v>3</v>
-      </c>
-      <c r="O11">
-        <v>1</v>
-      </c>
-      <c r="P11">
-        <v>2</v>
-      </c>
-      <c r="Q11">
-        <v>2</v>
-      </c>
-      <c r="R11">
-        <v>3</v>
-      </c>
-      <c r="S11">
-        <v>3</v>
-      </c>
-      <c r="T11">
-        <v>2</v>
-      </c>
-      <c r="U11" s="1">
-        <f>SUM(L11:T11)</f>
         <v>20</v>
       </c>
-      <c r="V11" s="1">
-        <f>K11+U11</f>
-        <v>37</v>
-      </c>
+      <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" t="s">
-        <v>11</v>
+      <c r="C12" t="s">
+        <v>12</v>
       </c>
       <c r="K12" s="1"/>
-      <c r="M12" t="s">
-        <v>12</v>
-      </c>
-      <c r="U12" s="1"/>
-      <c r="V12" s="1"/>
+      <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="K13" s="1"/>
-      <c r="U13" s="1"/>
-      <c r="V13" s="1"/>
+      <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>44074</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D14">
         <v>4</v>
       </c>
       <c r="E14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F14">
         <v>3</v>
       </c>
       <c r="G14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J14">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="K14" s="1">
         <f>SUM(B14:J14)</f>
-        <v>34</v>
-      </c>
-      <c r="L14">
-        <v>6</v>
-      </c>
-      <c r="M14">
-        <v>4</v>
-      </c>
-      <c r="N14">
-        <v>4</v>
-      </c>
-      <c r="O14">
-        <v>4</v>
-      </c>
-      <c r="P14">
-        <v>3</v>
-      </c>
-      <c r="Q14">
-        <v>4</v>
-      </c>
-      <c r="R14">
-        <v>5</v>
-      </c>
-      <c r="S14">
-        <v>4</v>
-      </c>
-      <c r="T14">
-        <v>5</v>
-      </c>
-      <c r="U14" s="1">
-        <f>SUM(L14:T14)</f>
         <v>39</v>
       </c>
-      <c r="V14" s="1">
-        <f>K14+U14</f>
-        <v>73</v>
-      </c>
+      <c r="L14" s="1"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C15">
         <v>2</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15">
         <v>2</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H15">
         <v>3</v>
@@ -1135,67 +1551,25 @@
       </c>
       <c r="K15" s="1">
         <f>SUM(B15:J15)</f>
-        <v>18</v>
-      </c>
-      <c r="L15">
-        <v>3</v>
-      </c>
-      <c r="M15">
-        <v>2</v>
-      </c>
-      <c r="N15">
-        <v>3</v>
-      </c>
-      <c r="O15">
-        <v>2</v>
-      </c>
-      <c r="P15">
-        <v>2</v>
-      </c>
-      <c r="Q15">
-        <v>2</v>
-      </c>
-      <c r="R15">
-        <v>3</v>
-      </c>
-      <c r="S15">
-        <v>2</v>
-      </c>
-      <c r="T15">
-        <v>2</v>
-      </c>
-      <c r="U15" s="1">
-        <f>SUM(L15:T15)</f>
         <v>21</v>
       </c>
-      <c r="V15" s="1">
-        <f>K15+U15</f>
-        <v>39</v>
-      </c>
+      <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" t="s">
-        <v>10</v>
+      <c r="C16" t="s">
+        <v>12</v>
       </c>
       <c r="K16" s="1"/>
-      <c r="M16" t="s">
-        <v>12</v>
-      </c>
-      <c r="U16" s="1"/>
-      <c r="V16" s="1"/>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="K17" s="1"/>
-      <c r="U17" s="1"/>
-      <c r="V17" s="1"/>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>44081</v>
       </c>
@@ -1209,13 +1583,13 @@
         <v>4</v>
       </c>
       <c r="E18" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G18" s="7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H18" s="7">
         <v>4</v>
@@ -1228,125 +1602,57 @@
       </c>
       <c r="K18" s="8">
         <f>SUM(B18:J18)</f>
-        <v>37</v>
-      </c>
-      <c r="L18" s="7">
-        <v>5</v>
-      </c>
-      <c r="M18" s="7">
-        <v>3</v>
-      </c>
-      <c r="N18" s="7">
-        <v>4</v>
-      </c>
-      <c r="O18" s="7">
-        <v>4</v>
-      </c>
-      <c r="P18" s="7">
-        <v>3</v>
-      </c>
-      <c r="Q18" s="7">
-        <v>2</v>
-      </c>
-      <c r="R18" s="7">
-        <v>4</v>
-      </c>
-      <c r="S18" s="7">
-        <v>4</v>
-      </c>
-      <c r="T18" s="7">
-        <v>4</v>
-      </c>
-      <c r="U18" s="8">
-        <f>SUM(L18:T18)</f>
         <v>33</v>
       </c>
-      <c r="V18" s="8">
-        <f>K18+U18</f>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="L18" s="8"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C19" s="7">
         <v>2</v>
       </c>
       <c r="D19" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E19" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" s="7">
         <v>2</v>
       </c>
       <c r="G19" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H19" s="7">
         <v>3</v>
       </c>
       <c r="I19" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J19" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K19" s="8">
         <f>SUM(B19:J19)</f>
-        <v>18</v>
-      </c>
-      <c r="L19" s="7">
-        <v>3</v>
-      </c>
-      <c r="M19" s="7">
-        <v>2</v>
-      </c>
-      <c r="N19" s="7">
-        <v>3</v>
-      </c>
-      <c r="O19" s="7">
-        <v>2</v>
-      </c>
-      <c r="P19" s="7">
-        <v>2</v>
-      </c>
-      <c r="Q19" s="7">
-        <v>1</v>
-      </c>
-      <c r="R19" s="7">
-        <v>3</v>
-      </c>
-      <c r="S19" s="7">
-        <v>3</v>
-      </c>
-      <c r="T19" s="7">
-        <v>2</v>
-      </c>
-      <c r="U19" s="8">
-        <f>SUM(L19:T19)</f>
         <v>21</v>
       </c>
-      <c r="V19" s="8">
-        <f>K19+U19</f>
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="L19" s="8"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
+      <c r="C20" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="D20" s="7"/>
-      <c r="E20" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
@@ -1354,20 +1660,8 @@
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
       <c r="L20" s="7"/>
-      <c r="M20" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="7"/>
-      <c r="S20" s="7"/>
-      <c r="T20" s="7"/>
-      <c r="U20" s="7"/>
-      <c r="V20" s="7"/>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>44090</v>
       </c>
@@ -1378,13 +1672,13 @@
         <v>4</v>
       </c>
       <c r="D22" s="7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E22" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F22" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G22" s="7">
         <v>4</v>
@@ -1393,63 +1687,29 @@
         <v>4</v>
       </c>
       <c r="I22" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J22" s="7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K22" s="8">
         <f>SUM(B22:J22)</f>
-        <v>34</v>
-      </c>
-      <c r="L22" s="7">
-        <v>4</v>
-      </c>
-      <c r="M22" s="7">
-        <v>4</v>
-      </c>
-      <c r="N22" s="7">
-        <v>5</v>
-      </c>
-      <c r="O22" s="7">
-        <v>3</v>
-      </c>
-      <c r="P22" s="7">
-        <v>4</v>
-      </c>
-      <c r="Q22" s="7">
-        <v>4</v>
-      </c>
-      <c r="R22" s="7">
-        <v>4</v>
-      </c>
-      <c r="S22" s="7">
-        <v>3</v>
-      </c>
-      <c r="T22" s="7">
-        <v>6</v>
-      </c>
-      <c r="U22" s="8">
-        <f>SUM(L22:T22)</f>
         <v>37</v>
       </c>
-      <c r="V22" s="8">
-        <f>K22+U22</f>
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="L22" s="8"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B23" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C23" s="7">
         <v>2</v>
       </c>
       <c r="D23" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E23" s="7">
         <v>2</v>
@@ -1458,10 +1718,10 @@
         <v>2</v>
       </c>
       <c r="G23" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H23" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I23" s="7">
         <v>2</v>
@@ -1471,79 +1731,29 @@
       </c>
       <c r="K23" s="8">
         <f>SUM(B23:J23)</f>
-        <v>21</v>
-      </c>
-      <c r="L23" s="7">
-        <v>2</v>
-      </c>
-      <c r="M23" s="7">
-        <v>2</v>
-      </c>
-      <c r="N23" s="7">
-        <v>3</v>
-      </c>
-      <c r="O23" s="7">
-        <v>2</v>
-      </c>
-      <c r="P23" s="7">
-        <v>2</v>
-      </c>
-      <c r="Q23" s="7">
-        <v>2</v>
-      </c>
-      <c r="R23" s="7">
-        <v>2</v>
-      </c>
-      <c r="S23" s="7">
-        <v>2</v>
-      </c>
-      <c r="T23" s="7">
-        <v>3</v>
-      </c>
-      <c r="U23" s="8">
-        <f>SUM(L23:T23)</f>
         <v>20</v>
       </c>
-      <c r="V23" s="8">
-        <f>K23+U23</f>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="L23" s="8"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
-      <c r="E24" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="E24" s="7"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
       <c r="J24" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="7"/>
-      <c r="Q24" s="7"/>
-      <c r="R24" s="7"/>
-      <c r="S24" s="7"/>
-      <c r="T24" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="U24" s="7"/>
-      <c r="V24" s="7"/>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="8"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -1556,18 +1766,8 @@
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="7"/>
-      <c r="O25" s="7"/>
-      <c r="P25" s="7"/>
-      <c r="Q25" s="7"/>
-      <c r="R25" s="7"/>
-      <c r="S25" s="7"/>
-      <c r="T25" s="7"/>
-      <c r="U25" s="7"/>
-      <c r="V25" s="7"/>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>44102</v>
       </c>
@@ -1578,19 +1778,19 @@
         <v>3</v>
       </c>
       <c r="D26" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E26" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F26" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G26" s="7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H26" s="7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I26" s="7">
         <v>5</v>
@@ -1600,45 +1800,11 @@
       </c>
       <c r="K26" s="8">
         <f>SUM(B26:J26)</f>
-        <v>34</v>
-      </c>
-      <c r="L26" s="7">
-        <v>4</v>
-      </c>
-      <c r="M26" s="7">
-        <v>3</v>
-      </c>
-      <c r="N26" s="7">
-        <v>5</v>
-      </c>
-      <c r="O26" s="7">
-        <v>4</v>
-      </c>
-      <c r="P26" s="7">
-        <v>4</v>
-      </c>
-      <c r="Q26" s="7">
-        <v>5</v>
-      </c>
-      <c r="R26" s="7">
-        <v>5</v>
-      </c>
-      <c r="S26" s="7">
-        <v>5</v>
-      </c>
-      <c r="T26" s="7">
-        <v>4</v>
-      </c>
-      <c r="U26" s="8">
-        <f>SUM(L26:T26)</f>
         <v>39</v>
       </c>
-      <c r="V26" s="8">
-        <f>K26+U26</f>
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="L26" s="8"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>8</v>
       </c>
@@ -1646,7 +1812,7 @@
         <v>2</v>
       </c>
       <c r="C27" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D27" s="7">
         <v>2</v>
@@ -1658,64 +1824,453 @@
         <v>2</v>
       </c>
       <c r="G27" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H27" s="7">
         <v>2</v>
       </c>
       <c r="I27" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J27" s="7">
         <v>2</v>
       </c>
       <c r="K27" s="8">
         <f>SUM(B27:J27)</f>
-        <v>16</v>
-      </c>
-      <c r="L27" s="7">
-        <v>2</v>
-      </c>
-      <c r="M27" s="7">
-        <v>2</v>
-      </c>
-      <c r="N27" s="7">
-        <v>2</v>
-      </c>
-      <c r="O27" s="7">
-        <v>2</v>
-      </c>
-      <c r="P27" s="7">
-        <v>2</v>
-      </c>
-      <c r="Q27" s="7">
-        <v>3</v>
-      </c>
-      <c r="R27" s="7">
-        <v>2</v>
-      </c>
-      <c r="S27" s="7">
-        <v>3</v>
-      </c>
-      <c r="T27" s="7">
-        <v>2</v>
-      </c>
-      <c r="U27" s="8">
-        <f>SUM(L27:T27)</f>
         <v>20</v>
       </c>
-      <c r="V27" s="8">
-        <f>K27+U27</f>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="L27" s="8"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9DD2039-084D-3C4E-B129-968266BAB55E}">
+  <dimension ref="A1:V30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1">
+        <v>7</v>
+      </c>
+      <c r="I2" s="1">
+        <v>8</v>
+      </c>
+      <c r="J2" s="1">
+        <v>9</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>125</v>
+      </c>
+      <c r="C4" s="1">
+        <v>150</v>
+      </c>
+      <c r="D4" s="1">
+        <v>118</v>
+      </c>
+      <c r="E4" s="1">
+        <v>117</v>
+      </c>
+      <c r="F4" s="1">
+        <v>134</v>
+      </c>
+      <c r="G4" s="1">
+        <v>174</v>
+      </c>
+      <c r="H4" s="1">
+        <v>136</v>
+      </c>
+      <c r="I4" s="1">
+        <v>100</v>
+      </c>
+      <c r="J4" s="1">
+        <v>155</v>
+      </c>
+      <c r="K4" s="1">
+        <v>1209</v>
+      </c>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>105</v>
+      </c>
+      <c r="C5" s="1">
+        <v>132</v>
+      </c>
+      <c r="D5" s="1">
+        <v>105</v>
+      </c>
+      <c r="E5" s="1">
+        <v>102</v>
+      </c>
+      <c r="F5" s="1">
+        <v>105</v>
+      </c>
+      <c r="G5" s="1">
+        <v>159</v>
+      </c>
+      <c r="H5" s="1">
+        <v>112</v>
+      </c>
+      <c r="I5" s="1">
+        <v>90</v>
+      </c>
+      <c r="J5" s="1">
+        <v>130</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1040</v>
+      </c>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1">
+        <v>77</v>
+      </c>
+      <c r="C6" s="1">
+        <v>117</v>
+      </c>
+      <c r="D6" s="1">
+        <v>90</v>
+      </c>
+      <c r="E6" s="1">
+        <v>92</v>
+      </c>
+      <c r="F6" s="1">
+        <v>77</v>
+      </c>
+      <c r="G6" s="1">
+        <v>93</v>
+      </c>
+      <c r="H6" s="1">
+        <v>85</v>
+      </c>
+      <c r="I6" s="1">
+        <v>78</v>
+      </c>
+      <c r="J6" s="1">
+        <v>110</v>
+      </c>
+      <c r="K6" s="1">
+        <v>819</v>
+      </c>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1">
+        <v>3</v>
+      </c>
+      <c r="F7" s="1">
+        <v>3</v>
+      </c>
+      <c r="G7" s="1">
+        <v>3</v>
+      </c>
+      <c r="H7" s="1">
+        <v>3</v>
+      </c>
+      <c r="I7" s="1">
+        <v>3</v>
+      </c>
+      <c r="J7" s="1">
+        <v>3</v>
+      </c>
+      <c r="K7" s="1">
+        <v>27</v>
+      </c>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" s="6"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="8"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" s="8"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="6"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" s="8"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" s="8"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" s="8"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" s="6"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" s="8"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28" s="8"/>
+      <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
@@ -1726,209 +2281,20 @@
       <c r="J28" s="7"/>
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
-      <c r="M28" s="7"/>
-      <c r="N28" s="7"/>
-      <c r="O28" s="7"/>
-      <c r="P28" s="7"/>
-      <c r="Q28" s="7"/>
-      <c r="R28" s="7"/>
-      <c r="S28" s="7"/>
-      <c r="T28" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="U28" s="7"/>
-      <c r="V28" s="7"/>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B31">
-        <f>AVERAGE(B10,B14,B18,B22,B26)</f>
-        <v>4</v>
-      </c>
-      <c r="C31">
-        <f t="shared" ref="C31:V31" si="0">AVERAGE(C10,C14,C18,C22,C26)</f>
-        <v>3.4</v>
-      </c>
-      <c r="D31">
-        <f t="shared" si="0"/>
-        <v>3.8</v>
-      </c>
-      <c r="E31">
-        <f t="shared" si="0"/>
-        <v>4.8</v>
-      </c>
-      <c r="F31">
-        <f t="shared" si="0"/>
-        <v>3.2</v>
-      </c>
-      <c r="G31">
-        <f t="shared" si="0"/>
-        <v>3.6</v>
-      </c>
-      <c r="H31">
-        <f t="shared" si="0"/>
-        <v>3.6</v>
-      </c>
-      <c r="I31">
-        <f t="shared" si="0"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="J31">
-        <f t="shared" si="0"/>
-        <v>4.8</v>
-      </c>
-      <c r="K31">
-        <f t="shared" si="0"/>
-        <v>35.6</v>
-      </c>
-      <c r="L31">
-        <f t="shared" si="0"/>
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="M31">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="N31">
-        <f t="shared" si="0"/>
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="O31">
-        <f t="shared" si="0"/>
-        <v>3.8</v>
-      </c>
-      <c r="P31">
-        <f t="shared" si="0"/>
-        <v>3.6</v>
-      </c>
-      <c r="Q31">
-        <f t="shared" si="0"/>
-        <v>3.8</v>
-      </c>
-      <c r="R31">
-        <f t="shared" si="0"/>
-        <v>4.8</v>
-      </c>
-      <c r="S31">
-        <f t="shared" si="0"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="T31">
-        <f t="shared" si="0"/>
-        <v>4.8</v>
-      </c>
-      <c r="U31">
-        <f t="shared" si="0"/>
-        <v>38.4</v>
-      </c>
-      <c r="V31">
-        <f t="shared" si="0"/>
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B32">
-        <f>AVERAGE(B11,B15,B19,B23,B26)</f>
-        <v>2.4</v>
-      </c>
-      <c r="C32">
-        <f t="shared" ref="C32:V32" si="1">AVERAGE(C11,C15,C19,C23,C26)</f>
-        <v>2</v>
-      </c>
-      <c r="D32">
-        <f t="shared" si="1"/>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E32">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="F32">
-        <f t="shared" si="1"/>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="G32">
-        <f t="shared" si="1"/>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H32">
-        <f t="shared" si="1"/>
-        <v>2.8</v>
-      </c>
-      <c r="I32">
-        <f t="shared" si="1"/>
-        <v>2.4</v>
-      </c>
-      <c r="J32">
-        <f t="shared" si="1"/>
-        <v>2.4</v>
-      </c>
-      <c r="K32">
-        <f t="shared" si="1"/>
-        <v>21.6</v>
-      </c>
-      <c r="L32">
-        <f t="shared" si="1"/>
-        <v>2.8</v>
-      </c>
-      <c r="M32">
-        <f t="shared" si="1"/>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="N32">
-        <f t="shared" si="1"/>
-        <v>3.4</v>
-      </c>
-      <c r="O32">
-        <f t="shared" si="1"/>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="P32">
-        <f t="shared" si="1"/>
-        <v>2.4</v>
-      </c>
-      <c r="Q32">
-        <f t="shared" si="1"/>
-        <v>2.4</v>
-      </c>
-      <c r="R32">
-        <f t="shared" si="1"/>
-        <v>3.2</v>
-      </c>
-      <c r="S32">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="T32">
-        <f t="shared" si="1"/>
-        <v>2.6</v>
-      </c>
-      <c r="U32">
-        <f t="shared" si="1"/>
-        <v>24.2</v>
-      </c>
-      <c r="V32">
-        <f t="shared" si="1"/>
-        <v>45.8</v>
-      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="K10 K14 K18:K19" formulaRange="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F45684-D9E4-2242-9821-C781990B9A28}">
   <dimension ref="A1:X12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1:F1"/>
     </sheetView>
   </sheetViews>
@@ -1936,16 +2302,16 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>18</v>
-      </c>
-      <c r="E1" t="s">
-        <v>19</v>
       </c>
       <c r="F1">
         <v>27511</v>

</xml_diff>

<commit_message>
Changed GolfReader to handle 9 hole golf xourses
</commit_message>
<xml_diff>
--- a/spec/fixtures/Golf.xlsx
+++ b/spec/fixtures/Golf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulkristoff/dev/golf/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B37E9CB-F085-C448-94B0-71DA35A3A1AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65AAC7EC-1521-054E-9125-5449F442CCD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1540" windowWidth="30200" windowHeight="17440" activeTab="2" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
+    <workbookView xWindow="2780" yWindow="1540" windowWidth="30200" windowHeight="17440" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
   </bookViews>
   <sheets>
     <sheet name="Knight's play 1-9" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="21">
   <si>
     <t>Hole</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>NC</t>
+  </si>
+  <si>
+    <t>2512 Ten Ten Rd</t>
+  </si>
+  <si>
+    <t>Apex</t>
   </si>
 </sst>
 </file>
@@ -477,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{045CE2A8-F6DB-4143-9691-363739FD69FB}">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K30" sqref="A30:K33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -486,6 +492,18 @@
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1">
+        <v>27539</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -1161,7 +1179,7 @@
   <dimension ref="A1:V30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1169,6 +1187,18 @@
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1">
+        <v>27539</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
@@ -1871,8 +1901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9DD2039-084D-3C4E-B129-968266BAB55E}">
   <dimension ref="A1:V30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1880,6 +1910,18 @@
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1">
+        <v>27539</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
started adding rounds & scores in GolfReader - reorganized  TeeHoleInfo
</commit_message>
<xml_diff>
--- a/spec/fixtures/Golf.xlsx
+++ b/spec/fixtures/Golf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulkristoff/dev/golf/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65AAC7EC-1521-054E-9125-5449F442CCD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C51157B-0808-724E-A947-3447EA028861}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1540" windowWidth="30200" windowHeight="17440" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
+    <workbookView xWindow="760" yWindow="460" windowWidth="15340" windowHeight="17440" activeTab="1" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
   </bookViews>
   <sheets>
     <sheet name="Knight's play 1-9" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="21">
   <si>
     <t>Hole</t>
   </si>
@@ -481,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{045CE2A8-F6DB-4143-9691-363739FD69FB}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -706,404 +706,320 @@
       <c r="A10" s="2">
         <v>44067</v>
       </c>
-      <c r="B10">
-        <v>4</v>
-      </c>
-      <c r="C10">
-        <v>4</v>
-      </c>
-      <c r="D10">
-        <v>4</v>
-      </c>
-      <c r="E10">
-        <v>5</v>
-      </c>
-      <c r="F10">
-        <v>3</v>
-      </c>
-      <c r="G10">
-        <v>5</v>
-      </c>
-      <c r="H10">
-        <v>3</v>
-      </c>
-      <c r="I10">
-        <v>6</v>
-      </c>
-      <c r="J10">
-        <v>5</v>
-      </c>
-      <c r="K10" s="1">
-        <f>SUM(B10:J10)</f>
-        <v>39</v>
-      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I11">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K11" s="1">
         <f>SUM(B11:J11)</f>
-        <v>17</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+      <c r="J12">
+        <v>2</v>
+      </c>
+      <c r="K12" s="1">
+        <f>SUM(B12:J12)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>10</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>10</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G13" t="s">
         <v>11</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I13" t="s">
         <v>11</v>
       </c>
-      <c r="K12" s="1"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
         <v>44074</v>
       </c>
-      <c r="B14">
-        <v>3</v>
-      </c>
-      <c r="C14">
-        <v>3</v>
-      </c>
-      <c r="D14">
-        <v>4</v>
-      </c>
-      <c r="E14">
-        <v>5</v>
-      </c>
-      <c r="F14">
-        <v>3</v>
-      </c>
-      <c r="G14">
-        <v>2</v>
-      </c>
-      <c r="H14">
-        <v>4</v>
-      </c>
-      <c r="I14">
-        <v>3</v>
-      </c>
-      <c r="J14">
-        <v>7</v>
-      </c>
-      <c r="K14" s="1">
-        <f>SUM(B14:J14)</f>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="D15">
-        <v>2</v>
-      </c>
-      <c r="E15">
-        <v>3</v>
-      </c>
-      <c r="F15">
-        <v>2</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15">
-        <v>3</v>
-      </c>
-      <c r="I15">
-        <v>2</v>
-      </c>
-      <c r="J15">
-        <v>2</v>
-      </c>
-      <c r="K15" s="1">
-        <f>SUM(B15:J15)</f>
-        <v>18</v>
-      </c>
+      <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>5</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="I16">
+        <v>3</v>
+      </c>
+      <c r="J16">
+        <v>7</v>
+      </c>
+      <c r="K16" s="1">
+        <f>SUM(B16:J16)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+      <c r="I17">
+        <v>2</v>
+      </c>
+      <c r="J17">
+        <v>2</v>
+      </c>
+      <c r="K17" s="1">
+        <f>SUM(B17:J17)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B18" t="s">
         <v>10</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D18" t="s">
         <v>10</v>
       </c>
-      <c r="K16" s="1"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="K17" s="1"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="6">
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K19" s="1"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="6">
         <v>44081</v>
       </c>
-      <c r="B18" s="7">
-        <v>5</v>
-      </c>
-      <c r="C18" s="7">
-        <v>3</v>
-      </c>
-      <c r="D18" s="7">
-        <v>4</v>
-      </c>
-      <c r="E18" s="7">
-        <v>5</v>
-      </c>
-      <c r="F18" s="7">
-        <v>4</v>
-      </c>
-      <c r="G18" s="7">
-        <v>4</v>
-      </c>
-      <c r="H18" s="7">
-        <v>4</v>
-      </c>
-      <c r="I18" s="7">
-        <v>4</v>
-      </c>
-      <c r="J18" s="7">
-        <v>4</v>
-      </c>
-      <c r="K18" s="8">
-        <f>SUM(B18:J18)</f>
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="7">
+        <v>5</v>
+      </c>
+      <c r="C21" s="7">
+        <v>3</v>
+      </c>
+      <c r="D21" s="7">
+        <v>4</v>
+      </c>
+      <c r="E21" s="7">
+        <v>5</v>
+      </c>
+      <c r="F21" s="7">
+        <v>4</v>
+      </c>
+      <c r="G21" s="7">
+        <v>4</v>
+      </c>
+      <c r="H21" s="7">
+        <v>4</v>
+      </c>
+      <c r="I21" s="7">
+        <v>4</v>
+      </c>
+      <c r="J21" s="7">
+        <v>4</v>
+      </c>
+      <c r="K21" s="8">
+        <f>SUM(B21:J21)</f>
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="8" t="s">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="7">
-        <v>2</v>
-      </c>
-      <c r="C19" s="7">
-        <v>2</v>
-      </c>
-      <c r="D19" s="7">
-        <v>2</v>
-      </c>
-      <c r="E19" s="7">
-        <v>3</v>
-      </c>
-      <c r="F19" s="7">
-        <v>2</v>
-      </c>
-      <c r="G19" s="7">
-        <v>2</v>
-      </c>
-      <c r="H19" s="7">
-        <v>3</v>
-      </c>
-      <c r="I19" s="7">
+      <c r="B22" s="7">
+        <v>2</v>
+      </c>
+      <c r="C22" s="7">
+        <v>2</v>
+      </c>
+      <c r="D22" s="7">
+        <v>2</v>
+      </c>
+      <c r="E22" s="7">
+        <v>3</v>
+      </c>
+      <c r="F22" s="7">
+        <v>2</v>
+      </c>
+      <c r="G22" s="7">
+        <v>2</v>
+      </c>
+      <c r="H22" s="7">
+        <v>3</v>
+      </c>
+      <c r="I22" s="7">
         <v>1</v>
       </c>
-      <c r="J19" s="7">
+      <c r="J22" s="7">
         <v>1</v>
-      </c>
-      <c r="K19" s="8">
-        <f>SUM(B19:J19)</f>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="6">
-        <v>44090</v>
-      </c>
-      <c r="B22" s="7">
-        <v>4</v>
-      </c>
-      <c r="C22" s="7">
-        <v>4</v>
-      </c>
-      <c r="D22" s="7">
-        <v>3</v>
-      </c>
-      <c r="E22" s="7">
-        <v>4</v>
-      </c>
-      <c r="F22" s="7">
-        <v>3</v>
-      </c>
-      <c r="G22" s="7">
-        <v>4</v>
-      </c>
-      <c r="H22" s="7">
-        <v>4</v>
-      </c>
-      <c r="I22" s="7">
-        <v>4</v>
-      </c>
-      <c r="J22" s="7">
-        <v>4</v>
       </c>
       <c r="K22" s="8">
         <f>SUM(B22:J22)</f>
-        <v>34</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="7">
-        <v>3</v>
-      </c>
-      <c r="C23" s="7">
-        <v>2</v>
-      </c>
-      <c r="D23" s="7">
+        <v>9</v>
+      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="6">
+        <v>44090</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E23" s="7">
-        <v>2</v>
-      </c>
-      <c r="F23" s="7">
-        <v>2</v>
-      </c>
-      <c r="G23" s="7">
-        <v>3</v>
-      </c>
-      <c r="H23" s="7">
-        <v>3</v>
-      </c>
-      <c r="I23" s="7">
-        <v>2</v>
-      </c>
-      <c r="J23" s="7">
-        <v>3</v>
-      </c>
-      <c r="K23" s="8">
-        <f>SUM(B23:J23)</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="K24" s="7"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="8"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="6">
-        <v>44102</v>
-      </c>
       <c r="B26" s="7">
         <v>4</v>
       </c>
       <c r="C26" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D26" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E26" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F26" s="7">
         <v>3</v>
       </c>
       <c r="G26" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H26" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I26" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J26" s="7">
         <v>4</v>
@@ -1118,14 +1034,14 @@
         <v>8</v>
       </c>
       <c r="B27" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C27" s="7">
+        <v>2</v>
+      </c>
+      <c r="D27" s="7">
         <v>1</v>
       </c>
-      <c r="D27" s="7">
-        <v>2</v>
-      </c>
       <c r="E27" s="7">
         <v>2</v>
       </c>
@@ -1133,20 +1049,20 @@
         <v>2</v>
       </c>
       <c r="G27" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H27" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I27" s="7">
         <v>2</v>
       </c>
       <c r="J27" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K27" s="8">
         <f>SUM(B27:J27)</f>
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -1158,28 +1074,150 @@
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
+      <c r="E28" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
+      <c r="J28" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="K28" s="7"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="8"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="6">
+        <v>44102</v>
+      </c>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="7">
+        <v>4</v>
+      </c>
+      <c r="C31" s="7">
+        <v>3</v>
+      </c>
+      <c r="D31" s="7">
+        <v>4</v>
+      </c>
+      <c r="E31" s="7">
+        <v>5</v>
+      </c>
+      <c r="F31" s="7">
+        <v>3</v>
+      </c>
+      <c r="G31" s="7">
+        <v>3</v>
+      </c>
+      <c r="H31" s="7">
+        <v>3</v>
+      </c>
+      <c r="I31" s="7">
+        <v>5</v>
+      </c>
+      <c r="J31" s="7">
+        <v>4</v>
+      </c>
+      <c r="K31" s="8">
+        <f>SUM(B31:J31)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="7">
+        <v>2</v>
+      </c>
+      <c r="C32" s="7">
+        <v>1</v>
+      </c>
+      <c r="D32" s="7">
+        <v>2</v>
+      </c>
+      <c r="E32" s="7">
+        <v>2</v>
+      </c>
+      <c r="F32" s="7">
+        <v>2</v>
+      </c>
+      <c r="G32" s="7">
+        <v>1</v>
+      </c>
+      <c r="H32" s="7">
+        <v>2</v>
+      </c>
+      <c r="I32" s="7">
+        <v>2</v>
+      </c>
+      <c r="J32" s="7">
+        <v>2</v>
+      </c>
+      <c r="K32" s="8">
+        <f>SUM(B32:J32)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <ignoredErrors>
-    <ignoredError sqref="K10 K14 K18:K19" formulaRange="1"/>
+    <ignoredError sqref="K11 K16 K21:K22" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8526A8B9-0C97-E94E-BA2A-E4D31B8BA027}">
-  <dimension ref="A1:V30"/>
+  <dimension ref="A1:V35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1427,410 +1465,330 @@
       <c r="A10" s="2">
         <v>44067</v>
       </c>
-      <c r="B10">
-        <v>4</v>
-      </c>
-      <c r="C10">
-        <v>6</v>
-      </c>
-      <c r="D10">
-        <v>5</v>
-      </c>
-      <c r="E10">
-        <v>4</v>
-      </c>
-      <c r="F10">
-        <v>4</v>
-      </c>
-      <c r="G10">
-        <v>4</v>
-      </c>
-      <c r="H10">
-        <v>6</v>
-      </c>
-      <c r="I10">
-        <v>6</v>
-      </c>
-      <c r="J10">
-        <v>5</v>
-      </c>
-      <c r="K10" s="1">
-        <f>SUM(B10:J10)</f>
-        <v>44</v>
-      </c>
-      <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H11">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I11">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K11" s="1">
         <f>SUM(B11:J11)</f>
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12">
+        <v>3</v>
+      </c>
+      <c r="I12">
+        <v>3</v>
+      </c>
+      <c r="J12">
+        <v>2</v>
+      </c>
+      <c r="K12" s="1">
+        <f>SUM(B12:J12)</f>
+        <v>20</v>
+      </c>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+      <c r="A14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
         <v>44074</v>
       </c>
-      <c r="B14">
-        <v>6</v>
-      </c>
-      <c r="C14">
-        <v>4</v>
-      </c>
-      <c r="D14">
-        <v>4</v>
-      </c>
-      <c r="E14">
-        <v>4</v>
-      </c>
-      <c r="F14">
-        <v>3</v>
-      </c>
-      <c r="G14">
-        <v>4</v>
-      </c>
-      <c r="H14">
-        <v>5</v>
-      </c>
-      <c r="I14">
-        <v>4</v>
-      </c>
-      <c r="J14">
-        <v>5</v>
-      </c>
-      <c r="K14" s="1">
-        <f>SUM(B14:J14)</f>
-        <v>39</v>
-      </c>
-      <c r="L14" s="1"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15">
-        <v>3</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="D15">
-        <v>3</v>
-      </c>
-      <c r="E15">
-        <v>2</v>
-      </c>
-      <c r="F15">
-        <v>2</v>
-      </c>
-      <c r="G15">
-        <v>2</v>
-      </c>
-      <c r="H15">
-        <v>3</v>
-      </c>
-      <c r="I15">
-        <v>2</v>
-      </c>
-      <c r="J15">
-        <v>2</v>
-      </c>
-      <c r="K15" s="1">
-        <f>SUM(B15:J15)</f>
-        <v>21</v>
-      </c>
+      <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
+      </c>
+      <c r="G16">
+        <v>4</v>
+      </c>
+      <c r="H16">
+        <v>5</v>
+      </c>
+      <c r="I16">
+        <v>4</v>
+      </c>
+      <c r="J16">
+        <v>5</v>
+      </c>
+      <c r="K16" s="1">
+        <f>SUM(B16:J16)</f>
+        <v>39</v>
+      </c>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+      <c r="I17">
+        <v>2</v>
+      </c>
+      <c r="J17">
+        <v>2</v>
+      </c>
+      <c r="K17" s="1">
+        <f>SUM(B17:J17)</f>
+        <v>21</v>
+      </c>
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C18" t="s">
         <v>12</v>
       </c>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="6">
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" s="6">
         <v>44081</v>
       </c>
-      <c r="B18" s="7">
-        <v>5</v>
-      </c>
-      <c r="C18" s="7">
-        <v>3</v>
-      </c>
-      <c r="D18" s="7">
-        <v>4</v>
-      </c>
-      <c r="E18" s="7">
-        <v>4</v>
-      </c>
-      <c r="F18" s="7">
-        <v>3</v>
-      </c>
-      <c r="G18" s="7">
-        <v>2</v>
-      </c>
-      <c r="H18" s="7">
-        <v>4</v>
-      </c>
-      <c r="I18" s="7">
-        <v>4</v>
-      </c>
-      <c r="J18" s="7">
-        <v>4</v>
-      </c>
-      <c r="K18" s="8">
-        <f>SUM(B18:J18)</f>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="7">
+        <v>5</v>
+      </c>
+      <c r="C21" s="7">
+        <v>3</v>
+      </c>
+      <c r="D21" s="7">
+        <v>4</v>
+      </c>
+      <c r="E21" s="7">
+        <v>4</v>
+      </c>
+      <c r="F21" s="7">
+        <v>3</v>
+      </c>
+      <c r="G21" s="7">
+        <v>2</v>
+      </c>
+      <c r="H21" s="7">
+        <v>4</v>
+      </c>
+      <c r="I21" s="7">
+        <v>4</v>
+      </c>
+      <c r="J21" s="7">
+        <v>4</v>
+      </c>
+      <c r="K21" s="8">
+        <f>SUM(B21:J21)</f>
         <v>33</v>
       </c>
-      <c r="L18" s="8"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="8" t="s">
+      <c r="L21" s="8"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="7">
-        <v>3</v>
-      </c>
-      <c r="C19" s="7">
-        <v>2</v>
-      </c>
-      <c r="D19" s="7">
-        <v>3</v>
-      </c>
-      <c r="E19" s="7">
-        <v>2</v>
-      </c>
-      <c r="F19" s="7">
-        <v>2</v>
-      </c>
-      <c r="G19" s="7">
+      <c r="B22" s="7">
+        <v>3</v>
+      </c>
+      <c r="C22" s="7">
+        <v>2</v>
+      </c>
+      <c r="D22" s="7">
+        <v>3</v>
+      </c>
+      <c r="E22" s="7">
+        <v>2</v>
+      </c>
+      <c r="F22" s="7">
+        <v>2</v>
+      </c>
+      <c r="G22" s="7">
         <v>1</v>
       </c>
-      <c r="H19" s="7">
-        <v>3</v>
-      </c>
-      <c r="I19" s="7">
-        <v>3</v>
-      </c>
-      <c r="J19" s="7">
-        <v>2</v>
-      </c>
-      <c r="K19" s="8">
-        <f>SUM(B19:J19)</f>
-        <v>21</v>
-      </c>
-      <c r="L19" s="8"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="6">
-        <v>44090</v>
-      </c>
-      <c r="B22" s="7">
-        <v>4</v>
-      </c>
-      <c r="C22" s="7">
-        <v>4</v>
-      </c>
-      <c r="D22" s="7">
-        <v>5</v>
-      </c>
-      <c r="E22" s="7">
-        <v>3</v>
-      </c>
-      <c r="F22" s="7">
-        <v>4</v>
-      </c>
-      <c r="G22" s="7">
-        <v>4</v>
-      </c>
       <c r="H22" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I22" s="7">
         <v>3</v>
       </c>
       <c r="J22" s="7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K22" s="8">
         <f>SUM(B22:J22)</f>
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="L22" s="8"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="7">
-        <v>2</v>
-      </c>
-      <c r="C23" s="7">
-        <v>2</v>
-      </c>
-      <c r="D23" s="7">
-        <v>3</v>
-      </c>
-      <c r="E23" s="7">
-        <v>2</v>
-      </c>
-      <c r="F23" s="7">
-        <v>2</v>
-      </c>
-      <c r="G23" s="7">
-        <v>2</v>
-      </c>
-      <c r="H23" s="7">
-        <v>2</v>
-      </c>
-      <c r="I23" s="7">
-        <v>2</v>
-      </c>
-      <c r="J23" s="7">
-        <v>3</v>
-      </c>
-      <c r="K23" s="8">
-        <f>SUM(B23:J23)</f>
-        <v>20</v>
-      </c>
-      <c r="L23" s="8"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7" t="s">
+      <c r="B23" s="7"/>
+      <c r="C23" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="8"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
+      <c r="A25" s="6">
+        <v>44090</v>
+      </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="6">
-        <v>44102</v>
+      <c r="A26" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="B26" s="7">
         <v>4</v>
       </c>
       <c r="C26" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D26" s="7">
         <v>5</v>
       </c>
       <c r="E26" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F26" s="7">
         <v>4</v>
       </c>
       <c r="G26" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H26" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I26" s="7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J26" s="7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K26" s="8">
         <f>SUM(B26:J26)</f>
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L26" s="8"/>
     </row>
@@ -1845,7 +1803,7 @@
         <v>2</v>
       </c>
       <c r="D27" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E27" s="7">
         <v>2</v>
@@ -1854,16 +1812,16 @@
         <v>2</v>
       </c>
       <c r="G27" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H27" s="7">
         <v>2</v>
       </c>
       <c r="I27" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J27" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K27" s="8">
         <f>SUM(B27:J27)</f>
@@ -1889,11 +1847,132 @@
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
     </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A29" s="8"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+    </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="1"/>
+      <c r="A30" s="6">
+        <v>44102</v>
+      </c>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="7">
+        <v>4</v>
+      </c>
+      <c r="C31" s="7">
+        <v>3</v>
+      </c>
+      <c r="D31" s="7">
+        <v>5</v>
+      </c>
+      <c r="E31" s="7">
+        <v>4</v>
+      </c>
+      <c r="F31" s="7">
+        <v>4</v>
+      </c>
+      <c r="G31" s="7">
+        <v>5</v>
+      </c>
+      <c r="H31" s="7">
+        <v>5</v>
+      </c>
+      <c r="I31" s="7">
+        <v>5</v>
+      </c>
+      <c r="J31" s="7">
+        <v>4</v>
+      </c>
+      <c r="K31" s="8">
+        <f>SUM(B31:J31)</f>
+        <v>39</v>
+      </c>
+      <c r="L31" s="8"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="7">
+        <v>2</v>
+      </c>
+      <c r="C32" s="7">
+        <v>2</v>
+      </c>
+      <c r="D32" s="7">
+        <v>2</v>
+      </c>
+      <c r="E32" s="7">
+        <v>2</v>
+      </c>
+      <c r="F32" s="7">
+        <v>2</v>
+      </c>
+      <c r="G32" s="7">
+        <v>3</v>
+      </c>
+      <c r="H32" s="7">
+        <v>2</v>
+      </c>
+      <c r="I32" s="7">
+        <v>3</v>
+      </c>
+      <c r="J32" s="7">
+        <v>2</v>
+      </c>
+      <c r="K32" s="8">
+        <f>SUM(B32:J32)</f>
+        <v>20</v>
+      </c>
+      <c r="L32" s="8"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A33" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A35" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2334,10 +2413,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F45684-D9E4-2242-9821-C781990B9A28}">
-  <dimension ref="A1:X12"/>
+  <dimension ref="A1:X13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:F1"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2537,7 +2616,7 @@
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5">
@@ -2826,179 +2905,205 @@
       </c>
       <c r="W8" s="1"/>
     </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+    </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>44042</v>
       </c>
-      <c r="B10" s="1">
-        <v>71.599999999999994</v>
-      </c>
-      <c r="C10" s="1">
-        <v>139</v>
-      </c>
-      <c r="D10">
-        <v>7</v>
-      </c>
-      <c r="E10">
-        <v>6</v>
-      </c>
-      <c r="F10">
-        <v>8</v>
-      </c>
-      <c r="G10">
-        <v>5</v>
-      </c>
-      <c r="H10">
-        <v>5</v>
-      </c>
-      <c r="I10">
-        <v>5</v>
-      </c>
-      <c r="J10">
-        <v>5</v>
-      </c>
-      <c r="K10" s="3">
-        <v>7</v>
-      </c>
-      <c r="L10" s="3">
-        <v>5</v>
-      </c>
-      <c r="M10" s="1">
-        <f>SUM(D10:L10)</f>
-        <v>53</v>
-      </c>
-      <c r="N10">
-        <v>8</v>
-      </c>
-      <c r="O10">
-        <v>4</v>
-      </c>
-      <c r="P10">
-        <v>8</v>
-      </c>
-      <c r="Q10">
-        <v>6</v>
-      </c>
-      <c r="R10">
-        <v>7</v>
-      </c>
-      <c r="S10">
-        <v>5</v>
-      </c>
-      <c r="T10">
-        <v>10</v>
-      </c>
-      <c r="U10" s="3">
-        <v>5</v>
-      </c>
-      <c r="V10" s="3">
-        <v>6</v>
-      </c>
-      <c r="W10" s="1">
-        <f>SUM(N10:V10)</f>
-        <v>59</v>
-      </c>
-      <c r="X10" s="1">
-        <f>M10+W10</f>
-        <v>112</v>
-      </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11">
+        <v>7</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
+      <c r="F11">
         <v>8</v>
       </c>
-      <c r="D11">
-        <v>3</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-      <c r="F11">
-        <v>3</v>
-      </c>
       <c r="G11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K11" s="3">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="L11" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M11" s="1">
         <f>SUM(D11:L11)</f>
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="N11">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="O11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P11">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="Q11">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="R11">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="S11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="T11">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="U11" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="V11" s="3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="W11" s="1">
         <f>SUM(N11:V11)</f>
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="X11" s="1">
         <f>M11+W11</f>
-        <v>37</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>2</v>
+      </c>
+      <c r="K12" s="3">
+        <v>2</v>
+      </c>
+      <c r="L12" s="3">
+        <v>1</v>
+      </c>
+      <c r="M12" s="1">
+        <f>SUM(D12:L12)</f>
+        <v>18</v>
+      </c>
+      <c r="N12">
+        <v>3</v>
+      </c>
+      <c r="O12">
+        <v>2</v>
+      </c>
+      <c r="P12">
+        <v>2</v>
+      </c>
+      <c r="Q12">
+        <v>2</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>2</v>
+      </c>
+      <c r="T12">
+        <v>2</v>
+      </c>
+      <c r="U12" s="3">
+        <v>3</v>
+      </c>
+      <c r="V12" s="3">
+        <v>2</v>
+      </c>
+      <c r="W12" s="1">
+        <f>SUM(N12:V12)</f>
+        <v>19</v>
+      </c>
+      <c r="X12" s="1">
+        <f>M12+W12</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G13" t="s">
         <v>12</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J13" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="1"/>
-      <c r="N12" t="s">
+      <c r="K13" s="1"/>
+      <c r="N13" t="s">
         <v>12</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="Q13" t="s">
         <v>12</v>
       </c>
-      <c r="R12" t="s">
+      <c r="R13" t="s">
         <v>12</v>
       </c>
-      <c r="T12" t="s">
+      <c r="T13" t="s">
         <v>12</v>
       </c>
-      <c r="U12" s="1"/>
-      <c r="V12" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added reading & writing of Rounds
</commit_message>
<xml_diff>
--- a/spec/fixtures/Golf.xlsx
+++ b/spec/fixtures/Golf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulkristoff/dev/golf/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C51157B-0808-724E-A947-3447EA028861}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004EBCD8-95B0-7A46-BE01-2C91DD80BE1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="460" windowWidth="15340" windowHeight="17440" activeTab="1" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
+    <workbookView xWindow="2180" yWindow="980" windowWidth="17600" windowHeight="17440" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
   </bookViews>
   <sheets>
     <sheet name="Knight's play 1-9" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="22">
   <si>
     <t>Hole</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>putts</t>
-  </si>
-  <si>
-    <t>penities</t>
   </si>
   <si>
     <t>M</t>
@@ -99,6 +96,12 @@
   </si>
   <si>
     <t>Apex</t>
+  </si>
+  <si>
+    <t>WW</t>
+  </si>
+  <si>
+    <t>penalties</t>
   </si>
 </sst>
 </file>
@@ -483,24 +486,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{045CE2A8-F6DB-4143-9691-363739FD69FB}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
-        <v>20</v>
-      </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F1">
         <v>27539</v>
@@ -781,19 +784,19 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
         <v>9</v>
       </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" t="s">
         <v>10</v>
       </c>
-      <c r="D13" t="s">
+      <c r="I13" t="s">
         <v>10</v>
-      </c>
-      <c r="G13" t="s">
-        <v>11</v>
-      </c>
-      <c r="I13" t="s">
-        <v>11</v>
       </c>
       <c r="K13" s="1"/>
     </row>
@@ -880,13 +883,13 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
         <v>9</v>
       </c>
-      <c r="B18" t="s">
-        <v>10</v>
-      </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K18" s="1"/>
     </row>
@@ -973,13 +976,13 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
@@ -1067,22 +1070,22 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>10</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
       <c r="J28" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K28" s="7"/>
     </row>
@@ -1188,10 +1191,10 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>10</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
@@ -1216,24 +1219,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8526A8B9-0C97-E94E-BA2A-E4D31B8BA027}">
   <dimension ref="A1:V35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
-        <v>20</v>
-      </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F1">
         <v>27539</v>
@@ -1542,10 +1545,10 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -1638,10 +1641,10 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -1734,11 +1737,11 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
@@ -1831,7 +1834,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -1842,7 +1845,7 @@
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
       <c r="J28" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
@@ -1953,7 +1956,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -1988,16 +1991,16 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
-        <v>20</v>
-      </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F1">
         <v>27539</v>
@@ -2413,26 +2416,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F45684-D9E4-2242-9821-C781990B9A28}">
-  <dimension ref="A1:X13"/>
+  <dimension ref="A1:X18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>17</v>
-      </c>
-      <c r="E1" t="s">
-        <v>18</v>
       </c>
       <c r="F1">
         <v>27511</v>
@@ -2443,10 +2446,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -3081,29 +3084,194 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="G13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K13" s="1"/>
       <c r="N13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="T13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>44139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16">
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <v>6</v>
+      </c>
+      <c r="F16">
+        <v>7</v>
+      </c>
+      <c r="G16">
+        <v>8</v>
+      </c>
+      <c r="H16">
+        <v>6</v>
+      </c>
+      <c r="I16">
+        <v>6</v>
+      </c>
+      <c r="J16">
+        <v>4</v>
+      </c>
+      <c r="K16" s="3">
+        <v>5</v>
+      </c>
+      <c r="L16" s="3">
+        <v>7</v>
+      </c>
+      <c r="M16" s="1">
+        <v>55</v>
+      </c>
+      <c r="N16">
+        <v>7</v>
+      </c>
+      <c r="O16">
+        <v>6</v>
+      </c>
+      <c r="P16">
+        <v>8</v>
+      </c>
+      <c r="Q16">
+        <v>5</v>
+      </c>
+      <c r="R16">
+        <v>6</v>
+      </c>
+      <c r="S16">
+        <v>5</v>
+      </c>
+      <c r="T16">
+        <v>7</v>
+      </c>
+      <c r="U16" s="3">
+        <v>6</v>
+      </c>
+      <c r="V16" s="3">
+        <v>6</v>
+      </c>
+      <c r="W16" s="1">
+        <f>SUM(N16:V16)</f>
+        <v>56</v>
+      </c>
+      <c r="X16" s="1">
+        <f>M16+W16</f>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="I17">
+        <v>3</v>
+      </c>
+      <c r="J17">
+        <v>3</v>
+      </c>
+      <c r="K17" s="3">
+        <v>1</v>
+      </c>
+      <c r="L17" s="3">
+        <v>2</v>
+      </c>
+      <c r="M17" s="1">
+        <f>SUM(D17:L17)</f>
+        <v>18</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <v>2</v>
+      </c>
+      <c r="P17">
+        <v>3</v>
+      </c>
+      <c r="Q17">
+        <v>2</v>
+      </c>
+      <c r="R17">
+        <v>2</v>
+      </c>
+      <c r="S17">
+        <v>1</v>
+      </c>
+      <c r="T17">
+        <v>2</v>
+      </c>
+      <c r="U17" s="3">
+        <v>1</v>
+      </c>
+      <c r="V17" s="3">
+        <v>2</v>
+      </c>
+      <c r="W17" s="1">
+        <f>SUM(N17:V17)</f>
+        <v>16</v>
+      </c>
+      <c r="X17" s="1">
+        <f>M17+W17</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" t="s">
+        <v>11</v>
+      </c>
+      <c r="K18" s="1"/>
+      <c r="R18" t="s">
+        <v>11</v>
+      </c>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Implemented showing tees for course, show round for given course and tee, button to show tees for course on the side
</commit_message>
<xml_diff>
--- a/spec/fixtures/Golf.xlsx
+++ b/spec/fixtures/Golf.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulkristoff/dev/golf/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004EBCD8-95B0-7A46-BE01-2C91DD80BE1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D938A41-0FE7-AF41-BE5D-FACD8883A9CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2180" yWindow="980" windowWidth="17600" windowHeight="17440" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
+    <workbookView xWindow="2180" yWindow="980" windowWidth="17600" windowHeight="17440" activeTab="3" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
   </bookViews>
   <sheets>
     <sheet name="Knight's play 1-9" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="23">
   <si>
     <t>Hole</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>penalties</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -486,7 +489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{045CE2A8-F6DB-4143-9691-363739FD69FB}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -2416,10 +2419,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F45684-D9E4-2242-9821-C781990B9A28}">
-  <dimension ref="A1:X18"/>
+  <dimension ref="A1:X28"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="M2" workbookViewId="0">
+      <selection activeCell="X27" sqref="X27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3273,6 +3276,332 @@
       <c r="U18" s="1"/>
       <c r="V18" s="1"/>
     </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>44294</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21">
+        <v>6</v>
+      </c>
+      <c r="E21">
+        <v>6</v>
+      </c>
+      <c r="F21">
+        <v>5</v>
+      </c>
+      <c r="G21">
+        <v>6</v>
+      </c>
+      <c r="H21">
+        <v>5</v>
+      </c>
+      <c r="I21">
+        <v>5</v>
+      </c>
+      <c r="J21">
+        <v>5</v>
+      </c>
+      <c r="K21" s="3">
+        <v>6</v>
+      </c>
+      <c r="L21" s="3">
+        <v>7</v>
+      </c>
+      <c r="M21" s="1">
+        <v>51</v>
+      </c>
+      <c r="N21">
+        <v>5</v>
+      </c>
+      <c r="O21">
+        <v>7</v>
+      </c>
+      <c r="P21">
+        <v>10</v>
+      </c>
+      <c r="Q21">
+        <v>5</v>
+      </c>
+      <c r="R21">
+        <v>5</v>
+      </c>
+      <c r="S21">
+        <v>5</v>
+      </c>
+      <c r="T21">
+        <v>6</v>
+      </c>
+      <c r="U21" s="3">
+        <v>6</v>
+      </c>
+      <c r="V21" s="3">
+        <v>5</v>
+      </c>
+      <c r="W21" s="1">
+        <v>54</v>
+      </c>
+      <c r="X21" s="1">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+      <c r="I22">
+        <v>2</v>
+      </c>
+      <c r="J22">
+        <v>2</v>
+      </c>
+      <c r="K22" s="3">
+        <v>2</v>
+      </c>
+      <c r="L22" s="3">
+        <v>2</v>
+      </c>
+      <c r="M22" s="1">
+        <v>18</v>
+      </c>
+      <c r="N22">
+        <v>2</v>
+      </c>
+      <c r="O22">
+        <v>3</v>
+      </c>
+      <c r="P22">
+        <v>2</v>
+      </c>
+      <c r="Q22">
+        <v>2</v>
+      </c>
+      <c r="R22">
+        <v>2</v>
+      </c>
+      <c r="S22">
+        <v>2</v>
+      </c>
+      <c r="T22">
+        <v>2</v>
+      </c>
+      <c r="U22" s="3">
+        <v>2</v>
+      </c>
+      <c r="V22" s="3">
+        <v>2</v>
+      </c>
+      <c r="W22" s="1">
+        <v>19</v>
+      </c>
+      <c r="X22" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I23" t="s">
+        <v>9</v>
+      </c>
+      <c r="J23" t="s">
+        <v>11</v>
+      </c>
+      <c r="K23" s="1"/>
+      <c r="P23" t="s">
+        <v>11</v>
+      </c>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>44301</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26">
+        <v>9</v>
+      </c>
+      <c r="E26">
+        <v>5</v>
+      </c>
+      <c r="F26">
+        <v>4</v>
+      </c>
+      <c r="G26">
+        <v>6</v>
+      </c>
+      <c r="H26">
+        <v>6</v>
+      </c>
+      <c r="I26">
+        <v>6</v>
+      </c>
+      <c r="J26">
+        <v>5</v>
+      </c>
+      <c r="K26" s="3">
+        <v>6</v>
+      </c>
+      <c r="L26" s="3">
+        <v>8</v>
+      </c>
+      <c r="M26" s="1">
+        <v>55</v>
+      </c>
+      <c r="N26">
+        <v>8</v>
+      </c>
+      <c r="O26">
+        <v>5</v>
+      </c>
+      <c r="P26">
+        <v>6</v>
+      </c>
+      <c r="Q26">
+        <v>7</v>
+      </c>
+      <c r="R26">
+        <v>6</v>
+      </c>
+      <c r="S26">
+        <v>6</v>
+      </c>
+      <c r="T26">
+        <v>7</v>
+      </c>
+      <c r="U26" s="3">
+        <v>6</v>
+      </c>
+      <c r="V26" s="3">
+        <v>6</v>
+      </c>
+      <c r="W26" s="1">
+        <v>57</v>
+      </c>
+      <c r="X26" s="1">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>2</v>
+      </c>
+      <c r="H27">
+        <v>2</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>2</v>
+      </c>
+      <c r="K27" s="3">
+        <v>2</v>
+      </c>
+      <c r="L27" s="3">
+        <v>3</v>
+      </c>
+      <c r="M27" s="1">
+        <v>18</v>
+      </c>
+      <c r="N27">
+        <v>2</v>
+      </c>
+      <c r="O27">
+        <v>3</v>
+      </c>
+      <c r="P27">
+        <v>2</v>
+      </c>
+      <c r="Q27">
+        <v>2</v>
+      </c>
+      <c r="R27">
+        <v>1</v>
+      </c>
+      <c r="S27">
+        <v>2</v>
+      </c>
+      <c r="T27">
+        <v>1</v>
+      </c>
+      <c r="U27" s="3">
+        <v>2</v>
+      </c>
+      <c r="V27" s="3">
+        <v>2</v>
+      </c>
+      <c r="W27" s="1">
+        <v>17</v>
+      </c>
+      <c r="X27" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F28" t="s">
+        <v>11</v>
+      </c>
+      <c r="I28" t="s">
+        <v>11</v>
+      </c>
+      <c r="K28" s="1"/>
+      <c r="P28" t="s">
+        <v>22</v>
+      </c>
+      <c r="T28" t="s">
+        <v>11</v>
+      </c>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
swiching to using ScoreHoles for many-to-many
</commit_message>
<xml_diff>
--- a/spec/fixtures/Golf.xlsx
+++ b/spec/fixtures/Golf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulkristoff/dev/golf/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D938A41-0FE7-AF41-BE5D-FACD8883A9CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4E9796-B4C8-D342-8094-1845654FFFCF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2180" yWindow="980" windowWidth="17600" windowHeight="17440" activeTab="3" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="24">
   <si>
     <t>Hole</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>LB</t>
   </si>
 </sst>
 </file>
@@ -2419,10 +2422,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F45684-D9E4-2242-9821-C781990B9A28}">
-  <dimension ref="A1:X28"/>
+  <dimension ref="A1:X33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M2" workbookViewId="0">
-      <selection activeCell="X27" sqref="X27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3602,6 +3605,182 @@
       <c r="U28" s="1"/>
       <c r="V28" s="1"/>
     </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <v>44308</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31">
+        <v>8</v>
+      </c>
+      <c r="E31">
+        <v>4</v>
+      </c>
+      <c r="F31">
+        <v>6</v>
+      </c>
+      <c r="G31">
+        <v>5</v>
+      </c>
+      <c r="H31">
+        <v>5</v>
+      </c>
+      <c r="I31">
+        <v>6</v>
+      </c>
+      <c r="J31">
+        <v>6</v>
+      </c>
+      <c r="K31" s="3">
+        <v>6</v>
+      </c>
+      <c r="L31" s="3">
+        <v>8</v>
+      </c>
+      <c r="M31" s="1">
+        <v>54</v>
+      </c>
+      <c r="N31">
+        <v>6</v>
+      </c>
+      <c r="O31">
+        <v>3</v>
+      </c>
+      <c r="P31">
+        <v>6</v>
+      </c>
+      <c r="Q31">
+        <v>8</v>
+      </c>
+      <c r="R31">
+        <v>10</v>
+      </c>
+      <c r="S31">
+        <v>6</v>
+      </c>
+      <c r="T31">
+        <v>7</v>
+      </c>
+      <c r="U31" s="3">
+        <v>6</v>
+      </c>
+      <c r="V31" s="3">
+        <v>5</v>
+      </c>
+      <c r="W31" s="1">
+        <v>57</v>
+      </c>
+      <c r="X31" s="1">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32">
+        <v>4</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>3</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>2</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>2</v>
+      </c>
+      <c r="K32" s="3">
+        <v>2</v>
+      </c>
+      <c r="L32" s="3">
+        <v>2</v>
+      </c>
+      <c r="M32" s="1">
+        <v>18</v>
+      </c>
+      <c r="N32">
+        <v>2</v>
+      </c>
+      <c r="O32">
+        <v>3</v>
+      </c>
+      <c r="P32">
+        <v>2</v>
+      </c>
+      <c r="Q32">
+        <v>2</v>
+      </c>
+      <c r="R32">
+        <v>1</v>
+      </c>
+      <c r="S32">
+        <v>2</v>
+      </c>
+      <c r="T32">
+        <v>1</v>
+      </c>
+      <c r="U32" s="3">
+        <v>2</v>
+      </c>
+      <c r="V32" s="3">
+        <v>2</v>
+      </c>
+      <c r="W32" s="1">
+        <v>17</v>
+      </c>
+      <c r="X32" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F33" t="s">
+        <v>11</v>
+      </c>
+      <c r="I33" t="s">
+        <v>11</v>
+      </c>
+      <c r="J33" t="s">
+        <v>11</v>
+      </c>
+      <c r="K33" s="1"/>
+      <c r="P33" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>23</v>
+      </c>
+      <c r="R33" t="s">
+        <v>11</v>
+      </c>
+      <c r="T33" t="s">
+        <v>11</v>
+      </c>
+      <c r="U33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="V33" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Found & fixed problem with reading/writing xlsx: tee.sorted_holes. Added  editing scores
</commit_message>
<xml_diff>
--- a/spec/fixtures/Golf.xlsx
+++ b/spec/fixtures/Golf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulkristoff/dev/golf/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4E9796-B4C8-D342-8094-1845654FFFCF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07657EFB-4AFE-C14F-A72E-35994E9D01D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2180" yWindow="980" windowWidth="17600" windowHeight="17440" activeTab="3" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
+    <workbookView xWindow="15380" yWindow="1180" windowWidth="17600" windowHeight="17440" activeTab="3" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
   </bookViews>
   <sheets>
     <sheet name="Knight's play 1-9" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="24">
   <si>
     <t>Hole</t>
   </si>
@@ -1226,7 +1226,7 @@
   <dimension ref="A1:V35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A35" sqref="A35:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2422,10 +2422,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F45684-D9E4-2242-9821-C781990B9A28}">
-  <dimension ref="A1:X33"/>
+  <dimension ref="A1:X38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="X37" sqref="X37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3748,7 +3748,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>21</v>
       </c>
@@ -3780,6 +3780,180 @@
       <c r="V33" s="1" t="s">
         <v>23</v>
       </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <v>44315</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36">
+        <v>5</v>
+      </c>
+      <c r="E36">
+        <v>4</v>
+      </c>
+      <c r="F36">
+        <v>4</v>
+      </c>
+      <c r="G36">
+        <v>8</v>
+      </c>
+      <c r="H36">
+        <v>6</v>
+      </c>
+      <c r="I36">
+        <v>5</v>
+      </c>
+      <c r="J36">
+        <v>4</v>
+      </c>
+      <c r="K36" s="3">
+        <v>6</v>
+      </c>
+      <c r="L36" s="3">
+        <v>7</v>
+      </c>
+      <c r="M36" s="1">
+        <v>49</v>
+      </c>
+      <c r="N36">
+        <v>6</v>
+      </c>
+      <c r="O36">
+        <v>7</v>
+      </c>
+      <c r="P36">
+        <v>5</v>
+      </c>
+      <c r="Q36">
+        <v>5</v>
+      </c>
+      <c r="R36">
+        <v>6</v>
+      </c>
+      <c r="S36">
+        <v>5</v>
+      </c>
+      <c r="T36">
+        <v>7</v>
+      </c>
+      <c r="U36" s="3">
+        <v>0</v>
+      </c>
+      <c r="V36" s="3">
+        <v>0</v>
+      </c>
+      <c r="W36" s="1">
+        <v>41</v>
+      </c>
+      <c r="X36" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>2</v>
+      </c>
+      <c r="H37">
+        <v>2</v>
+      </c>
+      <c r="I37">
+        <v>2</v>
+      </c>
+      <c r="J37">
+        <v>2</v>
+      </c>
+      <c r="K37" s="3">
+        <v>2</v>
+      </c>
+      <c r="L37" s="3">
+        <v>2</v>
+      </c>
+      <c r="M37" s="1">
+        <v>16</v>
+      </c>
+      <c r="N37">
+        <v>2</v>
+      </c>
+      <c r="O37">
+        <v>2</v>
+      </c>
+      <c r="P37">
+        <v>1</v>
+      </c>
+      <c r="Q37">
+        <v>2</v>
+      </c>
+      <c r="R37">
+        <v>2</v>
+      </c>
+      <c r="S37">
+        <v>2</v>
+      </c>
+      <c r="T37">
+        <v>3</v>
+      </c>
+      <c r="U37" s="3">
+        <v>0</v>
+      </c>
+      <c r="V37" s="3">
+        <v>0</v>
+      </c>
+      <c r="W37" s="1">
+        <v>14</v>
+      </c>
+      <c r="X37" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" t="s">
+        <v>20</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N38" t="s">
+        <v>11</v>
+      </c>
+      <c r="O38" t="s">
+        <v>11</v>
+      </c>
+      <c r="P38" t="s">
+        <v>22</v>
+      </c>
+      <c r="R38" t="s">
+        <v>11</v>
+      </c>
+      <c r="U38" s="1"/>
+      <c r="V38" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
refactoring other buttons editing to use fieldsets: expect_other_buttons for course
</commit_message>
<xml_diff>
--- a/spec/fixtures/Golf.xlsx
+++ b/spec/fixtures/Golf.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulkristoff/dev/golf/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07657EFB-4AFE-C14F-A72E-35994E9D01D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1122CEFA-05C9-3343-8F00-B6FD839E5B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15380" yWindow="1180" windowWidth="17600" windowHeight="17440" activeTab="3" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
+    <workbookView xWindow="7560" yWindow="1180" windowWidth="17600" windowHeight="17440" activeTab="2" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
   </bookViews>
   <sheets>
     <sheet name="Knight's play 1-9" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="25">
   <si>
     <t>Hole</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>LB</t>
+  </si>
+  <si>
+    <t>MM</t>
   </si>
 </sst>
 </file>
@@ -490,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{045CE2A8-F6DB-4143-9691-363739FD69FB}">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A34" sqref="A34:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1211,6 +1214,125 @@
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="8"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="6">
+        <v>44342</v>
+      </c>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="7">
+        <v>4</v>
+      </c>
+      <c r="C36" s="7">
+        <v>4</v>
+      </c>
+      <c r="D36" s="7">
+        <v>5</v>
+      </c>
+      <c r="E36" s="7">
+        <v>5</v>
+      </c>
+      <c r="F36" s="7">
+        <v>4</v>
+      </c>
+      <c r="G36" s="7">
+        <v>5</v>
+      </c>
+      <c r="H36" s="7">
+        <v>6</v>
+      </c>
+      <c r="I36" s="7">
+        <v>7</v>
+      </c>
+      <c r="J36" s="7">
+        <v>4</v>
+      </c>
+      <c r="K36" s="8">
+        <f>SUM(B36:J36)</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" s="7">
+        <v>2</v>
+      </c>
+      <c r="C37" s="7">
+        <v>2</v>
+      </c>
+      <c r="D37" s="7">
+        <v>2</v>
+      </c>
+      <c r="E37" s="7">
+        <v>2</v>
+      </c>
+      <c r="F37" s="7">
+        <v>2</v>
+      </c>
+      <c r="G37" s="7">
+        <v>2</v>
+      </c>
+      <c r="H37" s="7">
+        <v>3</v>
+      </c>
+      <c r="I37" s="7">
+        <v>3</v>
+      </c>
+      <c r="J37" s="7">
+        <v>2</v>
+      </c>
+      <c r="K37" s="8">
+        <f>SUM(B37:J37)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1989,8 +2111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9DD2039-084D-3C4E-B129-968266BAB55E}">
   <dimension ref="A1:V30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2232,31 +2354,119 @@
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
+      <c r="A10" s="6">
+        <v>44342</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="7">
+        <v>3</v>
+      </c>
+      <c r="C11" s="7">
+        <v>6</v>
+      </c>
+      <c r="D11" s="7">
+        <v>5</v>
+      </c>
+      <c r="E11" s="7">
+        <v>4</v>
+      </c>
+      <c r="F11" s="7">
+        <v>5</v>
+      </c>
+      <c r="G11" s="7">
+        <v>5</v>
+      </c>
+      <c r="H11" s="7">
+        <v>3</v>
+      </c>
+      <c r="I11" s="7">
+        <v>5</v>
+      </c>
+      <c r="J11" s="7">
+        <v>4</v>
+      </c>
+      <c r="K11" s="8">
+        <f>SUM(B11:J11)</f>
+        <v>40</v>
+      </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
+      <c r="A12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="7">
+        <v>1</v>
+      </c>
+      <c r="C12" s="7">
+        <v>2</v>
+      </c>
+      <c r="D12" s="7">
+        <v>3</v>
+      </c>
+      <c r="E12" s="7">
+        <v>2</v>
+      </c>
+      <c r="F12" s="7">
+        <v>2</v>
+      </c>
+      <c r="G12" s="7">
+        <v>3</v>
+      </c>
+      <c r="H12" s="7">
+        <v>1</v>
+      </c>
+      <c r="I12" s="7">
+        <v>2</v>
+      </c>
+      <c r="J12" s="7">
+        <v>1</v>
+      </c>
+      <c r="K12" s="8">
+        <f>SUM(B12:J12)</f>
+        <v>17</v>
+      </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
+      <c r="A13" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
@@ -2424,7 +2634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F45684-D9E4-2242-9821-C781990B9A28}">
   <dimension ref="A1:X38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+    <sheetView topLeftCell="M1" workbookViewId="0">
       <selection activeCell="X37" sqref="X37"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Clean up the showing of other_buttons
</commit_message>
<xml_diff>
--- a/spec/fixtures/Golf.xlsx
+++ b/spec/fixtures/Golf.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulkristoff/dev/golf/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A9DEF5A-D2DC-F241-95EC-DA79796345B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFB1DFF-0655-0249-A898-A31A2E2D982C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7560" yWindow="1180" windowWidth="17600" windowHeight="17440" activeTab="3" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
+    <workbookView xWindow="7560" yWindow="1180" windowWidth="17600" windowHeight="17440" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
   </bookViews>
   <sheets>
     <sheet name="Knight's play 1-9" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="30">
   <si>
     <t>Hole</t>
   </si>
@@ -540,15 +540,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{045CE2A8-F6DB-4143-9691-363739FD69FB}">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:XFD39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -565,905 +565,48 @@
         <v>27539</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>2</v>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="D2" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F2" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G2" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H2" s="1">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1">
+        <v>6</v>
+      </c>
+      <c r="J2" s="1">
         <v>7</v>
       </c>
-      <c r="I2" s="1">
+      <c r="K2" s="1">
         <v>8</v>
       </c>
-      <c r="J2" s="1">
+      <c r="L2" s="1">
         <v>9</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1">
-        <v>126</v>
-      </c>
-      <c r="C4" s="1">
-        <v>100</v>
-      </c>
-      <c r="D4" s="1">
-        <v>139</v>
-      </c>
-      <c r="E4" s="1">
-        <v>194</v>
-      </c>
-      <c r="F4" s="1">
-        <v>106</v>
-      </c>
-      <c r="G4" s="1">
-        <v>166</v>
-      </c>
-      <c r="H4" s="1">
-        <v>123</v>
-      </c>
-      <c r="I4" s="1">
-        <v>171</v>
-      </c>
-      <c r="J4" s="4">
-        <v>151</v>
-      </c>
-      <c r="K4" s="5">
-        <v>1276</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1">
-        <v>93</v>
-      </c>
-      <c r="C5" s="1">
-        <v>80</v>
-      </c>
-      <c r="D5" s="1">
-        <v>114</v>
-      </c>
-      <c r="E5" s="1">
-        <v>174</v>
-      </c>
-      <c r="F5" s="1">
-        <v>91</v>
-      </c>
-      <c r="G5" s="1">
-        <v>121</v>
-      </c>
-      <c r="H5" s="1">
-        <v>101</v>
-      </c>
-      <c r="I5" s="1">
-        <v>140</v>
-      </c>
-      <c r="J5" s="1">
-        <v>133</v>
-      </c>
-      <c r="K5" s="1">
-        <v>1047</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1">
-        <v>60</v>
-      </c>
-      <c r="C6" s="1">
-        <v>46</v>
-      </c>
-      <c r="D6" s="1">
-        <v>85</v>
-      </c>
-      <c r="E6" s="1">
-        <v>115</v>
-      </c>
-      <c r="F6" s="1">
-        <v>56</v>
-      </c>
-      <c r="G6" s="1">
-        <v>98</v>
-      </c>
-      <c r="H6" s="1">
-        <v>52</v>
-      </c>
-      <c r="I6" s="1">
-        <v>93</v>
-      </c>
-      <c r="J6" s="1">
-        <v>92</v>
-      </c>
-      <c r="K6" s="1">
-        <v>697</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1">
-        <v>3</v>
-      </c>
-      <c r="D7" s="1">
-        <v>3</v>
-      </c>
-      <c r="E7" s="1">
-        <v>3</v>
-      </c>
-      <c r="F7" s="1">
-        <v>3</v>
-      </c>
-      <c r="G7" s="1">
-        <v>3</v>
-      </c>
-      <c r="H7" s="1">
-        <v>3</v>
-      </c>
-      <c r="I7" s="1">
-        <v>3</v>
-      </c>
-      <c r="J7" s="1">
-        <v>3</v>
-      </c>
-      <c r="K7" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
-        <v>44067</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11">
-        <v>4</v>
-      </c>
-      <c r="C11">
-        <v>4</v>
-      </c>
-      <c r="D11">
-        <v>4</v>
-      </c>
-      <c r="E11">
-        <v>5</v>
-      </c>
-      <c r="F11">
-        <v>3</v>
-      </c>
-      <c r="G11">
-        <v>5</v>
-      </c>
-      <c r="H11">
-        <v>3</v>
-      </c>
-      <c r="I11">
-        <v>6</v>
-      </c>
-      <c r="J11">
-        <v>5</v>
-      </c>
-      <c r="K11" s="1">
-        <f>SUM(B11:J11)</f>
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-      <c r="E12">
-        <v>2</v>
-      </c>
-      <c r="F12">
-        <v>2</v>
-      </c>
-      <c r="G12">
-        <v>2</v>
-      </c>
-      <c r="H12">
-        <v>2</v>
-      </c>
-      <c r="I12">
-        <v>2</v>
-      </c>
-      <c r="J12">
-        <v>2</v>
-      </c>
-      <c r="K12" s="1">
-        <f>SUM(B12:J12)</f>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" t="s">
-        <v>10</v>
-      </c>
-      <c r="I13" t="s">
-        <v>10</v>
-      </c>
-      <c r="K13" s="1"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="K14" s="1"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <v>44074</v>
-      </c>
-      <c r="K15" s="1"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16">
-        <v>3</v>
-      </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
-      <c r="D16">
-        <v>4</v>
-      </c>
-      <c r="E16">
-        <v>5</v>
-      </c>
-      <c r="F16">
-        <v>3</v>
-      </c>
-      <c r="G16">
-        <v>2</v>
-      </c>
-      <c r="H16">
-        <v>4</v>
-      </c>
-      <c r="I16">
-        <v>3</v>
-      </c>
-      <c r="J16">
-        <v>7</v>
-      </c>
-      <c r="K16" s="1">
-        <f>SUM(B16:J16)</f>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="D17">
-        <v>2</v>
-      </c>
-      <c r="E17">
-        <v>3</v>
-      </c>
-      <c r="F17">
-        <v>2</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17">
-        <v>3</v>
-      </c>
-      <c r="I17">
-        <v>2</v>
-      </c>
-      <c r="J17">
-        <v>2</v>
-      </c>
-      <c r="K17" s="1">
-        <f>SUM(B17:J17)</f>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" t="s">
-        <v>9</v>
-      </c>
-      <c r="K18" s="1"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="K19" s="1"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="6">
-        <v>44081</v>
-      </c>
-      <c r="K20" s="1"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="7">
-        <v>5</v>
-      </c>
-      <c r="C21" s="7">
-        <v>3</v>
-      </c>
-      <c r="D21" s="7">
-        <v>4</v>
-      </c>
-      <c r="E21" s="7">
-        <v>5</v>
-      </c>
-      <c r="F21" s="7">
-        <v>4</v>
-      </c>
-      <c r="G21" s="7">
-        <v>4</v>
-      </c>
-      <c r="H21" s="7">
-        <v>4</v>
-      </c>
-      <c r="I21" s="7">
-        <v>4</v>
-      </c>
-      <c r="J21" s="7">
-        <v>4</v>
-      </c>
-      <c r="K21" s="8">
-        <f>SUM(B21:J21)</f>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="7">
-        <v>2</v>
-      </c>
-      <c r="C22" s="7">
-        <v>2</v>
-      </c>
-      <c r="D22" s="7">
-        <v>2</v>
-      </c>
-      <c r="E22" s="7">
-        <v>3</v>
-      </c>
-      <c r="F22" s="7">
-        <v>2</v>
-      </c>
-      <c r="G22" s="7">
-        <v>2</v>
-      </c>
-      <c r="H22" s="7">
-        <v>3</v>
-      </c>
-      <c r="I22" s="7">
-        <v>1</v>
-      </c>
-      <c r="J22" s="7">
-        <v>1</v>
-      </c>
-      <c r="K22" s="8">
-        <f>SUM(B22:J22)</f>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="6">
-        <v>44090</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B26" s="7">
-        <v>4</v>
-      </c>
-      <c r="C26" s="7">
-        <v>4</v>
-      </c>
-      <c r="D26" s="7">
-        <v>3</v>
-      </c>
-      <c r="E26" s="7">
-        <v>4</v>
-      </c>
-      <c r="F26" s="7">
-        <v>3</v>
-      </c>
-      <c r="G26" s="7">
-        <v>4</v>
-      </c>
-      <c r="H26" s="7">
-        <v>4</v>
-      </c>
-      <c r="I26" s="7">
-        <v>4</v>
-      </c>
-      <c r="J26" s="7">
-        <v>4</v>
-      </c>
-      <c r="K26" s="8">
-        <f>SUM(B26:J26)</f>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27" s="7">
-        <v>3</v>
-      </c>
-      <c r="C27" s="7">
-        <v>2</v>
-      </c>
-      <c r="D27" s="7">
-        <v>1</v>
-      </c>
-      <c r="E27" s="7">
-        <v>2</v>
-      </c>
-      <c r="F27" s="7">
-        <v>2</v>
-      </c>
-      <c r="G27" s="7">
-        <v>3</v>
-      </c>
-      <c r="H27" s="7">
-        <v>3</v>
-      </c>
-      <c r="I27" s="7">
-        <v>2</v>
-      </c>
-      <c r="J27" s="7">
-        <v>3</v>
-      </c>
-      <c r="K27" s="8">
-        <f>SUM(B27:J27)</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="K28" s="7"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="8"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="6">
-        <v>44102</v>
-      </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B31" s="7">
-        <v>4</v>
-      </c>
-      <c r="C31" s="7">
-        <v>3</v>
-      </c>
-      <c r="D31" s="7">
-        <v>4</v>
-      </c>
-      <c r="E31" s="7">
-        <v>5</v>
-      </c>
-      <c r="F31" s="7">
-        <v>3</v>
-      </c>
-      <c r="G31" s="7">
-        <v>3</v>
-      </c>
-      <c r="H31" s="7">
-        <v>3</v>
-      </c>
-      <c r="I31" s="7">
-        <v>5</v>
-      </c>
-      <c r="J31" s="7">
-        <v>4</v>
-      </c>
-      <c r="K31" s="8">
-        <f>SUM(B31:J31)</f>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B32" s="7">
-        <v>2</v>
-      </c>
-      <c r="C32" s="7">
-        <v>1</v>
-      </c>
-      <c r="D32" s="7">
-        <v>2</v>
-      </c>
-      <c r="E32" s="7">
-        <v>2</v>
-      </c>
-      <c r="F32" s="7">
-        <v>2</v>
-      </c>
-      <c r="G32" s="7">
-        <v>1</v>
-      </c>
-      <c r="H32" s="7">
-        <v>2</v>
-      </c>
-      <c r="I32" s="7">
-        <v>2</v>
-      </c>
-      <c r="J32" s="7">
-        <v>2</v>
-      </c>
-      <c r="K32" s="8">
-        <f>SUM(B32:J32)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A33" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A34" s="8"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="7"/>
-      <c r="K34" s="7"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A35" s="6">
-        <v>44342</v>
-      </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="7"/>
-      <c r="J35" s="7"/>
-      <c r="K35" s="7"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B36" s="7">
-        <v>4</v>
-      </c>
-      <c r="C36" s="7">
-        <v>4</v>
-      </c>
-      <c r="D36" s="7">
-        <v>5</v>
-      </c>
-      <c r="E36" s="7">
-        <v>5</v>
-      </c>
-      <c r="F36" s="7">
-        <v>4</v>
-      </c>
-      <c r="G36" s="7">
-        <v>5</v>
-      </c>
-      <c r="H36" s="7">
-        <v>6</v>
-      </c>
-      <c r="I36" s="7">
-        <v>7</v>
-      </c>
-      <c r="J36" s="7">
-        <v>4</v>
-      </c>
-      <c r="K36" s="8">
-        <f>SUM(B36:J36)</f>
-        <v>44</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A37" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B37" s="7">
-        <v>2</v>
-      </c>
-      <c r="C37" s="7">
-        <v>2</v>
-      </c>
-      <c r="D37" s="7">
-        <v>2</v>
-      </c>
-      <c r="E37" s="7">
-        <v>2</v>
-      </c>
-      <c r="F37" s="7">
-        <v>2</v>
-      </c>
-      <c r="G37" s="7">
-        <v>2</v>
-      </c>
-      <c r="H37" s="7">
-        <v>3</v>
-      </c>
-      <c r="I37" s="7">
-        <v>3</v>
-      </c>
-      <c r="J37" s="7">
-        <v>2</v>
-      </c>
-      <c r="K37" s="8">
-        <f>SUM(B37:J37)</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A38" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <ignoredErrors>
-    <ignoredError sqref="K11 K16 K21:K22" formulaRange="1"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8526A8B9-0C97-E94E-BA2A-E4D31B8BA027}">
-  <dimension ref="A1:V35"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:XFD39"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1">
-        <v>27539</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1">
-        <v>6</v>
-      </c>
-      <c r="H2" s="1">
-        <v>7</v>
-      </c>
-      <c r="I2" s="1">
-        <v>8</v>
-      </c>
-      <c r="J2" s="1">
-        <v>9</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="M2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1477,134 +620,136 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>134</v>
+        <v>71.599999999999994</v>
       </c>
       <c r="C4" s="1">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="D4" s="1">
-        <v>213</v>
+        <v>126</v>
       </c>
       <c r="E4" s="1">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F4" s="1">
-        <v>112</v>
+        <v>139</v>
       </c>
       <c r="G4" s="1">
-        <v>105</v>
+        <v>194</v>
       </c>
       <c r="H4" s="1">
-        <v>194</v>
+        <v>106</v>
       </c>
       <c r="I4" s="1">
+        <v>166</v>
+      </c>
+      <c r="J4" s="1">
+        <v>123</v>
+      </c>
+      <c r="K4" s="1">
+        <v>171</v>
+      </c>
+      <c r="L4" s="4">
+        <v>151</v>
+      </c>
+      <c r="M4" s="5">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>54</v>
+      </c>
+      <c r="C5" s="1">
+        <v>126</v>
+      </c>
+      <c r="D5" s="1">
+        <v>93</v>
+      </c>
+      <c r="E5" s="1">
+        <v>80</v>
+      </c>
+      <c r="F5" s="1">
+        <v>114</v>
+      </c>
+      <c r="G5" s="1">
+        <v>174</v>
+      </c>
+      <c r="H5" s="1">
+        <v>91</v>
+      </c>
+      <c r="I5" s="1">
+        <v>121</v>
+      </c>
+      <c r="J5" s="1">
+        <v>101</v>
+      </c>
+      <c r="K5" s="1">
         <v>140</v>
       </c>
-      <c r="J4" s="1">
-        <v>165</v>
-      </c>
-      <c r="K4" s="1">
-        <v>1325</v>
-      </c>
-      <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1">
-        <v>104</v>
-      </c>
-      <c r="C5" s="1">
-        <v>138</v>
-      </c>
-      <c r="D5" s="1">
-        <v>169</v>
-      </c>
-      <c r="E5" s="1">
-        <v>84</v>
-      </c>
-      <c r="F5" s="1">
-        <v>88</v>
-      </c>
-      <c r="G5" s="1">
-        <v>87</v>
-      </c>
-      <c r="H5" s="1">
-        <v>164</v>
-      </c>
-      <c r="I5" s="1">
-        <v>107</v>
-      </c>
-      <c r="J5" s="1">
-        <v>136</v>
-      </c>
-      <c r="K5" s="1">
-        <v>1077</v>
-      </c>
-      <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="L5" s="1">
+        <v>133</v>
+      </c>
+      <c r="M5" s="1">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="1">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1">
+        <v>113</v>
+      </c>
+      <c r="D6" s="1">
+        <v>60</v>
+      </c>
+      <c r="E6" s="1">
+        <v>46</v>
+      </c>
+      <c r="F6" s="1">
         <v>85</v>
       </c>
-      <c r="D6" s="1">
-        <v>110</v>
-      </c>
-      <c r="E6" s="1">
-        <v>64</v>
-      </c>
-      <c r="F6" s="1">
-        <v>72</v>
-      </c>
       <c r="G6" s="1">
-        <v>71</v>
+        <v>115</v>
       </c>
       <c r="H6" s="1">
-        <v>99</v>
+        <v>56</v>
       </c>
       <c r="I6" s="1">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="J6" s="1">
-        <v>90</v>
+        <v>52</v>
       </c>
       <c r="K6" s="1">
-        <v>746</v>
-      </c>
-      <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+      <c r="L6" s="1">
+        <v>92</v>
+      </c>
+      <c r="M6" s="1">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1">
-        <v>3</v>
-      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
       <c r="D7" s="1">
         <v>3</v>
       </c>
@@ -1627,35 +772,69 @@
         <v>3</v>
       </c>
       <c r="K7" s="1">
+        <v>3</v>
+      </c>
+      <c r="L7" s="1">
+        <v>3</v>
+      </c>
+      <c r="M7" s="1">
         <v>27</v>
       </c>
-      <c r="L7" s="1"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1">
+        <v>4</v>
+      </c>
+      <c r="H8" s="1">
+        <v>5</v>
+      </c>
+      <c r="I8" s="1">
+        <v>6</v>
+      </c>
+      <c r="J8" s="1">
+        <v>7</v>
+      </c>
+      <c r="K8" s="1">
+        <v>8</v>
+      </c>
+      <c r="L8" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>44067</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B11">
-        <v>4</v>
-      </c>
-      <c r="C11">
-        <v>6</v>
-      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
       <c r="D11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E11">
         <v>4</v>
@@ -1664,35 +843,36 @@
         <v>4</v>
       </c>
       <c r="G11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H11">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I11">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J11">
-        <v>5</v>
-      </c>
-      <c r="K11" s="1">
-        <f>SUM(B11:J11)</f>
-        <v>44</v>
-      </c>
-      <c r="L11" s="1"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="K11">
+        <v>6</v>
+      </c>
+      <c r="L11">
+        <v>5</v>
+      </c>
+      <c r="M11" s="1">
+        <f>SUM(D11:L11)</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
       <c r="D12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -1704,91 +884,102 @@
         <v>2</v>
       </c>
       <c r="H12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J12">
         <v>2</v>
       </c>
-      <c r="K12" s="1">
-        <f>SUM(B12:J12)</f>
-        <v>20</v>
-      </c>
-      <c r="L12" s="1"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="K12">
+        <v>2</v>
+      </c>
+      <c r="L12">
+        <v>2</v>
+      </c>
+      <c r="M12" s="1">
+        <f>SUM(D12:L12)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" t="s">
+        <v>10</v>
+      </c>
+      <c r="K13" t="s">
+        <v>10</v>
+      </c>
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>44074</v>
       </c>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="M15" s="1"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B16">
-        <v>6</v>
-      </c>
-      <c r="C16">
-        <v>4</v>
-      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
       <c r="D16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H16">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J16">
-        <v>5</v>
-      </c>
-      <c r="K16" s="1">
-        <f>SUM(B16:J16)</f>
-        <v>39</v>
-      </c>
-      <c r="L16" s="1"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="K16">
+        <v>3</v>
+      </c>
+      <c r="L16">
+        <v>7</v>
+      </c>
+      <c r="M16" s="1">
+        <f>SUM(D16:L16)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B17">
-        <v>3</v>
-      </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
       <c r="D17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E17">
         <v>2</v>
@@ -1797,66 +988,70 @@
         <v>2</v>
       </c>
       <c r="G17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J17">
-        <v>2</v>
-      </c>
-      <c r="K17" s="1">
-        <f>SUM(B17:J17)</f>
-        <v>21</v>
-      </c>
-      <c r="L17" s="1"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="K17">
+        <v>2</v>
+      </c>
+      <c r="L17">
+        <v>2</v>
+      </c>
+      <c r="M17" s="1">
+        <f>SUM(D17:L17)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C18" t="s">
-        <v>11</v>
-      </c>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" t="s">
+        <v>9</v>
+      </c>
+      <c r="M18" s="1"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>44081</v>
       </c>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="M20" s="1"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="7">
-        <v>5</v>
-      </c>
-      <c r="C21" s="7">
-        <v>3</v>
-      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E21" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F21" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G21" s="7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H21" s="7">
         <v>4</v>
@@ -1867,24 +1062,25 @@
       <c r="J21" s="7">
         <v>4</v>
       </c>
-      <c r="K21" s="8">
-        <f>SUM(B21:J21)</f>
-        <v>33</v>
-      </c>
-      <c r="L21" s="8"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K21" s="7">
+        <v>4</v>
+      </c>
+      <c r="L21" s="7">
+        <v>4</v>
+      </c>
+      <c r="M21" s="8">
+        <f>SUM(D21:L21)</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="7">
-        <v>3</v>
-      </c>
-      <c r="C22" s="7">
-        <v>2</v>
-      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
       <c r="D22" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E22" s="7">
         <v>2</v>
@@ -1893,93 +1089,98 @@
         <v>2</v>
       </c>
       <c r="G22" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H22" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I22" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J22" s="7">
-        <v>2</v>
-      </c>
-      <c r="K22" s="8">
-        <f>SUM(B22:J22)</f>
-        <v>21</v>
-      </c>
-      <c r="L22" s="8"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="K22" s="7">
+        <v>1</v>
+      </c>
+      <c r="L22" s="7">
+        <v>1</v>
+      </c>
+      <c r="M22" s="8">
+        <f>SUM(D22:L22)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7" t="s">
-        <v>11</v>
-      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
+      <c r="G23" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
       <c r="L23" s="7"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M23" s="7"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>44090</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="7">
-        <v>4</v>
-      </c>
-      <c r="C26" s="7">
-        <v>4</v>
-      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
       <c r="D26" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E26" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F26" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G26" s="7">
         <v>4</v>
       </c>
       <c r="H26" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I26" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J26" s="7">
-        <v>6</v>
-      </c>
-      <c r="K26" s="8">
-        <f>SUM(B26:J26)</f>
-        <v>37</v>
-      </c>
-      <c r="L26" s="8"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="K26" s="7">
+        <v>4</v>
+      </c>
+      <c r="L26" s="7">
+        <v>4</v>
+      </c>
+      <c r="M26" s="8">
+        <f>SUM(D26:L26)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="7">
-        <v>2</v>
-      </c>
-      <c r="C27" s="7">
-        <v>2</v>
-      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
       <c r="D27" s="7">
         <v>3</v>
       </c>
@@ -1987,7 +1188,7 @@
         <v>2</v>
       </c>
       <c r="F27" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G27" s="7">
         <v>2</v>
@@ -1996,39 +1197,49 @@
         <v>2</v>
       </c>
       <c r="I27" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J27" s="7">
         <v>3</v>
       </c>
-      <c r="K27" s="8">
-        <f>SUM(B27:J27)</f>
-        <v>20</v>
-      </c>
-      <c r="L27" s="8"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K27" s="7">
+        <v>2</v>
+      </c>
+      <c r="L27" s="7">
+        <v>3</v>
+      </c>
+      <c r="M27" s="8">
+        <f>SUM(D27:L27)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
+      <c r="G28" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
-      <c r="J28" s="7" t="s">
-        <v>11</v>
-      </c>
+      <c r="J28" s="7"/>
       <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L28" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M28" s="7"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="8"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
@@ -2038,13 +1249,14 @@
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
       <c r="L29" s="7"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M29" s="7"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>44102</v>
       </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
@@ -2054,22 +1266,19 @@
       <c r="J30" s="7"/>
       <c r="K30" s="7"/>
       <c r="L30" s="7"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M30" s="7"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="7">
-        <v>4</v>
-      </c>
-      <c r="C31" s="7">
-        <v>3</v>
-      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
       <c r="D31" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E31" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F31" s="7">
         <v>4</v>
@@ -2078,64 +1287,72 @@
         <v>5</v>
       </c>
       <c r="H31" s="7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I31" s="7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J31" s="7">
-        <v>4</v>
-      </c>
-      <c r="K31" s="8">
-        <f>SUM(B31:J31)</f>
-        <v>39</v>
-      </c>
-      <c r="L31" s="8"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="K31" s="7">
+        <v>5</v>
+      </c>
+      <c r="L31" s="7">
+        <v>4</v>
+      </c>
+      <c r="M31" s="8">
+        <f>SUM(D31:L31)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="7">
-        <v>2</v>
-      </c>
-      <c r="C32" s="7">
-        <v>2</v>
-      </c>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
       <c r="D32" s="7">
         <v>2</v>
       </c>
       <c r="E32" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32" s="7">
         <v>2</v>
       </c>
       <c r="G32" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H32" s="7">
         <v>2</v>
       </c>
       <c r="I32" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J32" s="7">
         <v>2</v>
       </c>
-      <c r="K32" s="8">
-        <f>SUM(B32:J32)</f>
-        <v>20</v>
-      </c>
-      <c r="L32" s="8"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K32" s="7">
+        <v>2</v>
+      </c>
+      <c r="L32" s="7">
+        <v>2</v>
+      </c>
+      <c r="M32" s="8">
+        <f>SUM(D32:L32)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
@@ -2144,27 +1361,383 @@
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="1"/>
+      <c r="M33" s="7"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" s="6">
+        <v>44267</v>
+      </c>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="7">
+        <v>4</v>
+      </c>
+      <c r="E36" s="7">
+        <v>5</v>
+      </c>
+      <c r="F36" s="7">
+        <v>3</v>
+      </c>
+      <c r="G36" s="7">
+        <v>4</v>
+      </c>
+      <c r="H36" s="7">
+        <v>4</v>
+      </c>
+      <c r="I36" s="7">
+        <v>4</v>
+      </c>
+      <c r="J36" s="7">
+        <v>7</v>
+      </c>
+      <c r="K36" s="7">
+        <v>6</v>
+      </c>
+      <c r="L36" s="7">
+        <v>6</v>
+      </c>
+      <c r="M36" s="8">
+        <f>SUM(D36:L36)</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="7">
+        <v>2</v>
+      </c>
+      <c r="E37" s="7">
+        <v>2</v>
+      </c>
+      <c r="F37" s="7">
+        <v>1</v>
+      </c>
+      <c r="G37" s="7">
+        <v>1</v>
+      </c>
+      <c r="H37" s="7">
+        <v>2</v>
+      </c>
+      <c r="I37" s="7">
+        <v>2</v>
+      </c>
+      <c r="J37" s="7">
+        <v>2</v>
+      </c>
+      <c r="K37" s="7">
+        <v>2</v>
+      </c>
+      <c r="L37" s="7">
+        <v>2</v>
+      </c>
+      <c r="M37" s="8">
+        <f>SUM(D37:L37)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40" s="6">
+        <v>44279</v>
+      </c>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="7">
+        <v>4</v>
+      </c>
+      <c r="E41" s="7">
+        <v>3</v>
+      </c>
+      <c r="F41" s="7">
+        <v>4</v>
+      </c>
+      <c r="G41" s="7">
+        <v>4</v>
+      </c>
+      <c r="H41" s="7">
+        <v>4</v>
+      </c>
+      <c r="I41" s="7">
+        <v>5</v>
+      </c>
+      <c r="J41" s="7">
+        <v>4</v>
+      </c>
+      <c r="K41" s="7">
+        <v>5</v>
+      </c>
+      <c r="L41" s="7">
+        <v>5</v>
+      </c>
+      <c r="M41" s="8">
+        <f>SUM(D41:L41)</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A42" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="7">
+        <v>2</v>
+      </c>
+      <c r="E42" s="7">
+        <v>2</v>
+      </c>
+      <c r="F42" s="7">
+        <v>2</v>
+      </c>
+      <c r="G42" s="7">
+        <v>2</v>
+      </c>
+      <c r="H42" s="7">
+        <v>2</v>
+      </c>
+      <c r="I42" s="7">
+        <v>2</v>
+      </c>
+      <c r="J42" s="7">
+        <v>3</v>
+      </c>
+      <c r="K42" s="7">
+        <v>1</v>
+      </c>
+      <c r="L42" s="7">
+        <v>3</v>
+      </c>
+      <c r="M42" s="8">
+        <f>SUM(D42:L42)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A43" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K43" s="7"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="7"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A45" s="6">
+        <v>44342</v>
+      </c>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="7"/>
+      <c r="M45" s="7"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="7">
+        <v>4</v>
+      </c>
+      <c r="E46" s="7">
+        <v>4</v>
+      </c>
+      <c r="F46" s="7">
+        <v>5</v>
+      </c>
+      <c r="G46" s="7">
+        <v>5</v>
+      </c>
+      <c r="H46" s="7">
+        <v>4</v>
+      </c>
+      <c r="I46" s="7">
+        <v>5</v>
+      </c>
+      <c r="J46" s="7">
+        <v>6</v>
+      </c>
+      <c r="K46" s="7">
+        <v>7</v>
+      </c>
+      <c r="L46" s="7">
+        <v>4</v>
+      </c>
+      <c r="M46" s="8">
+        <f>SUM(D46:L46)</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A47" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="7">
+        <v>2</v>
+      </c>
+      <c r="E47" s="7">
+        <v>2</v>
+      </c>
+      <c r="F47" s="7">
+        <v>2</v>
+      </c>
+      <c r="G47" s="7">
+        <v>2</v>
+      </c>
+      <c r="H47" s="7">
+        <v>2</v>
+      </c>
+      <c r="I47" s="7">
+        <v>2</v>
+      </c>
+      <c r="J47" s="7">
+        <v>3</v>
+      </c>
+      <c r="K47" s="7">
+        <v>3</v>
+      </c>
+      <c r="L47" s="7">
+        <v>2</v>
+      </c>
+      <c r="M47" s="8">
+        <f>SUM(D47:L47)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A48" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H48" s="7"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K48" s="7"/>
+      <c r="L48" s="7"/>
+      <c r="M48" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <ignoredErrors>
+    <ignoredError sqref="M11 M16 M21:M22" formulaRange="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9DD2039-084D-3C4E-B129-968266BAB55E}">
-  <dimension ref="A1:V30"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8526A8B9-0C97-E94E-BA2A-E4D31B8BA027}">
+  <dimension ref="A1:X48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -2181,42 +1754,46 @@
         <v>27539</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>2</v>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="D2" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F2" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G2" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H2" s="1">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1">
+        <v>6</v>
+      </c>
+      <c r="J2" s="1">
         <v>7</v>
       </c>
-      <c r="I2" s="1">
+      <c r="K2" s="1">
         <v>8</v>
       </c>
-      <c r="J2" s="1">
+      <c r="L2" s="1">
         <v>9</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -2226,557 +1803,8 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1">
-        <v>125</v>
-      </c>
-      <c r="C4" s="1">
-        <v>150</v>
-      </c>
-      <c r="D4" s="1">
-        <v>118</v>
-      </c>
-      <c r="E4" s="1">
-        <v>117</v>
-      </c>
-      <c r="F4" s="1">
-        <v>134</v>
-      </c>
-      <c r="G4" s="1">
-        <v>174</v>
-      </c>
-      <c r="H4" s="1">
-        <v>136</v>
-      </c>
-      <c r="I4" s="1">
-        <v>100</v>
-      </c>
-      <c r="J4" s="1">
-        <v>155</v>
-      </c>
-      <c r="K4" s="1">
-        <v>1209</v>
-      </c>
-      <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1">
-        <v>105</v>
-      </c>
-      <c r="C5" s="1">
-        <v>132</v>
-      </c>
-      <c r="D5" s="1">
-        <v>105</v>
-      </c>
-      <c r="E5" s="1">
-        <v>102</v>
-      </c>
-      <c r="F5" s="1">
-        <v>105</v>
-      </c>
-      <c r="G5" s="1">
-        <v>159</v>
-      </c>
-      <c r="H5" s="1">
-        <v>112</v>
-      </c>
-      <c r="I5" s="1">
-        <v>90</v>
-      </c>
-      <c r="J5" s="1">
-        <v>130</v>
-      </c>
-      <c r="K5" s="1">
-        <v>1040</v>
-      </c>
-      <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1">
-        <v>77</v>
-      </c>
-      <c r="C6" s="1">
-        <v>117</v>
-      </c>
-      <c r="D6" s="1">
-        <v>90</v>
-      </c>
-      <c r="E6" s="1">
-        <v>92</v>
-      </c>
-      <c r="F6" s="1">
-        <v>77</v>
-      </c>
-      <c r="G6" s="1">
-        <v>93</v>
-      </c>
-      <c r="H6" s="1">
-        <v>85</v>
-      </c>
-      <c r="I6" s="1">
-        <v>78</v>
-      </c>
-      <c r="J6" s="1">
-        <v>110</v>
-      </c>
-      <c r="K6" s="1">
-        <v>819</v>
-      </c>
-      <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1">
-        <v>3</v>
-      </c>
-      <c r="D7" s="1">
-        <v>3</v>
-      </c>
-      <c r="E7" s="1">
-        <v>3</v>
-      </c>
-      <c r="F7" s="1">
-        <v>3</v>
-      </c>
-      <c r="G7" s="1">
-        <v>3</v>
-      </c>
-      <c r="H7" s="1">
-        <v>3</v>
-      </c>
-      <c r="I7" s="1">
-        <v>3</v>
-      </c>
-      <c r="J7" s="1">
-        <v>3</v>
-      </c>
-      <c r="K7" s="1">
-        <v>27</v>
-      </c>
-      <c r="L7" s="1"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
-        <v>44342</v>
-      </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="7">
-        <v>3</v>
-      </c>
-      <c r="C11" s="7">
-        <v>6</v>
-      </c>
-      <c r="D11" s="7">
-        <v>5</v>
-      </c>
-      <c r="E11" s="7">
-        <v>4</v>
-      </c>
-      <c r="F11" s="7">
-        <v>5</v>
-      </c>
-      <c r="G11" s="7">
-        <v>5</v>
-      </c>
-      <c r="H11" s="7">
-        <v>3</v>
-      </c>
-      <c r="I11" s="7">
-        <v>5</v>
-      </c>
-      <c r="J11" s="7">
-        <v>4</v>
-      </c>
-      <c r="K11" s="8">
-        <f>SUM(B11:J11)</f>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="7">
-        <v>1</v>
-      </c>
-      <c r="C12" s="7">
-        <v>2</v>
-      </c>
-      <c r="D12" s="7">
-        <v>3</v>
-      </c>
-      <c r="E12" s="7">
-        <v>2</v>
-      </c>
-      <c r="F12" s="7">
-        <v>2</v>
-      </c>
-      <c r="G12" s="7">
-        <v>3</v>
-      </c>
-      <c r="H12" s="7">
-        <v>1</v>
-      </c>
-      <c r="I12" s="7">
-        <v>2</v>
-      </c>
-      <c r="J12" s="7">
-        <v>1</v>
-      </c>
-      <c r="K12" s="8">
-        <f>SUM(B12:J12)</f>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="8"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="8"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="6"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="8"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="8"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="8"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="6"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="8"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="8"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F45684-D9E4-2242-9821-C781990B9A28}">
-  <dimension ref="A1:X43"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L10" workbookViewId="0">
-      <selection activeCell="U43" sqref="U43"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1">
-        <v>27511</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1">
-        <v>2</v>
-      </c>
-      <c r="F2" s="1">
-        <v>3</v>
-      </c>
-      <c r="G2" s="1">
-        <v>4</v>
-      </c>
-      <c r="H2" s="1">
-        <v>5</v>
-      </c>
-      <c r="I2" s="1">
-        <v>6</v>
-      </c>
-      <c r="J2" s="1">
-        <v>7</v>
-      </c>
-      <c r="K2" s="1">
-        <v>8</v>
-      </c>
-      <c r="L2" s="1">
-        <v>9</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N2" s="1">
-        <v>10</v>
-      </c>
-      <c r="O2" s="1">
-        <v>11</v>
-      </c>
-      <c r="P2" s="1">
-        <v>12</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>13</v>
-      </c>
-      <c r="R2" s="1">
-        <v>14</v>
-      </c>
-      <c r="S2" s="1">
-        <v>15</v>
-      </c>
-      <c r="T2" s="1">
-        <v>16</v>
-      </c>
-      <c r="U2" s="1">
-        <v>17</v>
-      </c>
-      <c r="V2" s="1">
-        <v>18</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
@@ -2815,6 +1843,1797 @@
         <v>139</v>
       </c>
       <c r="D4" s="1">
+        <v>134</v>
+      </c>
+      <c r="E4" s="1">
+        <v>160</v>
+      </c>
+      <c r="F4" s="1">
+        <v>213</v>
+      </c>
+      <c r="G4" s="1">
+        <v>102</v>
+      </c>
+      <c r="H4" s="1">
+        <v>112</v>
+      </c>
+      <c r="I4" s="1">
+        <v>105</v>
+      </c>
+      <c r="J4" s="1">
+        <v>194</v>
+      </c>
+      <c r="K4" s="1">
+        <v>140</v>
+      </c>
+      <c r="L4" s="1">
+        <v>165</v>
+      </c>
+      <c r="M4" s="1">
+        <v>1325</v>
+      </c>
+      <c r="N4" s="1"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>54</v>
+      </c>
+      <c r="C5" s="1">
+        <v>126</v>
+      </c>
+      <c r="D5" s="1">
+        <v>104</v>
+      </c>
+      <c r="E5" s="1">
+        <v>138</v>
+      </c>
+      <c r="F5" s="1">
+        <v>169</v>
+      </c>
+      <c r="G5" s="1">
+        <v>84</v>
+      </c>
+      <c r="H5" s="1">
+        <v>88</v>
+      </c>
+      <c r="I5" s="1">
+        <v>87</v>
+      </c>
+      <c r="J5" s="1">
+        <v>164</v>
+      </c>
+      <c r="K5" s="1">
+        <v>107</v>
+      </c>
+      <c r="L5" s="1">
+        <v>136</v>
+      </c>
+      <c r="M5" s="1">
+        <v>1077</v>
+      </c>
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1">
+        <v>113</v>
+      </c>
+      <c r="D6" s="1">
+        <v>77</v>
+      </c>
+      <c r="E6" s="1">
+        <v>85</v>
+      </c>
+      <c r="F6" s="1">
+        <v>110</v>
+      </c>
+      <c r="G6" s="1">
+        <v>64</v>
+      </c>
+      <c r="H6" s="1">
+        <v>72</v>
+      </c>
+      <c r="I6" s="1">
+        <v>71</v>
+      </c>
+      <c r="J6" s="1">
+        <v>99</v>
+      </c>
+      <c r="K6" s="1">
+        <v>78</v>
+      </c>
+      <c r="L6" s="1">
+        <v>90</v>
+      </c>
+      <c r="M6" s="1">
+        <v>746</v>
+      </c>
+      <c r="N6" s="1"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1">
+        <v>3</v>
+      </c>
+      <c r="F7" s="1">
+        <v>3</v>
+      </c>
+      <c r="G7" s="1">
+        <v>3</v>
+      </c>
+      <c r="H7" s="1">
+        <v>3</v>
+      </c>
+      <c r="I7" s="1">
+        <v>3</v>
+      </c>
+      <c r="J7" s="1">
+        <v>3</v>
+      </c>
+      <c r="K7" s="1">
+        <v>3</v>
+      </c>
+      <c r="L7" s="1">
+        <v>3</v>
+      </c>
+      <c r="M7" s="1">
+        <v>27</v>
+      </c>
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1">
+        <v>4</v>
+      </c>
+      <c r="H8" s="1">
+        <v>5</v>
+      </c>
+      <c r="I8" s="1">
+        <v>6</v>
+      </c>
+      <c r="J8" s="1">
+        <v>7</v>
+      </c>
+      <c r="K8" s="1">
+        <v>8</v>
+      </c>
+      <c r="L8" s="1">
+        <v>9</v>
+      </c>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>44067</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>4</v>
+      </c>
+      <c r="J11">
+        <v>6</v>
+      </c>
+      <c r="K11">
+        <v>6</v>
+      </c>
+      <c r="L11">
+        <v>5</v>
+      </c>
+      <c r="M11" s="1">
+        <f>SUM(D11:L11)</f>
+        <v>44</v>
+      </c>
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+      <c r="J12">
+        <v>3</v>
+      </c>
+      <c r="K12">
+        <v>3</v>
+      </c>
+      <c r="L12">
+        <v>2</v>
+      </c>
+      <c r="M12" s="1">
+        <f>SUM(D12:L12)</f>
+        <v>20</v>
+      </c>
+      <c r="N12" s="1"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>44074</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16">
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="F16">
+        <v>4</v>
+      </c>
+      <c r="G16">
+        <v>4</v>
+      </c>
+      <c r="H16">
+        <v>3</v>
+      </c>
+      <c r="I16">
+        <v>4</v>
+      </c>
+      <c r="J16">
+        <v>5</v>
+      </c>
+      <c r="K16">
+        <v>4</v>
+      </c>
+      <c r="L16">
+        <v>5</v>
+      </c>
+      <c r="M16" s="1">
+        <f>SUM(D16:L16)</f>
+        <v>39</v>
+      </c>
+      <c r="N16" s="1"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>3</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="I17">
+        <v>2</v>
+      </c>
+      <c r="J17">
+        <v>3</v>
+      </c>
+      <c r="K17">
+        <v>2</v>
+      </c>
+      <c r="L17">
+        <v>2</v>
+      </c>
+      <c r="M17" s="1">
+        <f>SUM(D17:L17)</f>
+        <v>21</v>
+      </c>
+      <c r="N17" s="1"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="6">
+        <v>44081</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="7">
+        <v>5</v>
+      </c>
+      <c r="E21" s="7">
+        <v>3</v>
+      </c>
+      <c r="F21" s="7">
+        <v>4</v>
+      </c>
+      <c r="G21" s="7">
+        <v>4</v>
+      </c>
+      <c r="H21" s="7">
+        <v>3</v>
+      </c>
+      <c r="I21" s="7">
+        <v>2</v>
+      </c>
+      <c r="J21" s="7">
+        <v>4</v>
+      </c>
+      <c r="K21" s="7">
+        <v>4</v>
+      </c>
+      <c r="L21" s="7">
+        <v>4</v>
+      </c>
+      <c r="M21" s="8">
+        <f>SUM(D21:L21)</f>
+        <v>33</v>
+      </c>
+      <c r="N21" s="8"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="7">
+        <v>3</v>
+      </c>
+      <c r="E22" s="7">
+        <v>2</v>
+      </c>
+      <c r="F22" s="7">
+        <v>3</v>
+      </c>
+      <c r="G22" s="7">
+        <v>2</v>
+      </c>
+      <c r="H22" s="7">
+        <v>2</v>
+      </c>
+      <c r="I22" s="7">
+        <v>1</v>
+      </c>
+      <c r="J22" s="7">
+        <v>3</v>
+      </c>
+      <c r="K22" s="7">
+        <v>3</v>
+      </c>
+      <c r="L22" s="7">
+        <v>2</v>
+      </c>
+      <c r="M22" s="8">
+        <f>SUM(D22:L22)</f>
+        <v>21</v>
+      </c>
+      <c r="N22" s="8"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="6">
+        <v>44090</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="7">
+        <v>4</v>
+      </c>
+      <c r="E26" s="7">
+        <v>4</v>
+      </c>
+      <c r="F26" s="7">
+        <v>5</v>
+      </c>
+      <c r="G26" s="7">
+        <v>3</v>
+      </c>
+      <c r="H26" s="7">
+        <v>4</v>
+      </c>
+      <c r="I26" s="7">
+        <v>4</v>
+      </c>
+      <c r="J26" s="7">
+        <v>4</v>
+      </c>
+      <c r="K26" s="7">
+        <v>3</v>
+      </c>
+      <c r="L26" s="7">
+        <v>6</v>
+      </c>
+      <c r="M26" s="8">
+        <f>SUM(D26:L26)</f>
+        <v>37</v>
+      </c>
+      <c r="N26" s="8"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="7">
+        <v>2</v>
+      </c>
+      <c r="E27" s="7">
+        <v>2</v>
+      </c>
+      <c r="F27" s="7">
+        <v>3</v>
+      </c>
+      <c r="G27" s="7">
+        <v>2</v>
+      </c>
+      <c r="H27" s="7">
+        <v>2</v>
+      </c>
+      <c r="I27" s="7">
+        <v>2</v>
+      </c>
+      <c r="J27" s="7">
+        <v>2</v>
+      </c>
+      <c r="K27" s="7">
+        <v>2</v>
+      </c>
+      <c r="L27" s="7">
+        <v>3</v>
+      </c>
+      <c r="M27" s="8">
+        <f>SUM(D27:L27)</f>
+        <v>20</v>
+      </c>
+      <c r="N27" s="8"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" s="6">
+        <v>44102</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="7">
+        <v>4</v>
+      </c>
+      <c r="E31" s="7">
+        <v>3</v>
+      </c>
+      <c r="F31" s="7">
+        <v>5</v>
+      </c>
+      <c r="G31" s="7">
+        <v>4</v>
+      </c>
+      <c r="H31" s="7">
+        <v>4</v>
+      </c>
+      <c r="I31" s="7">
+        <v>5</v>
+      </c>
+      <c r="J31" s="7">
+        <v>5</v>
+      </c>
+      <c r="K31" s="7">
+        <v>5</v>
+      </c>
+      <c r="L31" s="7">
+        <v>4</v>
+      </c>
+      <c r="M31" s="8">
+        <f>SUM(D31:L31)</f>
+        <v>39</v>
+      </c>
+      <c r="N31" s="8"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="7">
+        <v>2</v>
+      </c>
+      <c r="E32" s="7">
+        <v>2</v>
+      </c>
+      <c r="F32" s="7">
+        <v>2</v>
+      </c>
+      <c r="G32" s="7">
+        <v>2</v>
+      </c>
+      <c r="H32" s="7">
+        <v>2</v>
+      </c>
+      <c r="I32" s="7">
+        <v>3</v>
+      </c>
+      <c r="J32" s="7">
+        <v>2</v>
+      </c>
+      <c r="K32" s="7">
+        <v>3</v>
+      </c>
+      <c r="L32" s="7">
+        <v>2</v>
+      </c>
+      <c r="M32" s="8">
+        <f>SUM(D32:L32)</f>
+        <v>20</v>
+      </c>
+      <c r="N32" s="8"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35" s="6">
+        <v>44267</v>
+      </c>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="7">
+        <v>3</v>
+      </c>
+      <c r="E36" s="7">
+        <v>6</v>
+      </c>
+      <c r="F36" s="7">
+        <v>8</v>
+      </c>
+      <c r="G36" s="7">
+        <v>4</v>
+      </c>
+      <c r="H36" s="7">
+        <v>4</v>
+      </c>
+      <c r="I36" s="7">
+        <v>7</v>
+      </c>
+      <c r="J36" s="7">
+        <v>4</v>
+      </c>
+      <c r="K36" s="7">
+        <v>4</v>
+      </c>
+      <c r="L36" s="7">
+        <v>5</v>
+      </c>
+      <c r="M36" s="8">
+        <f>SUM(D36:L36)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A37" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="7">
+        <v>1</v>
+      </c>
+      <c r="E37" s="7">
+        <v>2</v>
+      </c>
+      <c r="F37" s="7">
+        <v>2</v>
+      </c>
+      <c r="G37" s="7">
+        <v>2</v>
+      </c>
+      <c r="H37" s="7">
+        <v>3</v>
+      </c>
+      <c r="I37" s="7">
+        <v>5</v>
+      </c>
+      <c r="J37" s="7">
+        <v>2</v>
+      </c>
+      <c r="K37" s="7">
+        <v>1</v>
+      </c>
+      <c r="L37" s="7">
+        <v>2</v>
+      </c>
+      <c r="M37" s="8">
+        <f>SUM(D37:L37)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M38" s="7"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A40" s="6">
+        <v>44279</v>
+      </c>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="7">
+        <v>4</v>
+      </c>
+      <c r="E41" s="7">
+        <v>4</v>
+      </c>
+      <c r="F41" s="7">
+        <v>6</v>
+      </c>
+      <c r="G41" s="7">
+        <v>4</v>
+      </c>
+      <c r="H41" s="7">
+        <v>4</v>
+      </c>
+      <c r="I41" s="7">
+        <v>4</v>
+      </c>
+      <c r="J41" s="7">
+        <v>6</v>
+      </c>
+      <c r="K41" s="7">
+        <v>4</v>
+      </c>
+      <c r="L41" s="7">
+        <v>6</v>
+      </c>
+      <c r="M41" s="8">
+        <f>SUM(D41:L41)</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A42" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="7">
+        <v>2</v>
+      </c>
+      <c r="E42" s="7">
+        <v>2</v>
+      </c>
+      <c r="F42" s="7">
+        <v>4</v>
+      </c>
+      <c r="G42" s="7">
+        <v>2</v>
+      </c>
+      <c r="H42" s="7">
+        <v>2</v>
+      </c>
+      <c r="I42" s="7">
+        <v>2</v>
+      </c>
+      <c r="J42" s="7">
+        <v>4</v>
+      </c>
+      <c r="K42" s="7">
+        <v>2</v>
+      </c>
+      <c r="L42" s="7">
+        <v>3</v>
+      </c>
+      <c r="M42" s="8">
+        <f>SUM(D42:L42)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A43" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L43" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M43" s="7"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="7"/>
+      <c r="M45" s="7"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="7"/>
+      <c r="L46" s="7"/>
+      <c r="M46" s="8"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A47" s="8"/>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="7"/>
+      <c r="L47" s="7"/>
+      <c r="M47" s="8"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A48" s="8"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="7"/>
+      <c r="K48" s="7"/>
+      <c r="L48" s="7"/>
+      <c r="M48" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9DD2039-084D-3C4E-B129-968266BAB55E}">
+  <dimension ref="A1:X30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1">
+        <v>27539</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1">
+        <v>6</v>
+      </c>
+      <c r="J2" s="1">
+        <v>7</v>
+      </c>
+      <c r="K2" s="1">
+        <v>8</v>
+      </c>
+      <c r="L2" s="1">
+        <v>9</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>71.599999999999994</v>
+      </c>
+      <c r="C4" s="1">
+        <v>139</v>
+      </c>
+      <c r="D4" s="1">
+        <v>125</v>
+      </c>
+      <c r="E4" s="1">
+        <v>150</v>
+      </c>
+      <c r="F4" s="1">
+        <v>118</v>
+      </c>
+      <c r="G4" s="1">
+        <v>117</v>
+      </c>
+      <c r="H4" s="1">
+        <v>134</v>
+      </c>
+      <c r="I4" s="1">
+        <v>174</v>
+      </c>
+      <c r="J4" s="1">
+        <v>136</v>
+      </c>
+      <c r="K4" s="1">
+        <v>100</v>
+      </c>
+      <c r="L4" s="1">
+        <v>155</v>
+      </c>
+      <c r="M4" s="1">
+        <v>1209</v>
+      </c>
+      <c r="N4" s="1"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>54</v>
+      </c>
+      <c r="C5" s="1">
+        <v>126</v>
+      </c>
+      <c r="D5" s="1">
+        <v>105</v>
+      </c>
+      <c r="E5" s="1">
+        <v>132</v>
+      </c>
+      <c r="F5" s="1">
+        <v>105</v>
+      </c>
+      <c r="G5" s="1">
+        <v>102</v>
+      </c>
+      <c r="H5" s="1">
+        <v>105</v>
+      </c>
+      <c r="I5" s="1">
+        <v>159</v>
+      </c>
+      <c r="J5" s="1">
+        <v>112</v>
+      </c>
+      <c r="K5" s="1">
+        <v>90</v>
+      </c>
+      <c r="L5" s="1">
+        <v>130</v>
+      </c>
+      <c r="M5" s="1">
+        <v>1040</v>
+      </c>
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1">
+        <v>113</v>
+      </c>
+      <c r="D6" s="1">
+        <v>77</v>
+      </c>
+      <c r="E6" s="1">
+        <v>117</v>
+      </c>
+      <c r="F6" s="1">
+        <v>90</v>
+      </c>
+      <c r="G6" s="1">
+        <v>92</v>
+      </c>
+      <c r="H6" s="1">
+        <v>77</v>
+      </c>
+      <c r="I6" s="1">
+        <v>93</v>
+      </c>
+      <c r="J6" s="1">
+        <v>85</v>
+      </c>
+      <c r="K6" s="1">
+        <v>78</v>
+      </c>
+      <c r="L6" s="1">
+        <v>110</v>
+      </c>
+      <c r="M6" s="1">
+        <v>819</v>
+      </c>
+      <c r="N6" s="1"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1">
+        <v>3</v>
+      </c>
+      <c r="F7" s="1">
+        <v>3</v>
+      </c>
+      <c r="G7" s="1">
+        <v>3</v>
+      </c>
+      <c r="H7" s="1">
+        <v>3</v>
+      </c>
+      <c r="I7" s="1">
+        <v>3</v>
+      </c>
+      <c r="J7" s="1">
+        <v>3</v>
+      </c>
+      <c r="K7" s="1">
+        <v>3</v>
+      </c>
+      <c r="L7" s="1">
+        <v>3</v>
+      </c>
+      <c r="M7" s="1">
+        <v>27</v>
+      </c>
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1">
+        <v>4</v>
+      </c>
+      <c r="H8" s="1">
+        <v>5</v>
+      </c>
+      <c r="I8" s="1">
+        <v>6</v>
+      </c>
+      <c r="J8" s="1">
+        <v>7</v>
+      </c>
+      <c r="K8" s="1">
+        <v>8</v>
+      </c>
+      <c r="L8" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
+        <v>44342</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="7">
+        <v>3</v>
+      </c>
+      <c r="E11" s="7">
+        <v>6</v>
+      </c>
+      <c r="F11" s="7">
+        <v>5</v>
+      </c>
+      <c r="G11" s="7">
+        <v>4</v>
+      </c>
+      <c r="H11" s="7">
+        <v>5</v>
+      </c>
+      <c r="I11" s="7">
+        <v>5</v>
+      </c>
+      <c r="J11" s="7">
+        <v>3</v>
+      </c>
+      <c r="K11" s="7">
+        <v>5</v>
+      </c>
+      <c r="L11" s="7">
+        <v>4</v>
+      </c>
+      <c r="M11" s="8">
+        <f>SUM(D11:L11)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="7">
+        <v>1</v>
+      </c>
+      <c r="E12" s="7">
+        <v>2</v>
+      </c>
+      <c r="F12" s="7">
+        <v>3</v>
+      </c>
+      <c r="G12" s="7">
+        <v>2</v>
+      </c>
+      <c r="H12" s="7">
+        <v>2</v>
+      </c>
+      <c r="I12" s="7">
+        <v>3</v>
+      </c>
+      <c r="J12" s="7">
+        <v>1</v>
+      </c>
+      <c r="K12" s="7">
+        <v>2</v>
+      </c>
+      <c r="L12" s="7">
+        <v>1</v>
+      </c>
+      <c r="M12" s="8">
+        <f>SUM(D12:L12)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F45684-D9E4-2242-9821-C781990B9A28}">
+  <dimension ref="A1:X43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1">
+        <v>27511</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1">
+        <v>6</v>
+      </c>
+      <c r="J2" s="1">
+        <v>7</v>
+      </c>
+      <c r="K2" s="1">
+        <v>8</v>
+      </c>
+      <c r="L2" s="1">
+        <v>9</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" s="1">
+        <v>10</v>
+      </c>
+      <c r="O2" s="1">
+        <v>11</v>
+      </c>
+      <c r="P2" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>13</v>
+      </c>
+      <c r="R2" s="1">
+        <v>14</v>
+      </c>
+      <c r="S2" s="1">
+        <v>15</v>
+      </c>
+      <c r="T2" s="1">
+        <v>16</v>
+      </c>
+      <c r="U2" s="1">
+        <v>17</v>
+      </c>
+      <c r="V2" s="1">
+        <v>18</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>71.599999999999994</v>
+      </c>
+      <c r="C4" s="1">
+        <v>139</v>
+      </c>
+      <c r="D4" s="1">
         <v>411</v>
       </c>
       <c r="E4" s="1">

</xml_diff>

<commit_message>
Add form_txt check for editable fields
</commit_message>
<xml_diff>
--- a/spec/fixtures/Golf.xlsx
+++ b/spec/fixtures/Golf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulkristoff/dev/golf/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFB1DFF-0655-0249-A898-A31A2E2D982C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D996CB7E-12DC-7B4D-9CFE-886118FC434C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7560" yWindow="1180" windowWidth="17600" windowHeight="17440" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
+    <workbookView xWindow="2960" yWindow="1660" windowWidth="21120" windowHeight="17440" activeTab="3" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
   </bookViews>
   <sheets>
     <sheet name="Knight's play 1-9" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="35">
   <si>
     <t>Hole</t>
   </si>
@@ -128,6 +128,21 @@
   <si>
     <t>L</t>
   </si>
+  <si>
+    <t>Fairway</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>80 &lt;</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
 </sst>
 </file>
 
@@ -213,7 +228,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -225,6 +240,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -542,7 +558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{045CE2A8-F6DB-4143-9691-363739FD69FB}">
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
@@ -1729,10 +1745,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8526A8B9-0C97-E94E-BA2A-E4D31B8BA027}">
-  <dimension ref="A1:X48"/>
+  <dimension ref="A1:X50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:M50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2815,7 +2831,9 @@
       <c r="M43" s="7"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A45" s="6"/>
+      <c r="A45" s="6">
+        <v>44402</v>
+      </c>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
       <c r="D45" s="7"/>
@@ -2830,49 +2848,167 @@
       <c r="M45" s="7"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A46" s="1"/>
+      <c r="A46" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="7"/>
-      <c r="I46" s="7"/>
-      <c r="J46" s="7"/>
-      <c r="K46" s="7"/>
-      <c r="L46" s="7"/>
-      <c r="M46" s="8"/>
+      <c r="D46" s="7">
+        <v>3</v>
+      </c>
+      <c r="E46" s="7">
+        <v>5</v>
+      </c>
+      <c r="F46" s="7">
+        <v>4</v>
+      </c>
+      <c r="G46" s="7">
+        <v>4</v>
+      </c>
+      <c r="H46" s="7">
+        <v>4</v>
+      </c>
+      <c r="I46" s="7">
+        <v>4</v>
+      </c>
+      <c r="J46" s="7">
+        <v>4</v>
+      </c>
+      <c r="K46" s="7">
+        <v>3</v>
+      </c>
+      <c r="L46" s="7">
+        <v>8</v>
+      </c>
+      <c r="M46" s="8">
+        <f>SUM(D46:L46)</f>
+        <v>39</v>
+      </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A47" s="8"/>
+      <c r="A47" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
-      <c r="I47" s="7"/>
-      <c r="J47" s="7"/>
-      <c r="K47" s="7"/>
-      <c r="L47" s="7"/>
-      <c r="M47" s="8"/>
+      <c r="D47" s="7">
+        <v>1</v>
+      </c>
+      <c r="E47" s="7">
+        <v>2</v>
+      </c>
+      <c r="F47" s="7">
+        <v>2</v>
+      </c>
+      <c r="G47" s="7">
+        <v>2</v>
+      </c>
+      <c r="H47" s="7">
+        <v>2</v>
+      </c>
+      <c r="I47" s="7">
+        <v>2</v>
+      </c>
+      <c r="J47" s="7">
+        <v>2</v>
+      </c>
+      <c r="K47" s="7">
+        <v>2</v>
+      </c>
+      <c r="L47" s="7">
+        <v>3</v>
+      </c>
+      <c r="M47" s="8">
+        <f>SUM(D47:L47)</f>
+        <v>18</v>
+      </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A48" s="8"/>
+      <c r="A48" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
       <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
+      <c r="E48" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="F48" s="7"/>
       <c r="G48" s="7"/>
       <c r="H48" s="7"/>
       <c r="I48" s="7"/>
       <c r="J48" s="7"/>
-      <c r="K48" s="7"/>
-      <c r="L48" s="7"/>
+      <c r="K48" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L48" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="M48" s="7"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D49" t="s">
+        <v>31</v>
+      </c>
+      <c r="E49" t="s">
+        <v>31</v>
+      </c>
+      <c r="F49" t="s">
+        <v>31</v>
+      </c>
+      <c r="G49" t="s">
+        <v>31</v>
+      </c>
+      <c r="H49" t="s">
+        <v>31</v>
+      </c>
+      <c r="I49" t="s">
+        <v>31</v>
+      </c>
+      <c r="J49" t="s">
+        <v>31</v>
+      </c>
+      <c r="K49" t="s">
+        <v>31</v>
+      </c>
+      <c r="L49" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D50">
+        <v>2</v>
+      </c>
+      <c r="E50">
+        <v>4</v>
+      </c>
+      <c r="F50">
+        <v>3</v>
+      </c>
+      <c r="G50">
+        <v>4</v>
+      </c>
+      <c r="H50">
+        <v>3</v>
+      </c>
+      <c r="I50">
+        <v>3</v>
+      </c>
+      <c r="J50">
+        <v>3</v>
+      </c>
+      <c r="K50">
+        <v>2</v>
+      </c>
+      <c r="L50">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3498,10 +3634,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F45684-D9E4-2242-9821-C781990B9A28}">
-  <dimension ref="A1:X43"/>
+  <dimension ref="A1:X50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+    <sheetView tabSelected="1" topLeftCell="I19" workbookViewId="0">
+      <selection activeCell="W50" sqref="W50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5207,6 +5343,310 @@
       </c>
       <c r="V43" s="1"/>
     </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A45" s="2">
+        <v>44397</v>
+      </c>
+      <c r="B45" s="11">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C45" s="11">
+        <v>0.63541666666666663</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46">
+        <v>5</v>
+      </c>
+      <c r="E46">
+        <v>6</v>
+      </c>
+      <c r="F46">
+        <v>4</v>
+      </c>
+      <c r="G46">
+        <v>8</v>
+      </c>
+      <c r="H46">
+        <v>5</v>
+      </c>
+      <c r="I46">
+        <v>5</v>
+      </c>
+      <c r="J46">
+        <v>6</v>
+      </c>
+      <c r="K46" s="3">
+        <v>7</v>
+      </c>
+      <c r="L46" s="3">
+        <v>8</v>
+      </c>
+      <c r="M46" s="1">
+        <f>SUM(D46:L46)</f>
+        <v>54</v>
+      </c>
+      <c r="N46">
+        <v>8</v>
+      </c>
+      <c r="O46">
+        <v>5</v>
+      </c>
+      <c r="P46">
+        <v>10</v>
+      </c>
+      <c r="Q46">
+        <v>7</v>
+      </c>
+      <c r="R46">
+        <v>6</v>
+      </c>
+      <c r="S46">
+        <v>5</v>
+      </c>
+      <c r="T46">
+        <v>7</v>
+      </c>
+      <c r="U46" s="3">
+        <v>4</v>
+      </c>
+      <c r="V46" s="3">
+        <v>5</v>
+      </c>
+      <c r="W46" s="1">
+        <f>SUM(N46:V46)</f>
+        <v>57</v>
+      </c>
+      <c r="X46" s="1">
+        <f>W46+M46</f>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="E47">
+        <v>3</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+      <c r="G47">
+        <v>2</v>
+      </c>
+      <c r="H47">
+        <v>1</v>
+      </c>
+      <c r="I47">
+        <v>2</v>
+      </c>
+      <c r="J47">
+        <v>3</v>
+      </c>
+      <c r="K47" s="3">
+        <v>2</v>
+      </c>
+      <c r="L47" s="3">
+        <v>3</v>
+      </c>
+      <c r="M47" s="1">
+        <f>SUM(D47:L47)</f>
+        <v>19</v>
+      </c>
+      <c r="N47">
+        <v>3</v>
+      </c>
+      <c r="O47">
+        <v>1</v>
+      </c>
+      <c r="P47">
+        <v>2</v>
+      </c>
+      <c r="Q47">
+        <v>2</v>
+      </c>
+      <c r="R47">
+        <v>2</v>
+      </c>
+      <c r="S47">
+        <v>2</v>
+      </c>
+      <c r="T47">
+        <v>3</v>
+      </c>
+      <c r="U47" s="3">
+        <v>2</v>
+      </c>
+      <c r="V47" s="3">
+        <v>2</v>
+      </c>
+      <c r="W47" s="1">
+        <f>SUM(N47:V47)</f>
+        <v>19</v>
+      </c>
+      <c r="X47" s="1">
+        <f>W47+M47</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D48" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" t="s">
+        <v>11</v>
+      </c>
+      <c r="K48" s="1"/>
+      <c r="O48" t="s">
+        <v>11</v>
+      </c>
+      <c r="P48" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>29</v>
+      </c>
+      <c r="R48" t="s">
+        <v>20</v>
+      </c>
+      <c r="T48" t="s">
+        <v>11</v>
+      </c>
+      <c r="U48" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="V48" s="1"/>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D49" t="s">
+        <v>33</v>
+      </c>
+      <c r="E49" t="s">
+        <v>33</v>
+      </c>
+      <c r="F49" t="s">
+        <v>33</v>
+      </c>
+      <c r="G49" t="s">
+        <v>33</v>
+      </c>
+      <c r="H49" t="s">
+        <v>33</v>
+      </c>
+      <c r="I49" t="s">
+        <v>33</v>
+      </c>
+      <c r="J49" t="s">
+        <v>33</v>
+      </c>
+      <c r="K49" t="s">
+        <v>34</v>
+      </c>
+      <c r="L49" t="s">
+        <v>33</v>
+      </c>
+      <c r="N49" t="s">
+        <v>33</v>
+      </c>
+      <c r="O49" t="s">
+        <v>33</v>
+      </c>
+      <c r="P49" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>33</v>
+      </c>
+      <c r="R49" t="s">
+        <v>34</v>
+      </c>
+      <c r="S49" t="s">
+        <v>34</v>
+      </c>
+      <c r="T49" t="s">
+        <v>33</v>
+      </c>
+      <c r="U49" t="s">
+        <v>33</v>
+      </c>
+      <c r="V49" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D50">
+        <v>3</v>
+      </c>
+      <c r="E50">
+        <v>4</v>
+      </c>
+      <c r="F50">
+        <v>3</v>
+      </c>
+      <c r="G50">
+        <v>5</v>
+      </c>
+      <c r="H50">
+        <v>2</v>
+      </c>
+      <c r="I50">
+        <v>3</v>
+      </c>
+      <c r="J50">
+        <v>4</v>
+      </c>
+      <c r="K50">
+        <v>3</v>
+      </c>
+      <c r="L50">
+        <v>4</v>
+      </c>
+      <c r="N50">
+        <v>5</v>
+      </c>
+      <c r="O50">
+        <v>3</v>
+      </c>
+      <c r="P50">
+        <v>4</v>
+      </c>
+      <c r="Q50">
+        <v>5</v>
+      </c>
+      <c r="R50">
+        <v>3</v>
+      </c>
+      <c r="S50">
+        <v>3</v>
+      </c>
+      <c r="T50">
+        <v>4</v>
+      </c>
+      <c r="U50">
+        <v>3</v>
+      </c>
+      <c r="V50">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Handle excel file with extra round info.
</commit_message>
<xml_diff>
--- a/spec/fixtures/Golf.xlsx
+++ b/spec/fixtures/Golf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulkristoff/dev/golf/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D996CB7E-12DC-7B4D-9CFE-886118FC434C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9949019-B59C-8140-8899-02EAA93C0CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2960" yWindow="1660" windowWidth="21120" windowHeight="17440" activeTab="3" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19120" activeTab="1" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
   </bookViews>
   <sheets>
     <sheet name="Knight's play 1-9" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="38">
   <si>
     <t>Hole</t>
   </si>
@@ -143,6 +143,15 @@
   <si>
     <t>Y</t>
   </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Strokes inside 80</t>
+  </si>
+  <si>
+    <t>Fairways Hit</t>
+  </si>
 </sst>
 </file>
 
@@ -228,7 +237,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -241,6 +250,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="18" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="19" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -556,13 +567,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{045CE2A8-F6DB-4143-9691-363739FD69FB}">
-  <dimension ref="A1:M48"/>
+  <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1734,6 +1748,196 @@
       <c r="L48" s="7"/>
       <c r="M48" s="7"/>
     </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A50" s="6">
+        <v>44413</v>
+      </c>
+      <c r="B50" s="12">
+        <v>0.46875</v>
+      </c>
+      <c r="C50" s="13">
+        <v>0.51527777777777783</v>
+      </c>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="7"/>
+      <c r="K50" s="7"/>
+      <c r="L50" s="7"/>
+      <c r="M50" s="7"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="7">
+        <v>5</v>
+      </c>
+      <c r="E51" s="7">
+        <v>5</v>
+      </c>
+      <c r="F51" s="7">
+        <v>3</v>
+      </c>
+      <c r="G51" s="7">
+        <v>6</v>
+      </c>
+      <c r="H51" s="7">
+        <v>4</v>
+      </c>
+      <c r="I51" s="7">
+        <v>3</v>
+      </c>
+      <c r="J51" s="7">
+        <v>4</v>
+      </c>
+      <c r="K51" s="7">
+        <v>4</v>
+      </c>
+      <c r="L51" s="7">
+        <v>5</v>
+      </c>
+      <c r="M51" s="8">
+        <f>SUM(D51:L51)</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A52" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="7">
+        <v>3</v>
+      </c>
+      <c r="E52" s="7">
+        <v>3</v>
+      </c>
+      <c r="F52" s="7">
+        <v>1</v>
+      </c>
+      <c r="G52" s="7">
+        <v>3</v>
+      </c>
+      <c r="H52" s="7">
+        <v>2</v>
+      </c>
+      <c r="I52" s="7">
+        <v>1</v>
+      </c>
+      <c r="J52" s="7">
+        <v>3</v>
+      </c>
+      <c r="K52" s="7">
+        <v>2</v>
+      </c>
+      <c r="L52" s="7">
+        <v>3</v>
+      </c>
+      <c r="M52" s="8">
+        <f>SUM(D52:L52)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A53" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B53" s="8"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H53" s="7"/>
+      <c r="I53" s="7"/>
+      <c r="J53" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K53" s="7"/>
+      <c r="L53" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M53" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D54" t="s">
+        <v>35</v>
+      </c>
+      <c r="E54" t="s">
+        <v>35</v>
+      </c>
+      <c r="F54" t="s">
+        <v>35</v>
+      </c>
+      <c r="G54" t="s">
+        <v>35</v>
+      </c>
+      <c r="H54" t="s">
+        <v>35</v>
+      </c>
+      <c r="I54" t="s">
+        <v>35</v>
+      </c>
+      <c r="J54" t="s">
+        <v>35</v>
+      </c>
+      <c r="K54" t="s">
+        <v>35</v>
+      </c>
+      <c r="L54" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D55">
+        <v>4</v>
+      </c>
+      <c r="E55">
+        <v>4</v>
+      </c>
+      <c r="F55">
+        <v>2</v>
+      </c>
+      <c r="G55">
+        <v>5</v>
+      </c>
+      <c r="H55">
+        <v>3</v>
+      </c>
+      <c r="I55">
+        <v>2</v>
+      </c>
+      <c r="J55">
+        <v>3</v>
+      </c>
+      <c r="K55">
+        <v>3</v>
+      </c>
+      <c r="L55">
+        <v>4</v>
+      </c>
+      <c r="M55">
+        <f>SUM(D55:L55)</f>
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1745,10 +1949,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8526A8B9-0C97-E94E-BA2A-E4D31B8BA027}">
-  <dimension ref="A1:X50"/>
+  <dimension ref="A1:X57"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49:M50"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2946,9 +3150,9 @@
       </c>
       <c r="M48" s="7"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D49" t="s">
         <v>31</v>
@@ -2978,9 +3182,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D50">
         <v>2</v>
@@ -3008,6 +3212,192 @@
       </c>
       <c r="L50">
         <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A52" s="6">
+        <v>44413</v>
+      </c>
+      <c r="B52" s="12">
+        <v>0.51527777777777783</v>
+      </c>
+      <c r="C52" s="12">
+        <v>0.55972222222222223</v>
+      </c>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="7"/>
+      <c r="I52" s="7"/>
+      <c r="J52" s="7"/>
+      <c r="K52" s="7"/>
+      <c r="L52" s="7"/>
+      <c r="M52" s="7"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="7">
+        <v>3</v>
+      </c>
+      <c r="E53" s="7">
+        <v>5</v>
+      </c>
+      <c r="F53" s="7">
+        <v>4</v>
+      </c>
+      <c r="G53" s="7">
+        <v>5</v>
+      </c>
+      <c r="H53" s="7">
+        <v>4</v>
+      </c>
+      <c r="I53" s="7">
+        <v>3</v>
+      </c>
+      <c r="J53" s="7">
+        <v>4</v>
+      </c>
+      <c r="K53" s="7">
+        <v>4</v>
+      </c>
+      <c r="L53" s="7">
+        <v>6</v>
+      </c>
+      <c r="M53" s="8">
+        <f>SUM(D53:L53)</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A54" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="7">
+        <v>2</v>
+      </c>
+      <c r="E54" s="7">
+        <v>3</v>
+      </c>
+      <c r="F54" s="7">
+        <v>2</v>
+      </c>
+      <c r="G54" s="7">
+        <v>3</v>
+      </c>
+      <c r="H54" s="7">
+        <v>2</v>
+      </c>
+      <c r="I54" s="7">
+        <v>1</v>
+      </c>
+      <c r="J54" s="7">
+        <v>2</v>
+      </c>
+      <c r="K54" s="7">
+        <v>1</v>
+      </c>
+      <c r="L54" s="7">
+        <v>2</v>
+      </c>
+      <c r="M54" s="8">
+        <f>SUM(D54:L54)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A55" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B55" s="8"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H55" s="7"/>
+      <c r="I55" s="7"/>
+      <c r="J55" s="7"/>
+      <c r="K55" s="7"/>
+      <c r="L55" s="7"/>
+      <c r="M55" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D56" t="s">
+        <v>35</v>
+      </c>
+      <c r="E56" t="s">
+        <v>35</v>
+      </c>
+      <c r="F56" t="s">
+        <v>35</v>
+      </c>
+      <c r="G56" t="s">
+        <v>35</v>
+      </c>
+      <c r="H56" t="s">
+        <v>35</v>
+      </c>
+      <c r="I56" t="s">
+        <v>35</v>
+      </c>
+      <c r="J56" t="s">
+        <v>35</v>
+      </c>
+      <c r="K56" t="s">
+        <v>35</v>
+      </c>
+      <c r="L56" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="E57">
+        <v>4</v>
+      </c>
+      <c r="F57">
+        <v>3</v>
+      </c>
+      <c r="G57">
+        <v>4</v>
+      </c>
+      <c r="H57">
+        <v>3</v>
+      </c>
+      <c r="I57">
+        <v>3</v>
+      </c>
+      <c r="J57">
+        <v>3</v>
+      </c>
+      <c r="K57">
+        <v>3</v>
+      </c>
+      <c r="L57">
+        <v>5</v>
+      </c>
+      <c r="M57">
+        <f>SUM(D57:L57)</f>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -3636,7 +4026,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F45684-D9E4-2242-9821-C781990B9A28}">
   <dimension ref="A1:X50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I19" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="W50" sqref="W50"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Course performance - hole average
</commit_message>
<xml_diff>
--- a/spec/fixtures/Golf.xlsx
+++ b/spec/fixtures/Golf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulkristoff/dev/golf/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9949019-B59C-8140-8899-02EAA93C0CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5995B2A-F22D-8D4E-A322-6114B27461FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19120" activeTab="1" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="33600" windowHeight="19120" activeTab="2" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
   </bookViews>
   <sheets>
     <sheet name="Knight's play 1-9" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="38">
   <si>
     <t>Hole</t>
   </si>
@@ -157,7 +157,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -191,6 +191,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -237,7 +245,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -252,6 +260,7 @@
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="19" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -569,7 +578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{045CE2A8-F6DB-4143-9691-363739FD69FB}">
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
@@ -1949,10 +1958,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8526A8B9-0C97-E94E-BA2A-E4D31B8BA027}">
-  <dimension ref="A1:X57"/>
+  <dimension ref="A1:X64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58:M64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3327,8 +3336,7 @@
       <c r="I55" s="7"/>
       <c r="J55" s="7"/>
       <c r="K55" s="7"/>
-      <c r="L55" s="7"/>
-      <c r="M55" s="7" t="s">
+      <c r="L55" s="7" t="s">
         <v>11</v>
       </c>
     </row>
@@ -3398,6 +3406,194 @@
       <c r="M57">
         <f>SUM(D57:L57)</f>
         <v>30</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A59" s="6">
+        <v>44418</v>
+      </c>
+      <c r="B59" s="12">
+        <v>0.5625</v>
+      </c>
+      <c r="C59" s="12">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="7"/>
+      <c r="H59" s="7"/>
+      <c r="I59" s="7"/>
+      <c r="J59" s="7"/>
+      <c r="K59" s="7"/>
+      <c r="L59" s="7"/>
+      <c r="M59" s="7"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="7">
+        <v>2</v>
+      </c>
+      <c r="E60" s="7">
+        <v>3</v>
+      </c>
+      <c r="F60" s="7">
+        <v>5</v>
+      </c>
+      <c r="G60" s="7">
+        <v>2</v>
+      </c>
+      <c r="H60" s="7">
+        <v>4</v>
+      </c>
+      <c r="I60" s="7">
+        <v>4</v>
+      </c>
+      <c r="J60" s="7">
+        <v>4</v>
+      </c>
+      <c r="K60" s="7">
+        <v>5</v>
+      </c>
+      <c r="L60" s="7">
+        <v>6</v>
+      </c>
+      <c r="M60" s="8">
+        <f>SUM(D60:L60)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A61" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B61" s="8"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="7">
+        <v>1</v>
+      </c>
+      <c r="E61" s="7">
+        <v>2</v>
+      </c>
+      <c r="F61" s="7">
+        <v>3</v>
+      </c>
+      <c r="G61" s="7">
+        <v>1</v>
+      </c>
+      <c r="H61" s="7">
+        <v>2</v>
+      </c>
+      <c r="I61" s="7">
+        <v>2</v>
+      </c>
+      <c r="J61" s="7">
+        <v>1</v>
+      </c>
+      <c r="K61" s="7">
+        <v>2</v>
+      </c>
+      <c r="L61" s="7">
+        <v>3</v>
+      </c>
+      <c r="M61" s="8">
+        <f>SUM(D61:L61)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A62" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B62" s="8"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="7"/>
+      <c r="I62" s="7"/>
+      <c r="J62" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="K62" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L62" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M62" s="7"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D63" t="s">
+        <v>35</v>
+      </c>
+      <c r="E63" t="s">
+        <v>35</v>
+      </c>
+      <c r="F63" t="s">
+        <v>35</v>
+      </c>
+      <c r="G63" t="s">
+        <v>35</v>
+      </c>
+      <c r="H63" t="s">
+        <v>35</v>
+      </c>
+      <c r="I63" t="s">
+        <v>35</v>
+      </c>
+      <c r="J63" t="s">
+        <v>35</v>
+      </c>
+      <c r="K63" t="s">
+        <v>35</v>
+      </c>
+      <c r="L63" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>2</v>
+      </c>
+      <c r="F64">
+        <v>4</v>
+      </c>
+      <c r="G64">
+        <v>1</v>
+      </c>
+      <c r="H64">
+        <v>3</v>
+      </c>
+      <c r="I64">
+        <v>3</v>
+      </c>
+      <c r="J64">
+        <v>3</v>
+      </c>
+      <c r="K64">
+        <v>4</v>
+      </c>
+      <c r="L64" s="14">
+        <v>5</v>
+      </c>
+      <c r="M64">
+        <f>SUM(D64:L64)</f>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -3410,8 +3606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9DD2039-084D-3C4E-B129-968266BAB55E}">
   <dimension ref="A1:X30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3835,69 +4031,193 @@
       <c r="M13" s="7"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="M15" s="1"/>
+      <c r="A15" s="6">
+        <v>44418</v>
+      </c>
+      <c r="B15" s="12">
+        <v>0.51527777777777783</v>
+      </c>
+      <c r="C15" s="12">
+        <v>0.5625</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
       <c r="N15" s="1"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
+      <c r="A16" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="M16" s="1"/>
+      <c r="D16" s="7">
+        <v>5</v>
+      </c>
+      <c r="E16" s="7">
+        <v>5</v>
+      </c>
+      <c r="F16" s="7">
+        <v>4</v>
+      </c>
+      <c r="G16" s="7">
+        <v>4</v>
+      </c>
+      <c r="H16" s="7">
+        <v>4</v>
+      </c>
+      <c r="I16" s="7">
+        <v>4</v>
+      </c>
+      <c r="J16" s="7">
+        <v>5</v>
+      </c>
+      <c r="K16" s="7">
+        <v>4</v>
+      </c>
+      <c r="L16" s="7">
+        <v>4</v>
+      </c>
+      <c r="M16" s="8">
+        <f>SUM(D16:L16)</f>
+        <v>39</v>
+      </c>
       <c r="N16" s="1"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="M17" s="1"/>
+      <c r="A17" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="7">
+        <v>2</v>
+      </c>
+      <c r="E17" s="7">
+        <v>2</v>
+      </c>
+      <c r="F17" s="7">
+        <v>2</v>
+      </c>
+      <c r="G17" s="7">
+        <v>2</v>
+      </c>
+      <c r="H17" s="7">
+        <v>2</v>
+      </c>
+      <c r="I17" s="7">
+        <v>2</v>
+      </c>
+      <c r="J17" s="7">
+        <v>2</v>
+      </c>
+      <c r="K17" s="7">
+        <v>2</v>
+      </c>
+      <c r="L17" s="7">
+        <v>2</v>
+      </c>
+      <c r="M17" s="8">
+        <f>SUM(D17:L17)</f>
+        <v>18</v>
+      </c>
       <c r="N17" s="1"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
+      <c r="A18" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
+      <c r="I18" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
       <c r="L18" s="7"/>
-      <c r="M18" s="8"/>
+      <c r="M18" s="7"/>
       <c r="N18" s="8"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="8"/>
+      <c r="A19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19" t="s">
+        <v>35</v>
+      </c>
+      <c r="I19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J19" t="s">
+        <v>35</v>
+      </c>
+      <c r="K19" t="s">
+        <v>35</v>
+      </c>
+      <c r="L19" t="s">
+        <v>35</v>
+      </c>
       <c r="N19" s="8"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
+      <c r="A20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+      <c r="E20">
+        <v>4</v>
+      </c>
+      <c r="F20">
+        <v>3</v>
+      </c>
+      <c r="G20">
+        <v>3</v>
+      </c>
+      <c r="H20">
+        <v>3</v>
+      </c>
+      <c r="I20">
+        <v>3</v>
+      </c>
+      <c r="J20">
+        <v>4</v>
+      </c>
+      <c r="K20">
+        <v>3</v>
+      </c>
+      <c r="L20" s="14">
+        <v>3</v>
+      </c>
+      <c r="M20">
+        <f>SUM(D20:L20)</f>
+        <v>30</v>
+      </c>
       <c r="N20" s="7"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added golf terms, squares and circles for strokes
</commit_message>
<xml_diff>
--- a/spec/fixtures/Golf.xlsx
+++ b/spec/fixtures/Golf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulkristoff/dev/golf/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA1B8A9-8BD2-3B41-9E10-CD23D0DDCD0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F57B86BE-A8F9-BA4E-8A54-B1D4F65F15DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="860" windowWidth="31760" windowHeight="12920" activeTab="3" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
+    <workbookView xWindow="60" yWindow="860" windowWidth="31760" windowHeight="12920" activeTab="2" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
   </bookViews>
   <sheets>
     <sheet name="Beachwood Golf Course" sheetId="6" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="48">
   <si>
     <t>Hole</t>
   </si>
@@ -1458,10 +1458,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{045CE2A8-F6DB-4143-9691-363739FD69FB}">
-  <dimension ref="A1:M76"/>
+  <dimension ref="A1:M83"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70:M76"/>
+    <sheetView topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="M83" sqref="M83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3391,6 +3391,190 @@
         <v>31</v>
       </c>
     </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A78" s="6">
+        <v>44532</v>
+      </c>
+      <c r="B78" s="12">
+        <v>0.46875</v>
+      </c>
+      <c r="C78" s="13">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="D78" s="7"/>
+      <c r="E78" s="7"/>
+      <c r="F78" s="7"/>
+      <c r="G78" s="7"/>
+      <c r="H78" s="7"/>
+      <c r="I78" s="7"/>
+      <c r="J78" s="7"/>
+      <c r="K78" s="7"/>
+      <c r="L78" s="7"/>
+      <c r="M78" s="7"/>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="7">
+        <v>6</v>
+      </c>
+      <c r="E79" s="7">
+        <v>3</v>
+      </c>
+      <c r="F79" s="7">
+        <v>4</v>
+      </c>
+      <c r="G79" s="7">
+        <v>5</v>
+      </c>
+      <c r="H79" s="7">
+        <v>3</v>
+      </c>
+      <c r="I79" s="7">
+        <v>5</v>
+      </c>
+      <c r="J79" s="7">
+        <v>3</v>
+      </c>
+      <c r="K79" s="7">
+        <v>4</v>
+      </c>
+      <c r="L79" s="7">
+        <v>5</v>
+      </c>
+      <c r="M79" s="8">
+        <f>SUM(D79:L79)</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A80" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B80" s="8"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="7">
+        <v>2</v>
+      </c>
+      <c r="E80" s="7">
+        <v>2</v>
+      </c>
+      <c r="F80" s="7">
+        <v>1</v>
+      </c>
+      <c r="G80" s="7">
+        <v>3</v>
+      </c>
+      <c r="H80" s="7">
+        <v>2</v>
+      </c>
+      <c r="I80" s="7">
+        <v>2</v>
+      </c>
+      <c r="J80" s="7">
+        <v>1</v>
+      </c>
+      <c r="K80" s="7">
+        <v>2</v>
+      </c>
+      <c r="L80" s="7">
+        <v>2</v>
+      </c>
+      <c r="M80" s="8">
+        <f>SUM(D80:L80)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A81" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B81" s="8"/>
+      <c r="C81" s="8"/>
+      <c r="D81" s="7"/>
+      <c r="E81" s="7"/>
+      <c r="F81" s="7"/>
+      <c r="G81" s="7"/>
+      <c r="H81" s="7"/>
+      <c r="I81" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J81" s="7"/>
+      <c r="K81" s="7"/>
+      <c r="L81" s="7"/>
+      <c r="M81" s="7"/>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D82" t="s">
+        <v>35</v>
+      </c>
+      <c r="E82" t="s">
+        <v>35</v>
+      </c>
+      <c r="F82" t="s">
+        <v>35</v>
+      </c>
+      <c r="G82" t="s">
+        <v>35</v>
+      </c>
+      <c r="H82" t="s">
+        <v>35</v>
+      </c>
+      <c r="I82" t="s">
+        <v>35</v>
+      </c>
+      <c r="J82" t="s">
+        <v>35</v>
+      </c>
+      <c r="K82" t="s">
+        <v>35</v>
+      </c>
+      <c r="L82" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D83">
+        <v>5</v>
+      </c>
+      <c r="E83">
+        <v>2</v>
+      </c>
+      <c r="F83">
+        <v>3</v>
+      </c>
+      <c r="G83">
+        <v>4</v>
+      </c>
+      <c r="H83">
+        <v>2</v>
+      </c>
+      <c r="I83">
+        <v>3</v>
+      </c>
+      <c r="J83">
+        <v>2</v>
+      </c>
+      <c r="K83">
+        <v>3</v>
+      </c>
+      <c r="L83">
+        <v>4</v>
+      </c>
+      <c r="M83">
+        <f>SUM(D83:L83)</f>
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3402,10 +3586,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8526A8B9-0C97-E94E-BA2A-E4D31B8BA027}">
-  <dimension ref="A1:X71"/>
+  <dimension ref="A1:X78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="M78" sqref="M78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5227,6 +5411,190 @@
         <v>28</v>
       </c>
     </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A73" s="6">
+        <v>44532</v>
+      </c>
+      <c r="B73" s="12">
+        <v>0.53125</v>
+      </c>
+      <c r="C73" s="12">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="D73" s="7"/>
+      <c r="E73" s="7"/>
+      <c r="F73" s="7"/>
+      <c r="G73" s="7"/>
+      <c r="H73" s="7"/>
+      <c r="I73" s="7"/>
+      <c r="J73" s="7"/>
+      <c r="K73" s="7"/>
+      <c r="L73" s="7"/>
+      <c r="M73" s="7"/>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="7">
+        <v>4</v>
+      </c>
+      <c r="E74" s="7">
+        <v>5</v>
+      </c>
+      <c r="F74" s="7">
+        <v>6</v>
+      </c>
+      <c r="G74" s="7">
+        <v>4</v>
+      </c>
+      <c r="H74" s="7">
+        <v>3</v>
+      </c>
+      <c r="I74" s="7">
+        <v>3</v>
+      </c>
+      <c r="J74" s="7">
+        <v>3</v>
+      </c>
+      <c r="K74" s="7">
+        <v>3</v>
+      </c>
+      <c r="L74" s="7">
+        <v>4</v>
+      </c>
+      <c r="M74" s="8">
+        <f>SUM(D74:L74)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A75" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B75" s="8"/>
+      <c r="C75" s="8"/>
+      <c r="D75" s="7">
+        <v>2</v>
+      </c>
+      <c r="E75" s="7">
+        <v>3</v>
+      </c>
+      <c r="F75" s="7">
+        <v>3</v>
+      </c>
+      <c r="G75" s="7">
+        <v>3</v>
+      </c>
+      <c r="H75" s="7">
+        <v>1</v>
+      </c>
+      <c r="I75" s="7">
+        <v>1</v>
+      </c>
+      <c r="J75" s="7">
+        <v>2</v>
+      </c>
+      <c r="K75" s="7">
+        <v>2</v>
+      </c>
+      <c r="L75" s="7">
+        <v>3</v>
+      </c>
+      <c r="M75" s="8">
+        <f>SUM(D75:L75)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A76" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B76" s="8"/>
+      <c r="C76" s="8"/>
+      <c r="D76" s="7"/>
+      <c r="E76" s="7"/>
+      <c r="F76" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G76" s="7"/>
+      <c r="H76" s="7"/>
+      <c r="I76" s="7"/>
+      <c r="J76" s="7"/>
+      <c r="K76" s="7"/>
+      <c r="L76" s="7"/>
+      <c r="M76" s="7"/>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D77" t="s">
+        <v>35</v>
+      </c>
+      <c r="E77" t="s">
+        <v>35</v>
+      </c>
+      <c r="F77" t="s">
+        <v>35</v>
+      </c>
+      <c r="G77" t="s">
+        <v>35</v>
+      </c>
+      <c r="H77" t="s">
+        <v>35</v>
+      </c>
+      <c r="I77" t="s">
+        <v>35</v>
+      </c>
+      <c r="J77" t="s">
+        <v>35</v>
+      </c>
+      <c r="K77" t="s">
+        <v>35</v>
+      </c>
+      <c r="L77" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D78">
+        <v>3</v>
+      </c>
+      <c r="E78">
+        <v>4</v>
+      </c>
+      <c r="F78">
+        <v>5</v>
+      </c>
+      <c r="G78">
+        <v>3</v>
+      </c>
+      <c r="H78">
+        <v>2</v>
+      </c>
+      <c r="I78">
+        <v>2</v>
+      </c>
+      <c r="J78">
+        <v>2</v>
+      </c>
+      <c r="K78">
+        <v>2</v>
+      </c>
+      <c r="L78" s="14">
+        <v>3</v>
+      </c>
+      <c r="M78">
+        <f>SUM(D78:L78)</f>
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -5237,7 +5605,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9DD2039-084D-3C4E-B129-968266BAB55E}">
   <dimension ref="A1:X30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Create Account, Adjusted the calculation handicap index; store on account.
</commit_message>
<xml_diff>
--- a/spec/fixtures/Golf.xlsx
+++ b/spec/fixtures/Golf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulkristoff/dev/golf/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8BE463-A2D9-F049-8AD2-6538561ACD06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E2D534-0D4D-D34E-8E0B-6F7575FAD4E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="860" windowWidth="31760" windowHeight="12920" activeTab="2" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="48">
   <si>
     <t>Hole</t>
   </si>
@@ -3774,10 +3774,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8526A8B9-0C97-E94E-BA2A-E4D31B8BA027}">
-  <dimension ref="A1:X85"/>
+  <dimension ref="A1:X92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79:XFD79"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5971,6 +5971,194 @@
         <v>28</v>
       </c>
     </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A87" s="6">
+        <v>44202</v>
+      </c>
+      <c r="B87" s="12">
+        <v>0.64444444444444449</v>
+      </c>
+      <c r="C87" s="12">
+        <v>0.6875</v>
+      </c>
+      <c r="D87" s="7"/>
+      <c r="E87" s="7"/>
+      <c r="F87" s="7"/>
+      <c r="G87" s="7"/>
+      <c r="H87" s="7"/>
+      <c r="I87" s="7"/>
+      <c r="J87" s="7"/>
+      <c r="K87" s="7"/>
+      <c r="L87" s="7"/>
+      <c r="M87" s="7"/>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B88" s="1"/>
+      <c r="C88" s="1"/>
+      <c r="D88" s="7">
+        <v>4</v>
+      </c>
+      <c r="E88" s="7">
+        <v>3</v>
+      </c>
+      <c r="F88" s="7">
+        <v>4</v>
+      </c>
+      <c r="G88" s="7">
+        <v>5</v>
+      </c>
+      <c r="H88" s="7">
+        <v>5</v>
+      </c>
+      <c r="I88" s="7">
+        <v>4</v>
+      </c>
+      <c r="J88" s="7">
+        <v>7</v>
+      </c>
+      <c r="K88" s="7">
+        <v>5</v>
+      </c>
+      <c r="L88" s="7">
+        <v>7</v>
+      </c>
+      <c r="M88" s="8">
+        <f>SUM(D88:L88)</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A89" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B89" s="8"/>
+      <c r="C89" s="8"/>
+      <c r="D89" s="7">
+        <v>2</v>
+      </c>
+      <c r="E89" s="7">
+        <v>2</v>
+      </c>
+      <c r="F89" s="7">
+        <v>1</v>
+      </c>
+      <c r="G89" s="7">
+        <v>3</v>
+      </c>
+      <c r="H89" s="7">
+        <v>3</v>
+      </c>
+      <c r="I89" s="7">
+        <v>2</v>
+      </c>
+      <c r="J89" s="7">
+        <v>4</v>
+      </c>
+      <c r="K89" s="7">
+        <v>2</v>
+      </c>
+      <c r="L89" s="7">
+        <v>4</v>
+      </c>
+      <c r="M89" s="8">
+        <f>SUM(D89:L89)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A90" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B90" s="8"/>
+      <c r="C90" s="8"/>
+      <c r="D90" s="7"/>
+      <c r="E90" s="7"/>
+      <c r="F90" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G90" s="7"/>
+      <c r="H90" s="7"/>
+      <c r="I90" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J90" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K90" s="7"/>
+      <c r="L90" s="7"/>
+      <c r="M90" s="7"/>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D91" t="s">
+        <v>35</v>
+      </c>
+      <c r="E91" t="s">
+        <v>35</v>
+      </c>
+      <c r="F91" t="s">
+        <v>35</v>
+      </c>
+      <c r="G91" t="s">
+        <v>35</v>
+      </c>
+      <c r="H91" t="s">
+        <v>35</v>
+      </c>
+      <c r="I91" t="s">
+        <v>35</v>
+      </c>
+      <c r="J91" t="s">
+        <v>35</v>
+      </c>
+      <c r="K91" t="s">
+        <v>35</v>
+      </c>
+      <c r="L91" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D92" s="7">
+        <v>3</v>
+      </c>
+      <c r="E92" s="7">
+        <v>2</v>
+      </c>
+      <c r="F92" s="7">
+        <v>3</v>
+      </c>
+      <c r="G92" s="7">
+        <v>4</v>
+      </c>
+      <c r="H92" s="7">
+        <v>4</v>
+      </c>
+      <c r="I92" s="7">
+        <v>3</v>
+      </c>
+      <c r="J92" s="7">
+        <v>6</v>
+      </c>
+      <c r="K92" s="7">
+        <v>4</v>
+      </c>
+      <c r="L92" s="7">
+        <v>5</v>
+      </c>
+      <c r="M92">
+        <f>SUM(D92:L92)</f>
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
First pass at adding 9 hole courses with some tests
</commit_message>
<xml_diff>
--- a/spec/fixtures/Golf.xlsx
+++ b/spec/fixtures/Golf.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulkristoff/dev/golf/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E2D534-0D4D-D34E-8E0B-6F7575FAD4E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C471BD-BBBA-4E44-AD77-8ECF849ADE40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="860" windowWidth="31760" windowHeight="12920" activeTab="2" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
+    <workbookView xWindow="60" yWindow="860" windowWidth="31760" windowHeight="12920" activeTab="4" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
   </bookViews>
   <sheets>
     <sheet name="Beachwood Golf Course" sheetId="6" r:id="rId1"/>
@@ -1460,8 +1460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{045CE2A8-F6DB-4143-9691-363739FD69FB}">
   <dimension ref="A1:M90"/>
   <sheetViews>
-    <sheetView topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91:M97"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1547,10 +1547,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>71.599999999999994</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="D4" s="1">
         <v>126</v>
@@ -1588,10 +1588,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="1">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="D5" s="1">
         <v>93</v>
@@ -1629,7 +1629,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="1">
         <v>113</v>
@@ -3776,8 +3776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8526A8B9-0C97-E94E-BA2A-E4D31B8BA027}">
   <dimension ref="A1:X92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3882,10 +3882,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>71.599999999999994</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="D4" s="1">
         <v>134</v>
@@ -3924,10 +3924,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="1">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="D5" s="1">
         <v>104</v>
@@ -3966,7 +3966,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="1">
         <v>113</v>
@@ -6170,7 +6170,7 @@
   <dimension ref="A1:X30"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="B4" sqref="B4:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6275,10 +6275,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>71.599999999999994</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="D4" s="1">
         <v>125</v>
@@ -6317,10 +6317,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="1">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="D5" s="1">
         <v>105</v>
@@ -6359,7 +6359,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="1">
         <v>113</v>
@@ -7009,8 +7009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F45684-D9E4-2242-9821-C781990B9A28}">
   <dimension ref="A1:X50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X7" sqref="X7:X8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="W38" sqref="W38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8439,16 +8439,18 @@
         <v>7</v>
       </c>
       <c r="U36" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="V36" s="3">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="W36" s="1">
-        <v>41</v>
+        <f>SUM(N36:V36)</f>
+        <v>53</v>
       </c>
       <c r="X36" s="1">
-        <v>90</v>
+        <f>M36+W36</f>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.2">
@@ -8507,16 +8509,18 @@
         <v>3</v>
       </c>
       <c r="U37" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V37" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W37" s="1">
-        <v>14</v>
+        <f>SUM(N37:V37)</f>
+        <v>18</v>
       </c>
       <c r="X37" s="1">
-        <v>30</v>
+        <f>M37+W37</f>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added tests to round_info_spec & round_info9_spec
</commit_message>
<xml_diff>
--- a/spec/fixtures/Golf.xlsx
+++ b/spec/fixtures/Golf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulkristoff/dev/golf/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C471BD-BBBA-4E44-AD77-8ECF849ADE40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1CFA8F-FD47-1846-A160-DDB7918A9965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="860" windowWidth="31760" windowHeight="12920" activeTab="4" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
+    <workbookView xWindow="60" yWindow="860" windowWidth="31760" windowHeight="12920" activeTab="2" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
   </bookViews>
   <sheets>
     <sheet name="Beachwood Golf Course" sheetId="6" r:id="rId1"/>
@@ -1460,8 +1460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{045CE2A8-F6DB-4143-9691-363739FD69FB}">
   <dimension ref="A1:M90"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C6"/>
+    <sheetView topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3776,8 +3776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8526A8B9-0C97-E94E-BA2A-E4D31B8BA027}">
   <dimension ref="A1:X92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C6"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="D89" sqref="D89:E92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5973,7 +5973,7 @@
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" s="6">
-        <v>44202</v>
+        <v>44567</v>
       </c>
       <c r="B87" s="12">
         <v>0.64444444444444449</v>
@@ -6169,7 +6169,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9DD2039-084D-3C4E-B129-968266BAB55E}">
   <dimension ref="A1:X30"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4:C6"/>
     </sheetView>
   </sheetViews>
@@ -7009,7 +7009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F45684-D9E4-2242-9821-C781990B9A28}">
   <dimension ref="A1:X50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="W38" sqref="W38"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added tests for RoundInfoSpec
</commit_message>
<xml_diff>
--- a/spec/fixtures/Golf.xlsx
+++ b/spec/fixtures/Golf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulkristoff/dev/golf/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1CFA8F-FD47-1846-A160-DDB7918A9965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76305FF-7385-F64A-BA6B-56F7D2817791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="860" windowWidth="31760" windowHeight="12920" activeTab="2" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
+    <workbookView xWindow="60" yWindow="860" windowWidth="31760" windowHeight="12920" activeTab="4" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
   </bookViews>
   <sheets>
     <sheet name="Beachwood Golf Course" sheetId="6" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="48">
   <si>
     <t>Hole</t>
   </si>
@@ -1458,10 +1458,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{045CE2A8-F6DB-4143-9691-363739FD69FB}">
-  <dimension ref="A1:M90"/>
+  <dimension ref="A1:M97"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78"/>
+    <sheetView topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91:M97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3763,6 +3763,196 @@
         <v>27</v>
       </c>
     </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A92" s="6">
+        <v>44603</v>
+      </c>
+      <c r="B92" s="12">
+        <v>0.53541666666666665</v>
+      </c>
+      <c r="C92" s="13">
+        <v>0.59791666666666665</v>
+      </c>
+      <c r="D92" s="7"/>
+      <c r="E92" s="7"/>
+      <c r="F92" s="7"/>
+      <c r="G92" s="7"/>
+      <c r="H92" s="7"/>
+      <c r="I92" s="7"/>
+      <c r="J92" s="7"/>
+      <c r="K92" s="7"/>
+      <c r="L92" s="7"/>
+      <c r="M92" s="7"/>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
+      <c r="D93" s="7">
+        <v>4</v>
+      </c>
+      <c r="E93" s="7">
+        <v>5</v>
+      </c>
+      <c r="F93" s="7">
+        <v>3</v>
+      </c>
+      <c r="G93" s="7">
+        <v>5</v>
+      </c>
+      <c r="H93" s="7">
+        <v>7</v>
+      </c>
+      <c r="I93" s="7">
+        <v>5</v>
+      </c>
+      <c r="J93" s="7">
+        <v>6</v>
+      </c>
+      <c r="K93" s="7">
+        <v>3</v>
+      </c>
+      <c r="L93" s="7">
+        <v>5</v>
+      </c>
+      <c r="M93" s="8">
+        <f>SUM(D93:L93)</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A94" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B94" s="8"/>
+      <c r="C94" s="8"/>
+      <c r="D94" s="7">
+        <v>2</v>
+      </c>
+      <c r="E94" s="7">
+        <v>3</v>
+      </c>
+      <c r="F94" s="7">
+        <v>1</v>
+      </c>
+      <c r="G94" s="7">
+        <v>2</v>
+      </c>
+      <c r="H94" s="7">
+        <v>2</v>
+      </c>
+      <c r="I94" s="7">
+        <v>3</v>
+      </c>
+      <c r="J94" s="7">
+        <v>2</v>
+      </c>
+      <c r="K94" s="7">
+        <v>2</v>
+      </c>
+      <c r="L94" s="7">
+        <v>3</v>
+      </c>
+      <c r="M94" s="8">
+        <f>SUM(D94:L94)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A95" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B95" s="8"/>
+      <c r="C95" s="8"/>
+      <c r="D95" s="7"/>
+      <c r="E95" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F95" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G95" s="7"/>
+      <c r="H95" s="7"/>
+      <c r="I95" s="7"/>
+      <c r="J95" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K95" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L95" s="7"/>
+      <c r="M95" s="7"/>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D96" t="s">
+        <v>35</v>
+      </c>
+      <c r="E96" t="s">
+        <v>35</v>
+      </c>
+      <c r="F96" t="s">
+        <v>35</v>
+      </c>
+      <c r="G96" t="s">
+        <v>35</v>
+      </c>
+      <c r="H96" t="s">
+        <v>35</v>
+      </c>
+      <c r="I96" t="s">
+        <v>35</v>
+      </c>
+      <c r="J96" t="s">
+        <v>35</v>
+      </c>
+      <c r="K96" t="s">
+        <v>35</v>
+      </c>
+      <c r="L96" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D97">
+        <v>3</v>
+      </c>
+      <c r="E97">
+        <v>4</v>
+      </c>
+      <c r="F97">
+        <v>2</v>
+      </c>
+      <c r="G97">
+        <v>5</v>
+      </c>
+      <c r="H97">
+        <v>4</v>
+      </c>
+      <c r="I97">
+        <v>5</v>
+      </c>
+      <c r="J97" s="3">
+        <v>3</v>
+      </c>
+      <c r="K97">
+        <v>2</v>
+      </c>
+      <c r="L97">
+        <v>1</v>
+      </c>
+      <c r="M97">
+        <f>SUM(D97:L97)</f>
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3774,10 +3964,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8526A8B9-0C97-E94E-BA2A-E4D31B8BA027}">
-  <dimension ref="A1:X92"/>
+  <dimension ref="A1:X99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="D89" sqref="D89:E92"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="M99" sqref="M99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6159,6 +6349,194 @@
         <v>34</v>
       </c>
     </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A94" s="6">
+        <v>44603</v>
+      </c>
+      <c r="B94" s="13">
+        <v>0.59791666666666665</v>
+      </c>
+      <c r="C94" s="13">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D94" s="7"/>
+      <c r="E94" s="7"/>
+      <c r="F94" s="7"/>
+      <c r="G94" s="7"/>
+      <c r="H94" s="7"/>
+      <c r="I94" s="7"/>
+      <c r="J94" s="7"/>
+      <c r="K94" s="7"/>
+      <c r="L94" s="7"/>
+      <c r="M94" s="7"/>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+      <c r="D95" s="7">
+        <v>4</v>
+      </c>
+      <c r="E95" s="7">
+        <v>5</v>
+      </c>
+      <c r="F95" s="7">
+        <v>7</v>
+      </c>
+      <c r="G95" s="7">
+        <v>4</v>
+      </c>
+      <c r="H95" s="7">
+        <v>4</v>
+      </c>
+      <c r="I95" s="7">
+        <v>4</v>
+      </c>
+      <c r="J95" s="7">
+        <v>6</v>
+      </c>
+      <c r="K95" s="7">
+        <v>7</v>
+      </c>
+      <c r="L95" s="7">
+        <v>5</v>
+      </c>
+      <c r="M95" s="8">
+        <f>SUM(D95:L95)</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A96" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B96" s="8"/>
+      <c r="C96" s="8"/>
+      <c r="D96" s="7">
+        <v>1</v>
+      </c>
+      <c r="E96" s="7">
+        <v>2</v>
+      </c>
+      <c r="F96" s="7">
+        <v>3</v>
+      </c>
+      <c r="G96" s="7">
+        <v>2</v>
+      </c>
+      <c r="H96" s="7">
+        <v>2</v>
+      </c>
+      <c r="I96" s="7">
+        <v>2</v>
+      </c>
+      <c r="J96" s="7">
+        <v>4</v>
+      </c>
+      <c r="K96" s="7">
+        <v>2</v>
+      </c>
+      <c r="L96" s="7">
+        <v>2</v>
+      </c>
+      <c r="M96" s="8">
+        <f>SUM(D96:L96)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A97" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B97" s="8"/>
+      <c r="C97" s="8"/>
+      <c r="D97" s="7"/>
+      <c r="E97" s="7"/>
+      <c r="F97" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G97" s="7"/>
+      <c r="H97" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I97" s="7"/>
+      <c r="J97" s="7"/>
+      <c r="K97" s="7"/>
+      <c r="L97" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M97" s="7"/>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A98" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D98" t="s">
+        <v>35</v>
+      </c>
+      <c r="E98" t="s">
+        <v>35</v>
+      </c>
+      <c r="F98" t="s">
+        <v>35</v>
+      </c>
+      <c r="G98" t="s">
+        <v>35</v>
+      </c>
+      <c r="H98" t="s">
+        <v>35</v>
+      </c>
+      <c r="I98" t="s">
+        <v>35</v>
+      </c>
+      <c r="J98" t="s">
+        <v>35</v>
+      </c>
+      <c r="K98" t="s">
+        <v>35</v>
+      </c>
+      <c r="L98" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D99">
+        <v>3</v>
+      </c>
+      <c r="E99">
+        <v>4</v>
+      </c>
+      <c r="F99">
+        <v>6</v>
+      </c>
+      <c r="G99">
+        <v>3</v>
+      </c>
+      <c r="H99">
+        <v>5</v>
+      </c>
+      <c r="I99">
+        <v>3</v>
+      </c>
+      <c r="J99" s="3">
+        <v>5</v>
+      </c>
+      <c r="K99">
+        <v>6</v>
+      </c>
+      <c r="L99">
+        <v>3</v>
+      </c>
+      <c r="M99">
+        <f>SUM(D99:L99)</f>
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -6169,7 +6547,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9DD2039-084D-3C4E-B129-968266BAB55E}">
   <dimension ref="A1:X30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B4" sqref="B4:C6"/>
     </sheetView>
   </sheetViews>
@@ -7007,10 +7385,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F45684-D9E4-2242-9821-C781990B9A28}">
-  <dimension ref="A1:X50"/>
+  <dimension ref="A1:X57"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="W38" sqref="W38"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="X58" sqref="X58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8916,7 +9294,7 @@
       </c>
       <c r="V48" s="1"/>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>30</v>
       </c>
@@ -8975,7 +9353,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>32</v>
       </c>
@@ -9032,6 +9410,308 @@
       </c>
       <c r="V50">
         <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A52" s="2">
+        <v>44609</v>
+      </c>
+      <c r="B52" s="11">
+        <v>0.47500000000000003</v>
+      </c>
+      <c r="C52" s="11">
+        <v>0.65972222222222221</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53">
+        <v>7</v>
+      </c>
+      <c r="E53">
+        <v>7</v>
+      </c>
+      <c r="F53">
+        <v>4</v>
+      </c>
+      <c r="G53">
+        <v>6</v>
+      </c>
+      <c r="H53">
+        <v>7</v>
+      </c>
+      <c r="I53">
+        <v>6</v>
+      </c>
+      <c r="J53">
+        <v>5</v>
+      </c>
+      <c r="K53" s="3">
+        <v>4</v>
+      </c>
+      <c r="L53" s="3">
+        <v>10</v>
+      </c>
+      <c r="M53" s="1">
+        <f>SUM(D53:L53)</f>
+        <v>56</v>
+      </c>
+      <c r="N53">
+        <v>5</v>
+      </c>
+      <c r="O53">
+        <v>5</v>
+      </c>
+      <c r="P53">
+        <v>9</v>
+      </c>
+      <c r="Q53">
+        <v>6</v>
+      </c>
+      <c r="R53">
+        <v>7</v>
+      </c>
+      <c r="S53">
+        <v>6</v>
+      </c>
+      <c r="T53">
+        <v>7</v>
+      </c>
+      <c r="U53" s="3">
+        <v>5</v>
+      </c>
+      <c r="V53" s="3">
+        <v>5</v>
+      </c>
+      <c r="W53" s="1">
+        <f>SUM(N53:V53)</f>
+        <v>55</v>
+      </c>
+      <c r="X53" s="1">
+        <f>W53+M53</f>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>2</v>
+      </c>
+      <c r="F54">
+        <v>2</v>
+      </c>
+      <c r="G54">
+        <v>2</v>
+      </c>
+      <c r="H54">
+        <v>4</v>
+      </c>
+      <c r="I54">
+        <v>3</v>
+      </c>
+      <c r="J54">
+        <v>2</v>
+      </c>
+      <c r="K54" s="3">
+        <v>2</v>
+      </c>
+      <c r="L54" s="3">
+        <v>2</v>
+      </c>
+      <c r="M54" s="1">
+        <f>SUM(D54:L54)</f>
+        <v>20</v>
+      </c>
+      <c r="N54">
+        <v>2</v>
+      </c>
+      <c r="O54">
+        <v>3</v>
+      </c>
+      <c r="P54">
+        <v>2</v>
+      </c>
+      <c r="Q54">
+        <v>3</v>
+      </c>
+      <c r="R54">
+        <v>3</v>
+      </c>
+      <c r="S54">
+        <v>2</v>
+      </c>
+      <c r="T54">
+        <v>4</v>
+      </c>
+      <c r="U54" s="3">
+        <v>2</v>
+      </c>
+      <c r="V54" s="3">
+        <v>2</v>
+      </c>
+      <c r="W54" s="1">
+        <f>SUM(N54:V54)</f>
+        <v>23</v>
+      </c>
+      <c r="X54" s="1">
+        <f>W54+M54</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D55" t="s">
+        <v>24</v>
+      </c>
+      <c r="K55" s="1"/>
+      <c r="L55" t="s">
+        <v>11</v>
+      </c>
+      <c r="P55" t="s">
+        <v>22</v>
+      </c>
+      <c r="U55" s="1"/>
+      <c r="V55" s="1"/>
+    </row>
+    <row r="56" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D56" t="s">
+        <v>34</v>
+      </c>
+      <c r="E56" t="s">
+        <v>33</v>
+      </c>
+      <c r="F56" t="s">
+        <v>33</v>
+      </c>
+      <c r="G56" t="s">
+        <v>33</v>
+      </c>
+      <c r="H56" t="s">
+        <v>33</v>
+      </c>
+      <c r="I56" t="s">
+        <v>33</v>
+      </c>
+      <c r="J56" t="s">
+        <v>33</v>
+      </c>
+      <c r="K56" t="s">
+        <v>33</v>
+      </c>
+      <c r="L56" t="s">
+        <v>33</v>
+      </c>
+      <c r="N56" t="s">
+        <v>34</v>
+      </c>
+      <c r="O56" t="s">
+        <v>33</v>
+      </c>
+      <c r="P56" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>33</v>
+      </c>
+      <c r="R56" t="s">
+        <v>33</v>
+      </c>
+      <c r="S56" t="s">
+        <v>33</v>
+      </c>
+      <c r="T56" t="s">
+        <v>34</v>
+      </c>
+      <c r="U56" t="s">
+        <v>33</v>
+      </c>
+      <c r="V56" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D57">
+        <v>4</v>
+      </c>
+      <c r="E57">
+        <v>4</v>
+      </c>
+      <c r="F57">
+        <v>3</v>
+      </c>
+      <c r="G57">
+        <v>4</v>
+      </c>
+      <c r="H57">
+        <v>5</v>
+      </c>
+      <c r="I57">
+        <v>4</v>
+      </c>
+      <c r="J57">
+        <v>4</v>
+      </c>
+      <c r="K57">
+        <v>2</v>
+      </c>
+      <c r="L57">
+        <v>6</v>
+      </c>
+      <c r="M57">
+        <f>SUM(D57:L57)</f>
+        <v>36</v>
+      </c>
+      <c r="N57">
+        <v>3</v>
+      </c>
+      <c r="O57">
+        <v>4</v>
+      </c>
+      <c r="P57">
+        <v>6</v>
+      </c>
+      <c r="Q57">
+        <v>4</v>
+      </c>
+      <c r="R57">
+        <v>5</v>
+      </c>
+      <c r="S57">
+        <v>4</v>
+      </c>
+      <c r="T57">
+        <v>5</v>
+      </c>
+      <c r="U57">
+        <v>4</v>
+      </c>
+      <c r="V57">
+        <v>3</v>
+      </c>
+      <c r="W57">
+        <f>SUM(N57:V57)</f>
+        <v>38</v>
+      </c>
+      <c r="X57">
+        <f>M57+W57</f>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactoring mostly tests: create_round9 & create_round18
</commit_message>
<xml_diff>
--- a/spec/fixtures/Golf.xlsx
+++ b/spec/fixtures/Golf.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulkristoff/dev/golf/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76305FF-7385-F64A-BA6B-56F7D2817791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90C0008-3FF1-9A4B-9C85-B85589F2E5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="860" windowWidth="31760" windowHeight="12920" activeTab="4" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="48">
   <si>
     <t>Hole</t>
   </si>
@@ -7385,10 +7385,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F45684-D9E4-2242-9821-C781990B9A28}">
-  <dimension ref="A1:X57"/>
+  <dimension ref="A1:X64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="X58" sqref="X58"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="W64" sqref="W64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9714,6 +9714,307 @@
         <v>74</v>
       </c>
     </row>
+    <row r="59" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A59" s="2">
+        <v>44618</v>
+      </c>
+      <c r="B59" s="11">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="C59" s="11">
+        <v>0.70138888888888884</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60">
+        <v>6</v>
+      </c>
+      <c r="E60">
+        <v>4</v>
+      </c>
+      <c r="F60">
+        <v>4</v>
+      </c>
+      <c r="G60">
+        <v>6</v>
+      </c>
+      <c r="H60">
+        <v>6</v>
+      </c>
+      <c r="I60">
+        <v>9</v>
+      </c>
+      <c r="J60">
+        <v>5</v>
+      </c>
+      <c r="K60" s="3">
+        <v>8</v>
+      </c>
+      <c r="L60" s="3">
+        <v>6</v>
+      </c>
+      <c r="M60" s="1">
+        <f>SUM(D60:L60)</f>
+        <v>54</v>
+      </c>
+      <c r="N60">
+        <v>6</v>
+      </c>
+      <c r="O60">
+        <v>7</v>
+      </c>
+      <c r="P60">
+        <v>8</v>
+      </c>
+      <c r="Q60">
+        <v>7</v>
+      </c>
+      <c r="R60">
+        <v>8</v>
+      </c>
+      <c r="S60" s="10">
+        <v>7</v>
+      </c>
+      <c r="T60">
+        <v>8</v>
+      </c>
+      <c r="U60" s="3">
+        <v>5</v>
+      </c>
+      <c r="V60" s="3">
+        <v>8</v>
+      </c>
+      <c r="W60" s="1">
+        <f>SUM(N60:V60)</f>
+        <v>64</v>
+      </c>
+      <c r="X60" s="1">
+        <f>W60+M60</f>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="61" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D61">
+        <v>2</v>
+      </c>
+      <c r="E61">
+        <v>2</v>
+      </c>
+      <c r="F61">
+        <v>2</v>
+      </c>
+      <c r="G61">
+        <v>2</v>
+      </c>
+      <c r="H61">
+        <v>2</v>
+      </c>
+      <c r="I61">
+        <v>3</v>
+      </c>
+      <c r="J61">
+        <v>2</v>
+      </c>
+      <c r="K61" s="3">
+        <v>3</v>
+      </c>
+      <c r="L61" s="3">
+        <v>1</v>
+      </c>
+      <c r="M61" s="1">
+        <f>SUM(D61:L61)</f>
+        <v>19</v>
+      </c>
+      <c r="N61">
+        <v>2</v>
+      </c>
+      <c r="O61">
+        <v>2</v>
+      </c>
+      <c r="P61">
+        <v>1</v>
+      </c>
+      <c r="Q61">
+        <v>3</v>
+      </c>
+      <c r="R61">
+        <v>2</v>
+      </c>
+      <c r="S61">
+        <v>1</v>
+      </c>
+      <c r="T61">
+        <v>2</v>
+      </c>
+      <c r="U61" s="3">
+        <v>1</v>
+      </c>
+      <c r="V61" s="3">
+        <v>2</v>
+      </c>
+      <c r="W61" s="1">
+        <f>SUM(N61:V61)</f>
+        <v>16</v>
+      </c>
+      <c r="X61" s="1">
+        <f>W61+M61</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="62" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J62" t="s">
+        <v>11</v>
+      </c>
+      <c r="K62" s="1"/>
+      <c r="O62" t="s">
+        <v>11</v>
+      </c>
+      <c r="P62" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>11</v>
+      </c>
+      <c r="R62" t="s">
+        <v>11</v>
+      </c>
+      <c r="S62" t="s">
+        <v>11</v>
+      </c>
+      <c r="U62" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="V62" s="1"/>
+    </row>
+    <row r="63" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D63" t="s">
+        <v>33</v>
+      </c>
+      <c r="E63" t="s">
+        <v>34</v>
+      </c>
+      <c r="G63" t="s">
+        <v>33</v>
+      </c>
+      <c r="H63" t="s">
+        <v>33</v>
+      </c>
+      <c r="I63" t="s">
+        <v>33</v>
+      </c>
+      <c r="K63" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="L63" t="s">
+        <v>33</v>
+      </c>
+      <c r="N63" t="s">
+        <v>33</v>
+      </c>
+      <c r="P63" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>33</v>
+      </c>
+      <c r="R63" t="s">
+        <v>33</v>
+      </c>
+      <c r="S63" t="s">
+        <v>33</v>
+      </c>
+      <c r="T63" t="s">
+        <v>33</v>
+      </c>
+      <c r="V63" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="64" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D64">
+        <v>4</v>
+      </c>
+      <c r="E64">
+        <v>2</v>
+      </c>
+      <c r="F64">
+        <v>3</v>
+      </c>
+      <c r="G64">
+        <v>4</v>
+      </c>
+      <c r="H64">
+        <v>5</v>
+      </c>
+      <c r="I64">
+        <v>4</v>
+      </c>
+      <c r="J64">
+        <v>3</v>
+      </c>
+      <c r="K64">
+        <v>4</v>
+      </c>
+      <c r="L64">
+        <v>3</v>
+      </c>
+      <c r="M64">
+        <f>SUM(D64:L64)</f>
+        <v>32</v>
+      </c>
+      <c r="N64">
+        <v>4</v>
+      </c>
+      <c r="O64">
+        <v>4</v>
+      </c>
+      <c r="P64">
+        <v>4</v>
+      </c>
+      <c r="Q64">
+        <v>4</v>
+      </c>
+      <c r="R64">
+        <v>5</v>
+      </c>
+      <c r="S64">
+        <v>4</v>
+      </c>
+      <c r="T64">
+        <v>4</v>
+      </c>
+      <c r="U64">
+        <v>2</v>
+      </c>
+      <c r="V64">
+        <v>6</v>
+      </c>
+      <c r="W64">
+        <f>SUM(N64:V64)</f>
+        <v>37</v>
+      </c>
+      <c r="X64">
+        <f>M64+W64</f>
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rename course_handicap to calc_course_handicap Rename initial_handicap_index to initial_hix added tests for calc_course_handicap added calc_course_hdcp for a round
</commit_message>
<xml_diff>
--- a/spec/fixtures/Golf.xlsx
+++ b/spec/fixtures/Golf.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulkristoff/dev/golf/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90C0008-3FF1-9A4B-9C85-B85589F2E5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B44DB7E-4181-7946-B2A6-D583C1C7DAEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="860" windowWidth="31760" windowHeight="12920" activeTab="4" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
+    <workbookView xWindow="60" yWindow="860" windowWidth="31760" windowHeight="12920" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
   </bookViews>
   <sheets>
     <sheet name="Beachwood Golf Course" sheetId="6" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="48">
   <si>
     <t>Hole</t>
   </si>
@@ -620,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7EF7B00-A774-EB4A-8778-3EE04B4CA963}">
-  <dimension ref="A1:X15"/>
+  <dimension ref="A1:X22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="W7" sqref="W7:X8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W22" sqref="W22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1451,6 +1451,321 @@
         <v>60</v>
       </c>
     </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>44635</v>
+      </c>
+      <c r="B17" s="11">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="C17" s="11">
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18">
+        <v>6</v>
+      </c>
+      <c r="E18">
+        <v>5</v>
+      </c>
+      <c r="F18">
+        <v>8</v>
+      </c>
+      <c r="G18">
+        <v>3</v>
+      </c>
+      <c r="H18">
+        <v>6</v>
+      </c>
+      <c r="I18">
+        <v>5</v>
+      </c>
+      <c r="J18">
+        <v>5</v>
+      </c>
+      <c r="K18" s="3">
+        <v>6</v>
+      </c>
+      <c r="L18" s="3">
+        <v>9</v>
+      </c>
+      <c r="M18" s="1">
+        <f>SUM(D18:L18)</f>
+        <v>53</v>
+      </c>
+      <c r="N18">
+        <v>7</v>
+      </c>
+      <c r="O18">
+        <v>6</v>
+      </c>
+      <c r="P18">
+        <v>5</v>
+      </c>
+      <c r="Q18">
+        <v>5</v>
+      </c>
+      <c r="R18">
+        <v>5</v>
+      </c>
+      <c r="S18">
+        <v>6</v>
+      </c>
+      <c r="T18">
+        <v>5</v>
+      </c>
+      <c r="U18" s="3">
+        <v>5</v>
+      </c>
+      <c r="V18" s="3">
+        <v>5</v>
+      </c>
+      <c r="W18" s="1">
+        <f>SUM(N18:V18)</f>
+        <v>49</v>
+      </c>
+      <c r="X18" s="1">
+        <f>W18+M18</f>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>2</v>
+      </c>
+      <c r="I19">
+        <v>2</v>
+      </c>
+      <c r="J19">
+        <v>2</v>
+      </c>
+      <c r="K19" s="3">
+        <v>2</v>
+      </c>
+      <c r="L19" s="3">
+        <v>1</v>
+      </c>
+      <c r="M19" s="1">
+        <f>SUM(D19:L19)</f>
+        <v>17</v>
+      </c>
+      <c r="N19">
+        <v>3</v>
+      </c>
+      <c r="O19">
+        <v>2</v>
+      </c>
+      <c r="P19">
+        <v>2</v>
+      </c>
+      <c r="Q19">
+        <v>2</v>
+      </c>
+      <c r="R19">
+        <v>1</v>
+      </c>
+      <c r="S19">
+        <v>2</v>
+      </c>
+      <c r="T19">
+        <v>2</v>
+      </c>
+      <c r="U19" s="3">
+        <v>1</v>
+      </c>
+      <c r="V19" s="3">
+        <v>2</v>
+      </c>
+      <c r="W19" s="1">
+        <f>SUM(N19:V19)</f>
+        <v>17</v>
+      </c>
+      <c r="X19" s="1">
+        <f>W19+M19</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K20" s="1"/>
+      <c r="P20" t="s">
+        <v>22</v>
+      </c>
+      <c r="S20" t="s">
+        <v>11</v>
+      </c>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21" t="s">
+        <v>33</v>
+      </c>
+      <c r="I21" t="s">
+        <v>34</v>
+      </c>
+      <c r="J21" t="s">
+        <v>33</v>
+      </c>
+      <c r="L21" t="s">
+        <v>33</v>
+      </c>
+      <c r="N21" t="s">
+        <v>33</v>
+      </c>
+      <c r="O21" t="s">
+        <v>33</v>
+      </c>
+      <c r="P21" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>33</v>
+      </c>
+      <c r="R21" t="s">
+        <v>34</v>
+      </c>
+      <c r="T21" t="s">
+        <v>34</v>
+      </c>
+      <c r="U21" t="s">
+        <v>33</v>
+      </c>
+      <c r="V21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
+      <c r="H22">
+        <v>4</v>
+      </c>
+      <c r="I22">
+        <v>3</v>
+      </c>
+      <c r="J22">
+        <v>3</v>
+      </c>
+      <c r="K22">
+        <v>5</v>
+      </c>
+      <c r="L22">
+        <v>5</v>
+      </c>
+      <c r="M22">
+        <f>SUM(D22:L22)</f>
+        <v>33</v>
+      </c>
+      <c r="N22">
+        <v>5</v>
+      </c>
+      <c r="O22">
+        <v>4</v>
+      </c>
+      <c r="P22">
+        <v>3</v>
+      </c>
+      <c r="Q22">
+        <v>3</v>
+      </c>
+      <c r="R22">
+        <v>3</v>
+      </c>
+      <c r="S22">
+        <v>4</v>
+      </c>
+      <c r="T22">
+        <v>3</v>
+      </c>
+      <c r="U22">
+        <v>2</v>
+      </c>
+      <c r="V22">
+        <v>3</v>
+      </c>
+      <c r="W22">
+        <f>SUM(N22:V22)</f>
+        <v>30</v>
+      </c>
+      <c r="X22">
+        <f>M22+W22</f>
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7387,7 +7702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F45684-D9E4-2242-9821-C781990B9A28}">
   <dimension ref="A1:X64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="W64" sqref="W64"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Trying to update code after upgrading macbook (12.6).  Had trouble getting ruby/rvm working.  So updated bundle.
</commit_message>
<xml_diff>
--- a/spec/fixtures/Golf.xlsx
+++ b/spec/fixtures/Golf.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulkristoff/dev/golf/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE51E86-278B-E74B-B018-B425EF87065F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD50772-997C-594F-9915-E32DB51ED8E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="31760" windowHeight="14440" activeTab="6" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
+    <workbookView xWindow="180" yWindow="920" windowWidth="31760" windowHeight="14440" activeTab="6" xr2:uid="{092F107D-2B6D-FE47-A2F2-04DB71A88C56}"/>
   </bookViews>
   <sheets>
     <sheet name="Aspen Golf Course" sheetId="11" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="68">
   <si>
     <t>Hole</t>
   </si>
@@ -248,6 +248,9 @@
   </si>
   <si>
     <t>#:00:00 PM</t>
+  </si>
+  <si>
+    <t>MW</t>
   </si>
 </sst>
 </file>
@@ -16010,10 +16013,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F45684-D9E4-2242-9821-C781990B9A28}">
-  <dimension ref="A1:X78"/>
+  <dimension ref="A1:X85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="W77" sqref="W77"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="U81" sqref="U81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19260,6 +19263,312 @@
         <v>68</v>
       </c>
     </row>
+    <row r="80" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A80" s="2">
+        <v>44846</v>
+      </c>
+      <c r="B80" s="8">
+        <v>0.36944444444444446</v>
+      </c>
+      <c r="C80" s="8">
+        <v>0.55555555555555558</v>
+      </c>
+    </row>
+    <row r="81" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+      <c r="D81">
+        <v>6</v>
+      </c>
+      <c r="E81">
+        <v>6</v>
+      </c>
+      <c r="F81">
+        <v>5</v>
+      </c>
+      <c r="G81">
+        <v>6</v>
+      </c>
+      <c r="H81">
+        <v>5</v>
+      </c>
+      <c r="I81">
+        <v>7</v>
+      </c>
+      <c r="J81">
+        <v>5</v>
+      </c>
+      <c r="K81">
+        <v>6</v>
+      </c>
+      <c r="L81">
+        <v>7</v>
+      </c>
+      <c r="M81" s="1">
+        <f>SUM(D81:L81)</f>
+        <v>53</v>
+      </c>
+      <c r="N81">
+        <v>6</v>
+      </c>
+      <c r="O81">
+        <v>5</v>
+      </c>
+      <c r="P81">
+        <v>7</v>
+      </c>
+      <c r="Q81">
+        <v>5</v>
+      </c>
+      <c r="R81">
+        <v>6</v>
+      </c>
+      <c r="S81" s="7">
+        <v>5</v>
+      </c>
+      <c r="T81">
+        <v>6</v>
+      </c>
+      <c r="U81">
+        <v>5</v>
+      </c>
+      <c r="V81">
+        <v>3</v>
+      </c>
+      <c r="W81" s="1">
+        <f>SUM(N81:V81)</f>
+        <v>48</v>
+      </c>
+      <c r="X81" s="1">
+        <f>W81+M81</f>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="82" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D82">
+        <v>1</v>
+      </c>
+      <c r="E82">
+        <v>2</v>
+      </c>
+      <c r="F82">
+        <v>2</v>
+      </c>
+      <c r="G82">
+        <v>3</v>
+      </c>
+      <c r="H82">
+        <v>1</v>
+      </c>
+      <c r="I82">
+        <v>2</v>
+      </c>
+      <c r="J82">
+        <v>2</v>
+      </c>
+      <c r="K82">
+        <v>2</v>
+      </c>
+      <c r="L82">
+        <v>2</v>
+      </c>
+      <c r="M82" s="19">
+        <f>SUM(D82:L82)</f>
+        <v>17</v>
+      </c>
+      <c r="N82">
+        <v>2</v>
+      </c>
+      <c r="O82">
+        <v>2</v>
+      </c>
+      <c r="P82">
+        <v>2</v>
+      </c>
+      <c r="Q82">
+        <v>3</v>
+      </c>
+      <c r="R82">
+        <v>1</v>
+      </c>
+      <c r="S82">
+        <v>1</v>
+      </c>
+      <c r="T82">
+        <v>1</v>
+      </c>
+      <c r="U82">
+        <v>1</v>
+      </c>
+      <c r="V82">
+        <v>1</v>
+      </c>
+      <c r="W82" s="1">
+        <f>SUM(N82:V82)</f>
+        <v>14</v>
+      </c>
+      <c r="X82" s="1">
+        <f>W82+M82</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="83" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H83" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="I83" t="s">
+        <v>11</v>
+      </c>
+      <c r="J83" t="s">
+        <v>11</v>
+      </c>
+      <c r="K83" s="1"/>
+      <c r="O83" t="s">
+        <v>11</v>
+      </c>
+      <c r="R83" t="s">
+        <v>9</v>
+      </c>
+      <c r="U83" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="V83" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D84" t="s">
+        <v>34</v>
+      </c>
+      <c r="E84" t="s">
+        <v>33</v>
+      </c>
+      <c r="G84" t="s">
+        <v>34</v>
+      </c>
+      <c r="H84" t="s">
+        <v>33</v>
+      </c>
+      <c r="I84" t="s">
+        <v>34</v>
+      </c>
+      <c r="K84" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="L84" t="s">
+        <v>34</v>
+      </c>
+      <c r="N84" t="s">
+        <v>34</v>
+      </c>
+      <c r="P84" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q84" t="s">
+        <v>33</v>
+      </c>
+      <c r="R84" t="s">
+        <v>34</v>
+      </c>
+      <c r="S84" t="s">
+        <v>33</v>
+      </c>
+      <c r="T84" t="s">
+        <v>33</v>
+      </c>
+      <c r="U84" t="s">
+        <v>33</v>
+      </c>
+      <c r="V84" t="s">
+        <v>34</v>
+      </c>
+      <c r="W84">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D85">
+        <v>4</v>
+      </c>
+      <c r="E85">
+        <v>3</v>
+      </c>
+      <c r="F85">
+        <v>4</v>
+      </c>
+      <c r="G85">
+        <v>4</v>
+      </c>
+      <c r="H85" s="14">
+        <v>2</v>
+      </c>
+      <c r="I85">
+        <v>4</v>
+      </c>
+      <c r="J85">
+        <v>4</v>
+      </c>
+      <c r="K85">
+        <v>4</v>
+      </c>
+      <c r="L85">
+        <v>3</v>
+      </c>
+      <c r="M85">
+        <f>SUM(D85:L85)</f>
+        <v>32</v>
+      </c>
+      <c r="N85">
+        <v>4</v>
+      </c>
+      <c r="O85">
+        <v>3</v>
+      </c>
+      <c r="P85">
+        <v>4</v>
+      </c>
+      <c r="Q85">
+        <v>3</v>
+      </c>
+      <c r="R85">
+        <v>4</v>
+      </c>
+      <c r="S85">
+        <v>3</v>
+      </c>
+      <c r="T85">
+        <v>4</v>
+      </c>
+      <c r="U85">
+        <v>4</v>
+      </c>
+      <c r="V85">
+        <v>1</v>
+      </c>
+      <c r="W85">
+        <f>SUM(N85:V85)</f>
+        <v>30</v>
+      </c>
+      <c r="X85">
+        <f>M85+W85</f>
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>